<commit_message>
Added Dependent test ids to test cases to avoid failures.
</commit_message>
<xml_diff>
--- a/src/test/test-data/MediaTestData.xlsx
+++ b/src/test/test-data/MediaTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="86">
   <si>
     <t>GET</t>
   </si>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L20"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -907,7 +907,9 @@
       <c r="H7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="J7" s="7" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
Added new test cases, images for Media Streaming service for Profile.
</commit_message>
<xml_diff>
--- a/src/test/test-data/MediaTestData.xlsx
+++ b/src/test/test-data/MediaTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="109">
   <si>
     <t>GET</t>
   </si>
@@ -128,9 +128,6 @@
     <t>OPQA-AA05</t>
   </si>
   <si>
-    <t>Verify that user is not able to update media witn invalid media ID for profile context using base64 API and check the error status</t>
-  </si>
-  <si>
     <t>/internal/media/(OPQA-AA01_mediaId)/base64</t>
   </si>
   <si>
@@ -140,33 +137,21 @@
     <t>{ "mediaId": "0f28b7f1-2bee-4178-ad9f-3d5e68d167", "base64Media": "data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAASwAAAEsCAYAAAB5fY51AAAABHNCSVQICAgIfAhkiAAAGYBJREFUeJzt3XuYFOWB7/HvW9U9V5gBBhxwAMVwEURBohgMRt2V9YKa5OhuPErcs15iPBv0PDlnZXWfk8c8m82um2fd9RKT+CTGVUyyu8nZTQRW18RoCCExxmgCchdE7gxzg5np6e6q9/xRM3JxlLl1V709v8/zjD7M9HS/9Ex/qap+6y3DYHzm2SpqU0vwgrngTcPaGXhmEtYO6m5FpAQYA6F9B2M2QbiF0H+d1vxyHr+mY8B3OaDvumfV9Rh7J5h5WFtLKm2wIdGHYiUi3YwB40Uf+ZzFmFawr2HN1/j7q77f77vr162XrboGa+/FMwvwfAgDBUpE+s4Y3m1HaNdizN/ywFXP9vnb+/xAy1Y8h192OTaEMAQUKhEZKANe95ZXkH2eB66+oo/fdRJ/ueoWLF/GT9UT5AY9TBGR4/hpCPL7MdzH3131xAfd9IODtWzl/cC9eH4ZYTCEIxQROUa0m5gF/pYHFt//fjfz3/cOlq34Aqmy+7HWx4YFGKGISDdrwRifVPoSLvyUZc13Xu7tZr0Ha9nK+0mV3U8+j45ViUjRhBZS6Uu58AbDmu+8dOKX37tL+JerbsHar2FMmd4BFJGiMwaszWLMnSce0/Lec2PLl/F8xUpE4mEtUYP48olfOj5Yy1Y8h5+q1wF2EYlVGICfqmfZiueO/fTRYC1bdQ1+2eWauiAiiRDkwC+7nGWrrun51NFgWXuv3g0UkUSJTve7t+ePUbDuWXU9nlkQzWAXEUmIMATPLOCeVddDT7CMvRPPR1MYRCRZbDSp1Ng7AQyfebaK0f5uDKP0zqCIJI4xYGmhOWhIUZtagg1r4x6TiEivrAVLLbWpJR5eMJdUemDrYomIFEMqbfCCuV60UqgOtotIgtkQ8KZ5WDtDwRKRRIumN8zwtAa7iCSeteCZSZ5iJSJOsLaXk59FRBJKwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOCMV9wBiYYHQHv3obdVVzxz/ISKxGz7BCkLIW8iHkPY597RRXDapltnjqjhlRNlxzfIMbG3qZP3BDla83cI7u9sACykPfA98BUwkDqUdrLA7UBhuPGscl8wYx8IZ9cwcV33Sb728+/+Pdf//17taeWndHlZuauTlHS1R1VImuiqtiBSFYdnK0rsKhQWyAWefUs31cyZw8/zJNNRVkR6CuHTkArYdOMJjP3uL7755gNaOLKT9wY9ZRE6q9IKVC8EzPHzVDG6YP5lx1WUFe6hNB47w+Oq3eHD1jiha2lUUKajSCVZooTPP0oWn8VeLZ1E/onChOtGGA0e44zuvsXpHC5SnQN0SKYjSCFY+5JTqMpb/9zksOrM+liEEFh57aSt3Pbe556KPsYxDpJS5Pw8rF3LpxBrWfO7C2GIF0d7g0kun8svPXhC9kxi6/++ASNK4HayugKun17Fq6UKmjhsR92gAuGBKHTuXXUJFVbr7HUoRGSruBisXcPWZY3n2jgVU+Mn6a0waVcmW/3URM8dWK1oiQyhZr/S+yoV8csY4/u3WC+IeyfuaOKqS5z5zAQ21Fdo9FBki7gUrsMypq+SbS+ZRkUr28CePqeL52+ZDNojmhonIoCT7FX8iC1jLv95+AWOqijdtYTDOmlDDM0vmatdQZAi4FaxswLc+MYvpCTnA3lc3njeZz86bEG1piciAuROsIOTchhpuWXhG3CMZkHuvmgXVZb2vDCEifeJGsCzgeXztutlxj2TAJo+u5FtXTIcubWWJDJQbwcqH3H52PRdMqYt7JINyy0enwMhyvWsoMkBuBItoFnkp+PYV06PzeESk35IfrCDk41PHMGNCTdwjGRKLzp5AQ3Vax7JEBiD5wcqF3PiRyZSVyMnEDTUVXHNWfbT6qYj0S/KDFcJVs0+NexRDasmHG7RbKDIAyQ5WYDl/6hhGpJM9zP6aWl/DpLFVOvgu0k/JLkE+5H/OnRD3KIZc/chyrplUo2CJ9FOyg5XymDJ+ZNyjKIgppypYIv2V3GBZqC73GVtTGfdICuKM+pEKlkg/JTdYWCaW+4yvLc1gTT9FwRLpr+QGy8L48hR1laV56cRZ9SP0TqFIPyU3WJT4ElIl/ZcTKYxEB0tE5FgKlog4Q8ESEWckOli2hA/0hNbqCtEi/ZTcYBk42BXQ1JmPeyQFsfFgu64OLdJPyQ0Whm2ZgF0tHXEPpCDe3NemYIn0U3KDZSCXDWhqy8Q9koJ4e/9hBUukn5IbLIB8yNa9bXGPoiDe2qstLJH+Snaw0h7/9NqeuEcx5Pa2Zfj+zjbwFSyR/kh2sDzD+u3NtGRK68D7pr1tNDZ1gFGwRPoj2cEC8A0rf19aW1nLf7MLUsl/6kWSJvmvmrTPd3/9Dl1BaVzq/Z3WDCs3HtTuoMgAJD9YvmHllibW7W6NeyRDYuXru9nXntPuoMgAJD9YAL7h4Re3xj2KQQuBO5/fDCnFSmQgHAmWx1NvHmDttsa4RzIo3/zZNujQ1pXIQLkRLANYuOFf3nD27MJtje3csWozlJfmgoQixeBGsAB8w87GDh75yea4R9JvIfDFZ9dDLtAJzyKD4E6wANI+d6/azO/2uDX7/clfbOfpdQegxK6vKFJsbr2CDOAbrvvmrzh4pCvu0fTJb99p5tbv/U7zrkSGgHuvIs+wta2LTz3xCm1dyZ4Bv2n/YeY9/gpUpLQrKDIE3AsWQMrjp2+3cu3jv6QroVee2bT/MJd/8xXI5HSSs8gQcTNYAGmPl7c3s/jrv6Ajl6xZ8G8daufMr/6Ct1s6wXf3KRZJGrdfTWU+P9nezPyv/JTf70nGTPgXN+7nQ3/zImTyipXIEHP/FZXyWN/cyfyvruX7r+2K7WLK7dmAv171Jn/4xKvRu4HaDRQZcu4HC8D3yOQD/vjJ17h9+avsai3uKqW/3d3KJQ+t5gsvbItmsWsmu0hBGJatTOZR64HKh9AV8MUrpnHrRWfQUFNRsId6fVcrD/10K0+u3QkjyrRVJVJgpResHtmAhppyrjurntsWnMbU8TVUDsFcqObOHBv2tPLgT7fxg7eaIBtojpVIkZRusACsjba4rOHaqaNZOHUsF59Zz/zJo7D0bWqUBXJByItbGln95j5eeKuJX+8+HK1n5XuaXyVSRKUdrGMFFoIwCljKZ3ZDDRc3jGRmXRVjq9LHnVTtGdjenGFjUwfP7Wpj394jUZhSXhQq7fqJxGL4LB3gG/B9KPPBwrr9h1m3tw1CS69LQHhEB889A1XD52kSSbLh+Uo0HI2RiDhDR4tFxBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnDM9zCUWOZbv/Y0/480mZ45cXMr18ToaUgiXDiyVaJy3s/ggslKcYU5VmYkWK+ooUI9IedeWpD0yWATJByN6OPIG17O7MczAb0JLJQ2c+OrH+3Y/u71DIBk3BktIXdi/k6BlIe0yqLOPC00ZzXkMNH508iurKMqoq01SXpxhZkaYi5ZHqY1wOZwNCC22dWTK5gM6uPJnOHBsb21mzs4WNB9tZv+8wh3Ih5MIoln73umrSb24u4NeeI7bL4wxE2ouu/lworjwfnoHqdOEfxwJhCPloK+rDp49iyaxTmDl5NHMmjWb8iLLCj+EEGw62s3VvK5v3tPK9TY28+lbz8YtC6sIlfeJesNpztD5wJdUVaaxN/tBTvsfPN+zjom+8Uphotefo/IerSae8RD8fnjG0tHdRd9/zhYtWz5ZU2ufGqWNYMH0cN54/iTFVxQ/UybRm8vznm/tYs2E/j25shMNd3ZeH07LbH8S9XUJrSac8fM/gyk825Xt9O4Y7EKE7z0c6VaDnoTtUM8dUcu3Z4/nsR0+nYUw16QQv0FhbkeKGeRO5Yd5ElrV08uqOJr6+ZgfPv9Ma7Tqm9QZ+b9wLFtFhAKcUeMDRllVyX5w9hvxpCC10BYyoq+LbV05n0TmnUlvu3q/0xFGVTJzbwCfmNvD6rha+tWYHj659JzpYn/Zd+NEWjXs/XRFrIRNwTsNI/u+i6Vx/bkPcIxoycyeO4pFPzeW+q2by2Itb+NKandHFU3QpOUATR8U1+ZDKlM/Xr5vN6rsuKqlYHWvCyHL++uOzefPzF3HjzHHdl6tzbddi6ClY4gZrIZPnkzPG8cbdC7njY2dQU8h3XhNi5viRLL/1An5w07kQEoVrGCv9n7i4LwgBw/f/dB7XnTsx7tEUnQH+27kN7J9+Cku/+xr/um4/lKeG5bEtbWFJsuVCPjZhJBv+4uJhGatjnVKd5ju3XsDDH5/ZfT3N4beLqC0sSa5swJ/NncA//slcaofB7l9f+AaWXjqNMSPKWfJvv4+ileDpG0NNW1iSPBY4kuWLi6bxxM3nKVa9uOn8yfzktvnRDHkXznIYIgqWJIuNJoE+fsMcvnDlmXGPJtH+YPo41t75kWhC7jCJloIlyWGBwPL4J2Zx+8IpcY/GCR85fQw/XHJu97SHuEdTeAqWJEd7NorVRWfEPRKnXDlrPP909ZmQDeIeSsEpWJIMXQEPXT+b2xcqVgNx9x9M4/9cOBky+biHUlAKlsQvG3DPx07nrkumxj0Sp9139SwuOWN097y10qRgSbxyIdfNGMuXPj477pE4b3RlmkeunxOtolqix7MULIlPaKkZUcY3Pn1eopeCccnsU2v48uXTIV+ax7MULImHBfIhP771fOqqirAK6TDyvxdN54zRlSU51UHBknjkQ7502VTOnzw67pGUnDLP8NC1sxQskSGRD7n4tFruuXJm3CMpWYvOmsBlk2uj41klRMGS4rIWPI9Hrp9DWoetCqbcN9x7xZnQVVrHshQsKa6ugK8s+hBnn1oT90hK3sIPjeWPZtSV1FaWgiVFY62F6jLu+sPpcQ9lWCjzDbctOK2kFv1TsKRo8ha+e9McyjSFoWj+eN7EaLG/Elk7S8GSohldXc4n5w3vRfji8DcXnx5dOqwEKFhSNJ6Bcl39pegWnz2heysr7pEMnn57RErcnImjuGz8iJKYl6VgiQwD1849tSQOvitYIsPA4ln1JbH2u4IlMgzU1VSwYGKN87uFCpbIMFBbnmLx1DHOr5WlYIkME7OnjI0mwzlMwRIZJi6eOtb503QULJFhYlRFigmOH8dSsESGkZumjXF6K0vBEhlGFkwe7fR5hboGuJSU/e05Nuxr4+DhDB1dAYfbOghyAWAAi/E8RtRUUlNdxvT6Gs4ZPyLuIRfVuLpqSPvRaToOTstSsMRZ+9uzbNrdwtpth/h/W5t4ZVtTdPEF34tejMb0/qK0RFsZ3btGZ04Zzec/fCoXzqjnrPEji/lXKLrT66oZW+bRmO2JuFsULHFKZz5k055WHnxpG798u5ktbdlobpHvQYUP+P2+z417D/OZ/9iAqdrKtZNr+YvLpvHRD40d+sEnwKTaChoqUjR2BS72SsESd6xav4+vvbyNFVuawDfRqSa+Ab//kTpO933YfMgPtxzih5sP8fmPTOK+xbNK8oo+48dU80ZLBheLpYPukni/39vGxQ+tZvE3fsWK7c1Q7kPKG/pz4wzR/aY8Hly7k4a/e5GXtjYO7WMkwHmTa52d2qBgSWIFwKMvbuGcB1fzs3daoSod7foVmgHKfLoyeS59bC3/tWF/4R+ziM6pH+ns1AYFSxLrtuW/YemKjdFvaRwL/3kGUh6XP/kbXtx0oPiPXyDTx1Y5u5ifgiWJk8mH/NFjv+DJV3dDmR+92xcXz4C1XPf0a7zd1BHfOIZQZUUaKtxcgVTBkkTJhZZPPfEKL2w9FL2oksAztGTyXPvEK66fOwxARVmKsVVpXCyWgiWJ8lf/sY4fbWqMtqySJOXxuz2HeWL1trhHMmiVZSkmVWoLS2RQfrJxP195eXs8x6v6Iu1xx8pNHHb8asojK1JMqi5TsEQG6mB7lsuWvx5NWUjq9CBjIBvw0I83xT2SQalMeYyrcPNahQqWJMI//Ncm6Mgmf93xtMfXf7OHA4e74h7JoIwsT9gudx8pWBK7LQcO88Aru6KTcpPOM+xu6uClzW5Pc6iprdQWlshA/P0LmyGbT+6u4InSHk//amfcoxgUz/d0DEukv3Y0d/K9Nw8m90B7bzzDz/ceYfPB9rhHMmCT6tycPOrQb4mUopfX7+VIZy7eyaH9ZQwt7Vm27GqOeyQDVuZ72iUU6a/71+x0a+uqh2f49w0H4x7FgKWKcU5mAbg5aikJ25o62LGzJfnvDPbG9/jWG3vjHsWATR9b7eSKDQqWxOaljQeSN6O9rwzQnmVnaybukQyIg60CFCyJiQV++9ahaPE8V/keb+xujXsUA+JorxQsiUdTe5YVO1vd3B3s4Rt27WuLexQDMrG23MlqKVgSi86uHG8f6nA7WJ5hx8EjcY9iQEZVpvUuoUhfbdx/BPJh3MMYHGNY39RJp4N/DwdbBShYEpOf72h2+/gVgIE3mjrpyrm9eoNLFCyJxfYDR9zeHQQwhl1HsgSBe1tYrlKwJBatrZ1uzW7vjQEUrKJSsKTo2nMhjRmHTnb+IMawo7kz7lEMGwqWFF1rJkdTrkS2Sgx0ZHUMq1gULCm6I115mnJuXir9PTzDxgNuTm1wkYIlRdfZlWd/LqQ0igWBq3MEHKRgSdFlsoH7c7B6GOjULmHRKFhSdK6/OXgcY9ilg+5Fo2CJDFJJBTjhFCyJh17kMgAKlhRdPhdA3ipa0m8KlhRdrisHOv9OBkDBkuIzRltXMiAKlsggBa6uN+wgBUtkMDxoPuTu9Qldo2CJDIr2bYtJwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZTgbLM3GPoH+MKeyAC33/Q82t0ZYm115DPVJxD6DfjKE9kwcgtDGPpQ9SvkdnNl+4V6lnaM/kSKc8rCvPRy4AxyL7QQJrsdbSmQ3iHkqfeIboNeTgz8CwbKUDv+YnaM/hxKuzR8qDigL+2+Da85H2odyPexRDJ7DQmYt7FP1jDFSn4x5Fv7m3hQVOPtEFpecjXr6BEWVxj2JYcPIYlogMTwqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGR5CPewwiIicX5PHIZZxcKlVEhhFjIJfBI5eNeygiIieXy+KR63JrPXARGX6shVwXHl2dELpxtQ8RGabCALo68bAhZNp1HEtEksmYqFE2xMN40NGm3UIRSSZro0YZDw/IkM1qK0tEkqdn6yqbBch4YDfjGWg7pK0sEUkWa6M2eQawmz0w2zAe5HPQ3qKtLBFJBmOiJuVzYDzAbPOAXRgTfbHtEOSyipaIxMuYqEVth3i3T7DLA/sjgnwGDFigeV/3NAdFS0TiYKIGNe+LmoQhapT9UVSlmx/dg2EC1kb7jOWVUDcBRUtEis/Cob3Q1Xl068qyl6c+d2q0WoO1P8Tzo9saE92wab92DUWkuIyJ2tMTKwDPjxrFu8vLeM8Q5DvevYExkDkCjbshDBUuESksY6LWNO6O2nNsi4J8B3jPQE+wnv7zn4NdhfGPuQMvqlzjLsh0dB+lFxEZYsaLGtO4q3vL6pjWGB+wq6JGHbuAX87eR5jnuONWxkRvKTbthbaD0fEtbW2JyFAwpnue1cGoMfncCX0xEOajNnU7ukm17rkm5lx1Cp5//nETSHvuoKszmnEKUFbZ/XnFS0T6wxxtR3sLtBw4epbNiRtD0bGrx3jmrqeP+e4T3PzIOjz/rPddwaFnK2vEKCivgnR5dMfYo18XEYFjItQ9VSHXBV0dcKTlg/fYPB/CYD1PLZ197KdT730A727C4HsYbyw2fP8BHG6OHtRPRdEqK4dUefRnERGAIA/5Lsh2RbEK8kdD9X6xMh6EQSPGu/s9X+r1Gz798P8A7wk8TJ+2mN69jX13Q0tEJCrMMe/4nfT2BkIshLfw9F1P9np3vbr50U9i7Q/wPNPrlpaIyFAyHoShxZjreOpz/97bTfzePgnAG6s2cvaV+4AL8f1KHZsSkYLxfAjDJkL7eZYvXf5+Nzv5NtqSRxfh2W/g+VMIQ7TPJyJDx4DnQRhsJzR3sPxzL5zk1n108yNPA0u6S4jCJSID926oAJbz1NJP9+W7+j59/amln8YL5hMGPwYb4KU0iVRE+scY8FKADQiDH+MF8/saKxjozM8/fXgxofkzDJcAo/BTfrTSQ6h5WCJylDHRwfTonMAAaMHyEp79Nv9818p+392gB7TkqzfhhwuwdhqW0/C8GYqWiHSf0LwJw9sYs4XAW8vyP39mMHf5/wE/pJZJKs/o/AAAAABJRU5ErkJggg==" }</t>
   </si>
   <si>
-    <t>Verify that user is not able to update media witn invalid media ID for profile context by Entity ID using base64 API and check the error status</t>
-  </si>
-  <si>
     <t>/internal/media/1p-profile/profile/(SYS_USER2)/base64</t>
   </si>
   <si>
-    <t>{ "mediaId": "(OPQA-AA02_mediaId)", "base64Media": "data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAASwAAAEsCAYAAAB5fY51AAAABHNCSVQICAgIfAhkiAAAGYBJREFUeJzt3XuYFOWB7/HvW9U9V5gBBhxwAMVwEURBohgMRt2V9YKa5OhuPErcs15iPBv0PDlnZXWfk8c8m82um2fd9RKT+CTGVUyyu8nZTQRW18RoCCExxmgCchdE7gxzg5np6e6q9/xRM3JxlLl1V709v8/zjD7M9HS/9Ex/qap+6y3DYHzm2SpqU0vwgrngTcPaGXhmEtYO6m5FpAQYA6F9B2M2QbiF0H+d1vxyHr+mY8B3OaDvumfV9Rh7J5h5WFtLKm2wIdGHYiUi3YwB40Uf+ZzFmFawr2HN1/j7q77f77vr162XrboGa+/FMwvwfAgDBUpE+s4Y3m1HaNdizN/ywFXP9vnb+/xAy1Y8h192OTaEMAQUKhEZKANe95ZXkH2eB66+oo/fdRJ/ueoWLF/GT9UT5AY9TBGR4/hpCPL7MdzH3131xAfd9IODtWzl/cC9eH4ZYTCEIxQROUa0m5gF/pYHFt//fjfz3/cOlq34Aqmy+7HWx4YFGKGISDdrwRifVPoSLvyUZc13Xu7tZr0Ha9nK+0mV3U8+j45ViUjRhBZS6Uu58AbDmu+8dOKX37tL+JerbsHar2FMmd4BFJGiMwaszWLMnSce0/Lec2PLl/F8xUpE4mEtUYP48olfOj5Yy1Y8h5+q1wF2EYlVGICfqmfZiueO/fTRYC1bdQ1+2eWauiAiiRDkwC+7nGWrrun51NFgWXuv3g0UkUSJTve7t+ePUbDuWXU9nlkQzWAXEUmIMATPLOCeVddDT7CMvRPPR1MYRCRZbDSp1Ng7AQyfebaK0f5uDKP0zqCIJI4xYGmhOWhIUZtagg1r4x6TiEivrAVLLbWpJR5eMJdUemDrYomIFEMqbfCCuV60UqgOtotIgtkQ8KZ5WDtDwRKRRIumN8zwtAa7iCSeteCZSZ5iJSJOsLaXk59FRBJKwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOCMV9wBiYYHQHv3obdVVzxz/ISKxGz7BCkLIW8iHkPY597RRXDapltnjqjhlRNlxzfIMbG3qZP3BDla83cI7u9sACykPfA98BUwkDqUdrLA7UBhuPGscl8wYx8IZ9cwcV33Sb728+/+Pdf//17taeWndHlZuauTlHS1R1VImuiqtiBSFYdnK0rsKhQWyAWefUs31cyZw8/zJNNRVkR6CuHTkArYdOMJjP3uL7755gNaOLKT9wY9ZRE6q9IKVC8EzPHzVDG6YP5lx1WUFe6hNB47w+Oq3eHD1jiha2lUUKajSCVZooTPP0oWn8VeLZ1E/onChOtGGA0e44zuvsXpHC5SnQN0SKYjSCFY+5JTqMpb/9zksOrM+liEEFh57aSt3Pbe556KPsYxDpJS5Pw8rF3LpxBrWfO7C2GIF0d7g0kun8svPXhC9kxi6/++ASNK4HayugKun17Fq6UKmjhsR92gAuGBKHTuXXUJFVbr7HUoRGSruBisXcPWZY3n2jgVU+Mn6a0waVcmW/3URM8dWK1oiQyhZr/S+yoV8csY4/u3WC+IeyfuaOKqS5z5zAQ21Fdo9FBki7gUrsMypq+SbS+ZRkUr28CePqeL52+ZDNojmhonIoCT7FX8iC1jLv95+AWOqijdtYTDOmlDDM0vmatdQZAi4FaxswLc+MYvpCTnA3lc3njeZz86bEG1piciAuROsIOTchhpuWXhG3CMZkHuvmgXVZb2vDCEifeJGsCzgeXztutlxj2TAJo+u5FtXTIcubWWJDJQbwcqH3H52PRdMqYt7JINyy0enwMhyvWsoMkBuBItoFnkp+PYV06PzeESk35IfrCDk41PHMGNCTdwjGRKLzp5AQ3Vax7JEBiD5wcqF3PiRyZSVyMnEDTUVXHNWfbT6qYj0S/KDFcJVs0+NexRDasmHG7RbKDIAyQ5WYDl/6hhGpJM9zP6aWl/DpLFVOvgu0k/JLkE+5H/OnRD3KIZc/chyrplUo2CJ9FOyg5XymDJ+ZNyjKIgppypYIv2V3GBZqC73GVtTGfdICuKM+pEKlkg/JTdYWCaW+4yvLc1gTT9FwRLpr+QGy8L48hR1laV56cRZ9SP0TqFIPyU3WJT4ElIl/ZcTKYxEB0tE5FgKlog4Q8ESEWckOli2hA/0hNbqCtEi/ZTcYBk42BXQ1JmPeyQFsfFgu64OLdJPyQ0Whm2ZgF0tHXEPpCDe3NemYIn0U3KDZSCXDWhqy8Q9koJ4e/9hBUukn5IbLIB8yNa9bXGPoiDe2qstLJH+Snaw0h7/9NqeuEcx5Pa2Zfj+zjbwFSyR/kh2sDzD+u3NtGRK68D7pr1tNDZ1gFGwRPoj2cEC8A0rf19aW1nLf7MLUsl/6kWSJvmvmrTPd3/9Dl1BaVzq/Z3WDCs3HtTuoMgAJD9YvmHllibW7W6NeyRDYuXru9nXntPuoMgAJD9YAL7h4Re3xj2KQQuBO5/fDCnFSmQgHAmWx1NvHmDttsa4RzIo3/zZNujQ1pXIQLkRLANYuOFf3nD27MJtje3csWozlJfmgoQixeBGsAB8w87GDh75yea4R9JvIfDFZ9dDLtAJzyKD4E6wANI+d6/azO/2uDX7/clfbOfpdQegxK6vKFJsbr2CDOAbrvvmrzh4pCvu0fTJb99p5tbv/U7zrkSGgHuvIs+wta2LTz3xCm1dyZ4Bv2n/YeY9/gpUpLQrKDIE3AsWQMrjp2+3cu3jv6QroVee2bT/MJd/8xXI5HSSs8gQcTNYAGmPl7c3s/jrv6Ajl6xZ8G8daufMr/6Ct1s6wXf3KRZJGrdfTWU+P9nezPyv/JTf70nGTPgXN+7nQ3/zImTyipXIEHP/FZXyWN/cyfyvruX7r+2K7WLK7dmAv171Jn/4xKvRu4HaDRQZcu4HC8D3yOQD/vjJ17h9+avsai3uKqW/3d3KJQ+t5gsvbItmsWsmu0hBGJatTOZR64HKh9AV8MUrpnHrRWfQUFNRsId6fVcrD/10K0+u3QkjyrRVJVJgpResHtmAhppyrjurntsWnMbU8TVUDsFcqObOHBv2tPLgT7fxg7eaIBtojpVIkZRusACsjba4rOHaqaNZOHUsF59Zz/zJo7D0bWqUBXJByItbGln95j5eeKuJX+8+HK1n5XuaXyVSRKUdrGMFFoIwCljKZ3ZDDRc3jGRmXRVjq9LHnVTtGdjenGFjUwfP7Wpj394jUZhSXhQq7fqJxGL4LB3gG/B9KPPBwrr9h1m3tw1CS69LQHhEB889A1XD52kSSbLh+Uo0HI2RiDhDR4tFxBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnDM9zCUWOZbv/Y0/480mZ45cXMr18ToaUgiXDiyVaJy3s/ggslKcYU5VmYkWK+ooUI9IedeWpD0yWATJByN6OPIG17O7MczAb0JLJQ2c+OrH+3Y/u71DIBk3BktIXdi/k6BlIe0yqLOPC00ZzXkMNH508iurKMqoq01SXpxhZkaYi5ZHqY1wOZwNCC22dWTK5gM6uPJnOHBsb21mzs4WNB9tZv+8wh3Ih5MIoln73umrSb24u4NeeI7bL4wxE2ouu/lworjwfnoHqdOEfxwJhCPloK+rDp49iyaxTmDl5NHMmjWb8iLLCj+EEGw62s3VvK5v3tPK9TY28+lbz8YtC6sIlfeJesNpztD5wJdUVaaxN/tBTvsfPN+zjom+8Uphotefo/IerSae8RD8fnjG0tHdRd9/zhYtWz5ZU2ufGqWNYMH0cN54/iTFVxQ/UybRm8vznm/tYs2E/j25shMNd3ZeH07LbH8S9XUJrSac8fM/gyk825Xt9O4Y7EKE7z0c6VaDnoTtUM8dUcu3Z4/nsR0+nYUw16QQv0FhbkeKGeRO5Yd5ElrV08uqOJr6+ZgfPv9Ma7Tqm9QZ+b9wLFtFhAKcUeMDRllVyX5w9hvxpCC10BYyoq+LbV05n0TmnUlvu3q/0xFGVTJzbwCfmNvD6rha+tWYHj659JzpYn/Zd+NEWjXs/XRFrIRNwTsNI/u+i6Vx/bkPcIxoycyeO4pFPzeW+q2by2Itb+NKandHFU3QpOUATR8U1+ZDKlM/Xr5vN6rsuKqlYHWvCyHL++uOzefPzF3HjzHHdl6tzbddi6ClY4gZrIZPnkzPG8cbdC7njY2dQU8h3XhNi5viRLL/1An5w07kQEoVrGCv9n7i4LwgBw/f/dB7XnTsx7tEUnQH+27kN7J9+Cku/+xr/um4/lKeG5bEtbWFJsuVCPjZhJBv+4uJhGatjnVKd5ju3XsDDH5/ZfT3N4beLqC0sSa5swJ/NncA//slcaofB7l9f+AaWXjqNMSPKWfJvv4+ileDpG0NNW1iSPBY4kuWLi6bxxM3nKVa9uOn8yfzktvnRDHkXznIYIgqWJIuNJoE+fsMcvnDlmXGPJtH+YPo41t75kWhC7jCJloIlyWGBwPL4J2Zx+8IpcY/GCR85fQw/XHJu97SHuEdTeAqWJEd7NorVRWfEPRKnXDlrPP909ZmQDeIeSsEpWJIMXQEPXT+b2xcqVgNx9x9M4/9cOBky+biHUlAKlsQvG3DPx07nrkumxj0Sp9139SwuOWN097y10qRgSbxyIdfNGMuXPj477pE4b3RlmkeunxOtolqix7MULIlPaKkZUcY3Pn1eopeCccnsU2v48uXTIV+ax7MULImHBfIhP771fOqqirAK6TDyvxdN54zRlSU51UHBknjkQ7502VTOnzw67pGUnDLP8NC1sxQskSGRD7n4tFruuXJm3CMpWYvOmsBlk2uj41klRMGS4rIWPI9Hrp9DWoetCqbcN9x7xZnQVVrHshQsKa6ugK8s+hBnn1oT90hK3sIPjeWPZtSV1FaWgiVFY62F6jLu+sPpcQ9lWCjzDbctOK2kFv1TsKRo8ha+e9McyjSFoWj+eN7EaLG/Elk7S8GSohldXc4n5w3vRfji8DcXnx5dOqwEKFhSNJ6Bcl39pegWnz2heysr7pEMnn57RErcnImjuGz8iJKYl6VgiQwD1849tSQOvitYIsPA4ln1JbH2u4IlMgzU1VSwYGKN87uFCpbIMFBbnmLx1DHOr5WlYIkME7OnjI0mwzlMwRIZJi6eOtb503QULJFhYlRFigmOH8dSsESGkZumjXF6K0vBEhlGFkwe7fR5hboGuJSU/e05Nuxr4+DhDB1dAYfbOghyAWAAi/E8RtRUUlNdxvT6Gs4ZPyLuIRfVuLpqSPvRaToOTstSsMRZ+9uzbNrdwtpth/h/W5t4ZVtTdPEF34tejMb0/qK0RFsZ3btGZ04Zzec/fCoXzqjnrPEji/lXKLrT66oZW+bRmO2JuFsULHFKZz5k055WHnxpG798u5ktbdlobpHvQYUP+P2+z417D/OZ/9iAqdrKtZNr+YvLpvHRD40d+sEnwKTaChoqUjR2BS72SsESd6xav4+vvbyNFVuawDfRqSa+Ab//kTpO933YfMgPtxzih5sP8fmPTOK+xbNK8oo+48dU80ZLBheLpYPukni/39vGxQ+tZvE3fsWK7c1Q7kPKG/pz4wzR/aY8Hly7k4a/e5GXtjYO7WMkwHmTa52d2qBgSWIFwKMvbuGcB1fzs3daoSod7foVmgHKfLoyeS59bC3/tWF/4R+ziM6pH+ns1AYFSxLrtuW/YemKjdFvaRwL/3kGUh6XP/kbXtx0oPiPXyDTx1Y5u5ifgiWJk8mH/NFjv+DJV3dDmR+92xcXz4C1XPf0a7zd1BHfOIZQZUUaKtxcgVTBkkTJhZZPPfEKL2w9FL2oksAztGTyXPvEK66fOwxARVmKsVVpXCyWgiWJ8lf/sY4fbWqMtqySJOXxuz2HeWL1trhHMmiVZSkmVWoLS2RQfrJxP195eXs8x6v6Iu1xx8pNHHb8asojK1JMqi5TsEQG6mB7lsuWvx5NWUjq9CBjIBvw0I83xT2SQalMeYyrcPNahQqWJMI//Ncm6Mgmf93xtMfXf7OHA4e74h7JoIwsT9gudx8pWBK7LQcO88Aru6KTcpPOM+xu6uClzW5Pc6iprdQWlshA/P0LmyGbT+6u4InSHk//amfcoxgUz/d0DEukv3Y0d/K9Nw8m90B7bzzDz/ceYfPB9rhHMmCT6tycPOrQb4mUopfX7+VIZy7eyaH9ZQwt7Vm27GqOeyQDVuZ72iUU6a/71+x0a+uqh2f49w0H4x7FgKWKcU5mAbg5aikJ25o62LGzJfnvDPbG9/jWG3vjHsWATR9b7eSKDQqWxOaljQeSN6O9rwzQnmVnaybukQyIg60CFCyJiQV++9ahaPE8V/keb+xujXsUA+JorxQsiUdTe5YVO1vd3B3s4Rt27WuLexQDMrG23MlqKVgSi86uHG8f6nA7WJ5hx8EjcY9iQEZVpvUuoUhfbdx/BPJh3MMYHGNY39RJp4N/DwdbBShYEpOf72h2+/gVgIE3mjrpyrm9eoNLFCyJxfYDR9zeHQQwhl1HsgSBe1tYrlKwJBatrZ1uzW7vjQEUrKJSsKTo2nMhjRmHTnb+IMawo7kz7lEMGwqWFF1rJkdTrkS2Sgx0ZHUMq1gULCm6I115mnJuXir9PTzDxgNuTm1wkYIlRdfZlWd/LqQ0igWBq3MEHKRgSdFlsoH7c7B6GOjULmHRKFhSdK6/OXgcY9ilg+5Fo2CJDFJJBTjhFCyJh17kMgAKlhRdPhdA3ipa0m8KlhRdrisHOv9OBkDBkuIzRltXMiAKlsggBa6uN+wgBUtkMDxoPuTu9Qldo2CJDIr2bYtJwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZTgbLM3GPoH+MKeyAC33/Q82t0ZYm115DPVJxD6DfjKE9kwcgtDGPpQ9SvkdnNl+4V6lnaM/kSKc8rCvPRy4AxyL7QQJrsdbSmQ3iHkqfeIboNeTgz8CwbKUDv+YnaM/hxKuzR8qDigL+2+Da85H2odyPexRDJ7DQmYt7FP1jDFSn4x5Fv7m3hQVOPtEFpecjXr6BEWVxj2JYcPIYlogMTwqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGR5CPewwiIicX5PHIZZxcKlVEhhFjIJfBI5eNeygiIieXy+KR63JrPXARGX6shVwXHl2dELpxtQ8RGabCALo68bAhZNp1HEtEksmYqFE2xMN40NGm3UIRSSZro0YZDw/IkM1qK0tEkqdn6yqbBch4YDfjGWg7pK0sEUkWa6M2eQawmz0w2zAe5HPQ3qKtLBFJBmOiJuVzYDzAbPOAXRgTfbHtEOSyipaIxMuYqEVth3i3T7DLA/sjgnwGDFigeV/3NAdFS0TiYKIGNe+LmoQhapT9UVSlmx/dg2EC1kb7jOWVUDcBRUtEis/Cob3Q1Xl068qyl6c+d2q0WoO1P8Tzo9saE92wab92DUWkuIyJ2tMTKwDPjxrFu8vLeM8Q5DvevYExkDkCjbshDBUuESksY6LWNO6O2nNsi4J8B3jPQE+wnv7zn4NdhfGPuQMvqlzjLsh0dB+lFxEZYsaLGtO4q3vL6pjWGB+wq6JGHbuAX87eR5jnuONWxkRvKTbthbaD0fEtbW2JyFAwpnue1cGoMfncCX0xEOajNnU7ukm17rkm5lx1Cp5//nETSHvuoKszmnEKUFbZ/XnFS0T6wxxtR3sLtBw4epbNiRtD0bGrx3jmrqeP+e4T3PzIOjz/rPddwaFnK2vEKCivgnR5dMfYo18XEYFjItQ9VSHXBV0dcKTlg/fYPB/CYD1PLZ197KdT730A727C4HsYbyw2fP8BHG6OHtRPRdEqK4dUefRnERGAIA/5Lsh2RbEK8kdD9X6xMh6EQSPGu/s9X+r1Gz798P8A7wk8TJ+2mN69jX13Q0tEJCrMMe/4nfT2BkIshLfw9F1P9np3vbr50U9i7Q/wPNPrlpaIyFAyHoShxZjreOpz/97bTfzePgnAG6s2cvaV+4AL8f1KHZsSkYLxfAjDJkL7eZYvXf5+Nzv5NtqSRxfh2W/g+VMIQ7TPJyJDx4DnQRhsJzR3sPxzL5zk1n108yNPA0u6S4jCJSID926oAJbz1NJP9+W7+j59/amln8YL5hMGPwYb4KU0iVRE+scY8FKADQiDH+MF8/saKxjozM8/fXgxofkzDJcAo/BTfrTSQ6h5WCJylDHRwfTonMAAaMHyEp79Nv9818p+392gB7TkqzfhhwuwdhqW0/C8GYqWiHSf0LwJw9sYs4XAW8vyP39mMHf5/wE/pJZJKs/o/AAAAABJRU5ErkJggg==" }</t>
-  </si>
-  <si>
     <t>OPQA-AA06</t>
   </si>
   <si>
     <t>OPQA-AA07</t>
   </si>
   <si>
-    <t>{ "mediaId": "(OPQA-AA02_mediaId)", "pathPrefix" : "stable-pics1", "base64Media": "data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAMgAAADLCAYAAAArzNwwAAAAGXRFWHRTb2Z0d2FyZQBBZG9iZSBJbWFnZVJlYWR5ccllPAAADylJREFUeNrsnb1y20gWhRvwuso1ienM2VCRNxsqm0xUttGYfAJR2WYys8kkPYHIJxAZTW0karKNTGWTGcrWkaFM2XKSqZlysNtXurBhivjvBvrnnCoUbYmkgO7++tzb3WgIAUEQBEEQBClWgCJoR98NfurJlwH/t89HWi9Tv090s+OrYj5I0R/RrxuULgCxBYKk4Q/l8X0KhL7mPx3JY8Ovd/wKeABI544w5F7/gF97hp1mAg050RrQAJA2gHjLr31LLyViWG4kLCvULABpAsWAYTjakR+4ohU7zEoCE6PWAUgZKAiIkcUu0cRdloAFgOwKnyaOO0VVrVOwbACIn2Ak4dMEPOQm+hSGzSUoEQDxwy0ofDr1MIRS4ioSlAUAcROMd/I4EeYNx9omyk/OfQi/AoABNQy/5vKYuQpKADAgVaBISM4AiB1wnAGM7kIvl3KUwDEwKPm+QPJtRDJPoKwBiBlgEBCX4nHWGzJH5CRTm/OT0JFw6gPgMFITeXySdTSBg7QPxoBdAzPf9oRdx7YtYXlmsWv8Io/XaHfWiMLgyfPXb/76fP/xNziIvlzjCq5hvVbsJsbnJqFFcEw41wAc9mvEuYnxeeMzS+CgXIPCqhdoW87oBYdcgQy51gixEFJBFoZcgcFwEBTvBWbDfVHEkBi1pD40FI4k3wAc/uihQzQtLwkNhIOWilyivXipHkMyQZKenYz/E+3Ee41MSd4DQ8DosWuM0DaglBYyJzn22kEYDkrGh2gP0HZeIp2kL53k2ktAUnBgGBcyEpJngAMCJIYBAjggWyDpapgXcEB1NOGRTncdhC/wH6hrqIGT9KST/Ns5QBiOCeoYaqgfJSR3EhLty1LCFuF4BzgghbrkTTq0KmgJDrqQK9QppFi0+vdQ5wLHoAU4sCoX0qlYHvu6lsqHmuHosXMADkiX+jqjE905yKXAJm6Qfg15FbhyaRvF4p1HsDIXaks0snX7+f7jf4zPQfiml/eoM6iDpH1f5d5boQY4kqXrENS2lLc9HTkI8o78Hm4mj7E8DpND9njk5K/4/1PxuKdtjOKqnY+cGRliYb4jU9TYKz8WgHd1oXD1QNj9bPYutK9ifiRQCAfZ2yeBId1tx5iqel5G6rntJ4ClUJEs9/2mX6JsFOv56ze0Vy5W6H7VQyglK0nZPrSf7z/e07628pjL8qZl33+Kx/2J0Sk91WsV97UrcRCMWj1xjXGbD49hZ6HHWY/gLE+012RUK1BQOdR7fUDFPGjNcHS2QyBvmXMkcI//lzqR9XHYWYglbexngd1ISLQDx1ha+p9dngQtAZfHkpaDc8jre/jVbzKB2MhBeJQFOyAasD1Njrufisen/fosCrFqLWhsOg9yCjjMhINEDUIeNK9yyLmRty5St5Oo7SBIzM2GIyOR9/mRdRtO2Ct1FE0c5NRzOGgSamrLyfKk2SGft4+iSKfyit9aDgL30H8nm2Yn8fkGtkrDvnUdxHf3mNsIR8pJxh7XXaW2W9lB4B4ilo1sz/aL4BuMfB3dKu0ioW4CHdS5Q9fh68hW6TZcyUHgHm64R6o+zzzu8F6VGdGq6iBHnrvHyrHrmXlcl6XCy9KA8Kz5xHNAli5dDPegK0/r8kR1DnLiORwbW0euCnTtaX32yjwLsQogvruHqxNsa4/r9EQJIEya72uuYhcvioc7fR3NGvDEaWMH8T05J93BHf1zkUJAUhsHQJCLGjV1ENwM5b5uPL72Xt5jFMoAcoL2Azmuo1qAcALTR/lBrodZfPdlZQdBeAX5omEdQN6i3LzQDyiC3W09zAmvKLTCRnBfdeByoorq3R0thVUtBwIgrpYBr1YvDQjCq2/Vd/jaEClkmAIcxHNAipZa+J6HhDmFBtvdnZfBPRx20u3h3hDu4b2LYAQrp+1nAXKAcvKmt0VnmFPHcJBq6gF653WQCwjH2cg/ditGESDEQo+yWwtVj1IzTDNU7ROTGACQ6po6el3nqNon6ucBglGNp1p3+dQonXL1ulTlZXAQCMpJ1MM8e4G+CIMWntZ3mJWcQH64qqOrA7SFWOgpsxuSq5AAkJyOYxuQIYrGOxdBned0HCHKoXrihuvyFxAM8frX08JBKgCCHCSnwFxLaPP2g4J2J+lQvi4cux7seVYQeoaeJKKqNCqzZb4l7nGG8Kq6gyDE8sBF+K65U1QlQiwd6jmQiyBSACBoYDlCaFWyjABIgwQO5w8HgRzrgTn/gIMAEL0hlsV5COAAIGhoOcLj9ABIK7Juko3DK8yeAxCEWRl6h2oDIG3Kmsk2dg8sLQEgrSrz0V0GaiKwUqKKNgCkuXo2hC1YWlJLEQBRlKxbkIu8g3uoCbFiFEktFzG2d2Z44R4ApNv4ftfjuwzRJaoHOYgRDdG0hF2eD4VWQ1RNLd3CQdSKQpkLg+AYCPfugOw8xLpDkTQOtSYGwEFOdoXqaKSdo1jYyLi5LrrcZI7heC+wIZyWHCRCuTTWQwPtcOiXwircMajJQZCDqIPkqu2kXf49GrGaoPibK3ksRLj1QwCiToO2nIRAlMd7wKHWPXY5CMIs9ZB80JmTMIAExxDFrUxxHiBwET05yUQDHHRvxwfkHMp1mwfILcqntjY5kNBEopK8hFyDvks8DuVijVXLIdYa5VMbjkN57OeAQj3+J9rVsA4onGucsWvk3Rm4EBiyVwJIsKsS5Mt/UUbV4fgj+jXiMhxw794v+Aw15GXyuYJQ6m2JJJy+81h+34rP4RLhV/W6lOX3KhMQrpBPAhNNteDY6miuSibPMfda6fD2JTfussk3fX6cHonkc7gUuA+9ilayDMdFgGA8vZzW3GPHOb0/hUS6l5ufy3M4yzmHIZ/DEFVWrSyzVvPeoJxKhTKHRXNHXNh7mnI7+s69PDj4HOh91Cueo+pKlakocpABJ4LQUzDm8pglM60Vk2xVPfmKzoMbftVz6PM5IELY3ZkEhYAgD1ELRkYHdMS5QdkyphxjyTFyrOAcElDoHDBUzO5BUUFZQJCHPCbPS1Vg5MAyYFC+59dNKmEnl4h0/X0+B6rnt0jmxVSW86wsIBPh7+2a1Chp+HXh00Wndl488jSh398ejQwKCsun+ZA4FdvHwnNxCDZhWHwItWNZ73vbPwwKCsn1RXAbhuKaJtcQgudGE667ykK2gePtH/6t4EPXDhYKoKgoDjUXnC+dOJqbXu/6YZGDkLV+cqQAVpxXAAp1ucqJcGMpyzfLS0oDwoVh+3LqFY9OxGjaWmChCMP2Wfqd4RWpzL5Yc4uTbprpHgMOreFXMncwFfauIF5m/aIMIDaGJHTO+3VmmqHaoND8AS31t+2O1DivnYQlLjxZlm2TXY51TqxBmW3lwbUt61SXeb8su/XotS3OkRVLQq1B8rCQ0yInWTQGhEd+TI/jk4qBzIHEhg41VuEgNiTr5wirjIIksiA0Xxa9oQogC2HuKEW8vcgMMkJTw9vMShkg3DubmnzhRiBzQ62FzW0mdKAhxr6turVMJobmpTv7sGKPEBvYIyzRBo12ERPbzLxsvlrnCVOmuQjcw3yZ1IkRGKXz1dDyHmGFZSRWuMhamDNNMK8y2ln3GYWmuMg1mp81MmGAp5J71AbEEBfZIDlHmKXTPZo4iAkuskabsyrMijoOs+Kq7tEIEHaRLiFBeIUwq1KHXmelRdPnpM9EdzOluDPQPnXVqUV1w/FGgDCR044uGOuu7AuzugqLa7fRUMFFLzrIB5B/IMwqq0UTMMOuCa0pbK5tr9qsu8YRjhJAeISizYQdDmKv2ryR6rhpKB6oPJuWdkCh/GMf7cxeyXbyvzZCufSDcLoOsb4QC/eADKhDZXc0KgWkpVALT+FFmKU9tNLlIMkTlSKLCxfSL52d3ELl7pmhppMcC00TiEVPhIW8dpBYKB5RDTU14lhTPoL8wwFp7OSU74cWaiwEsrmZhh4CQqKelXcoBy/UWQLyhKeKC+IO7coZqezsFrpufQhbKIixwsJAiOWOVHV2kc7dNLUDwjGhqqQdCxQRYm270KHOk2zDQZKk7FjR90BuaKPg89o3KQ/bKg1O2ptAAjgckoLObtxGhxm2XCiUSNWdaUd4hUQ90XFb95aEbZcIz7TXGXGAgwCQBI5FWycYdlEqPOpQ9SJ/R3vyHpDjtneyCbsqmRqQwEHc053JcHQKSA1IkIO4p43JcHQOSEVIAIh7ikyGwwhAUpDMCt6DEMs/HXe9e2ZoSknwuq3MeZLvBj9N0F6c01FOtDA2YWvZwLQSYxAu5NHb8WsqsCn2xLJbso6pbq/kMcyA49CUiCEwtABp44f3GZBEQtPSZqiVuiUoLuXRz6jbsUmPtAhNLERu/HsZSdwDPAi5rITjjDu+XXCs2Dlik845MLxAexxuZcGwEgpv0Ie01WOfXWOY8ZZzXmFhnAJLCjgvL9kwJNjM2sy6eydfTnPqbtzhnr1uAJLKSy5F9sZ0K07gYzRLY+rrIsc11tyxGV1fz2wp8M/3H++fv37zL/nPF/L4ccdb/k6hmHzPX/K9v6GJdhcWyzr4Wf7zl4xcIwmpjmU9GR8aB5ZWwojdpJfxlojdZI0m23oofJoDhnUjkIHFldFjSEY5b7PCxh0AY8hgDHPeZmwi7iQgW5VzmdNrkRZcQQBFbdn3Rf7olJWu4RQgKTdJRksEQGkFDCrrSc7bNlzWM5uvNXCw4i4Kwi6AojeUIs1EzYdmAhCzKpJylDnmUEol3yei+NkvzuV8geMVO2JH6Re8lSqUHnS/gKt848YnHEb1SoBx7uKoYeBJZU9E/vBjWuQm9LjilW9LWDiXG5V0C6fB8AqQGqFXkmQSLDcuw5KC4m2J3C3dicx9mGfyCpBUoxikwgdRoVEksMQOXD91Ekei/DMlkw7Dq8ENLwHZ6j2TBLRf4aMxhxcETGT6GH8KiAN+7VX4OF3b3MeQ03tAdoRfRxxm9Cp+fMMN6YZf466g4esg2H9gdxjW+JqY3WLp+41pAGR3I0vH5L0GXxWl4Pk99X9RJ35nx0tCoj4fL/ln/YoumBVCXWPYG4BUheWAYelr/nOx+Lrb4KAhnGUBXsMpAIgqWPpbsXzfskuIUqHgCndiApA2gBnwcdBSr1/FjQiGW3aJCEAAEBOg6aWg6TE4ukKmTSqvuU1CNNwHA0Bsh2i49aM8eBIIvggAQBAEQRAEQRbr/wIMAB2nwEL3kwxHAAAAAElFTkSuQmCC" }</t>
-  </si>
-  <si>
     <t>status=200||mediaId=(OPQA-AA02_mediaId)||entityId=(SYS_USER2)||entityType=profile||mediaType=image/png||context=1p-profile</t>
   </si>
   <si>
     <t>Verify that user is able to update his own media with custom pathPrefix for profile context by Entity ID using base64 API</t>
   </si>
   <si>
-    <t>Verify that user is not able to update media witn invalid Entity ID for profile context using base64 API and check the error status</t>
-  </si>
-  <si>
     <t>/internal/media/1p-profile/profile/(SYS_USER1)A/base64</t>
   </si>
   <si>
@@ -266,13 +251,97 @@
     <t>Verify that user is able to delete his own media by using Delete Media by Entity ID/Type API</t>
   </si>
   <si>
-    <t>status=200||mediaId=(OPQA-AA01_mediaId)||entityId=(SYS_USER1)||entityType=profile||mediaType=image/jpeg||context=1p-profile</t>
-  </si>
-  <si>
     <t>status=500||statusCode=500</t>
   </si>
   <si>
     <t>/media/1p-profile/profile/(SYS_USER2)A</t>
+  </si>
+  <si>
+    <t>{ "mediaId": "(OPQA-AA01_mediaId)", "mediaType" : "image/png", "base64Media": "data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAASwAAAEsCAYAAAB5fY51AAAABHNCSVQICAgIfAhkiAAAGYBJREFUeJzt3XuYFOWB7/HvW9U9V5gBBhxwAMVwEURBohgMRt2V9YKa5OhuPErcs15iPBv0PDlnZXWfk8c8m82um2fd9RKT+CTGVUyyu8nZTQRW18RoCCExxmgCchdE7gxzg5np6e6q9/xRM3JxlLl1V709v8/zjD7M9HS/9Ex/qap+6y3DYHzm2SpqU0vwgrngTcPaGXhmEtYO6m5FpAQYA6F9B2M2QbiF0H+d1vxyHr+mY8B3OaDvumfV9Rh7J5h5WFtLKm2wIdGHYiUi3YwB40Uf+ZzFmFawr2HN1/j7q77f77vr162XrboGa+/FMwvwfAgDBUpE+s4Y3m1HaNdizN/ywFXP9vnb+/xAy1Y8h192OTaEMAQUKhEZKANe95ZXkH2eB66+oo/fdRJ/ueoWLF/GT9UT5AY9TBGR4/hpCPL7MdzH3131xAfd9IODtWzl/cC9eH4ZYTCEIxQROUa0m5gF/pYHFt//fjfz3/cOlq34Aqmy+7HWx4YFGKGISDdrwRifVPoSLvyUZc13Xu7tZr0Ha9nK+0mV3U8+j45ViUjRhBZS6Uu58AbDmu+8dOKX37tL+JerbsHar2FMmd4BFJGiMwaszWLMnSce0/Lec2PLl/F8xUpE4mEtUYP48olfOj5Yy1Y8h5+q1wF2EYlVGICfqmfZiueO/fTRYC1bdQ1+2eWauiAiiRDkwC+7nGWrrun51NFgWXuv3g0UkUSJTve7t+ePUbDuWXU9nlkQzWAXEUmIMATPLOCeVddDT7CMvRPPR1MYRCRZbDSp1Ng7AQyfebaK0f5uDKP0zqCIJI4xYGmhOWhIUZtagg1r4x6TiEivrAVLLbWpJR5eMJdUemDrYomIFEMqbfCCuV60UqgOtotIgtkQ8KZ5WDtDwRKRRIumN8zwtAa7iCSeteCZSZ5iJSJOsLaXk59FRBJKwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOCMV9wBiYYHQHv3obdVVzxz/ISKxGz7BCkLIW8iHkPY597RRXDapltnjqjhlRNlxzfIMbG3qZP3BDla83cI7u9sACykPfA98BUwkDqUdrLA7UBhuPGscl8wYx8IZ9cwcV33Sb728+/+Pdf//17taeWndHlZuauTlHS1R1VImuiqtiBSFYdnK0rsKhQWyAWefUs31cyZw8/zJNNRVkR6CuHTkArYdOMJjP3uL7755gNaOLKT9wY9ZRE6q9IKVC8EzPHzVDG6YP5lx1WUFe6hNB47w+Oq3eHD1jiha2lUUKajSCVZooTPP0oWn8VeLZ1E/onChOtGGA0e44zuvsXpHC5SnQN0SKYjSCFY+5JTqMpb/9zksOrM+liEEFh57aSt3Pbe556KPsYxDpJS5Pw8rF3LpxBrWfO7C2GIF0d7g0kun8svPXhC9kxi6/++ASNK4HayugKun17Fq6UKmjhsR92gAuGBKHTuXXUJFVbr7HUoRGSruBisXcPWZY3n2jgVU+Mn6a0waVcmW/3URM8dWK1oiQyhZr/S+yoV8csY4/u3WC+IeyfuaOKqS5z5zAQ21Fdo9FBki7gUrsMypq+SbS+ZRkUr28CePqeL52+ZDNojmhonIoCT7FX8iC1jLv95+AWOqijdtYTDOmlDDM0vmatdQZAi4FaxswLc+MYvpCTnA3lc3njeZz86bEG1piciAuROsIOTchhpuWXhG3CMZkHuvmgXVZb2vDCEifeJGsCzgeXztutlxj2TAJo+u5FtXTIcubWWJDJQbwcqH3H52PRdMqYt7JINyy0enwMhyvWsoMkBuBItoFnkp+PYV06PzeESk35IfrCDk41PHMGNCTdwjGRKLzp5AQ3Vax7JEBiD5wcqF3PiRyZSVyMnEDTUVXHNWfbT6qYj0S/KDFcJVs0+NexRDasmHG7RbKDIAyQ5WYDl/6hhGpJM9zP6aWl/DpLFVOvgu0k/JLkE+5H/OnRD3KIZc/chyrplUo2CJ9FOyg5XymDJ+ZNyjKIgppypYIv2V3GBZqC73GVtTGfdICuKM+pEKlkg/JTdYWCaW+4yvLc1gTT9FwRLpr+QGy8L48hR1laV56cRZ9SP0TqFIPyU3WJT4ElIl/ZcTKYxEB0tE5FgKlog4Q8ESEWckOli2hA/0hNbqCtEi/ZTcYBk42BXQ1JmPeyQFsfFgu64OLdJPyQ0Whm2ZgF0tHXEPpCDe3NemYIn0U3KDZSCXDWhqy8Q9koJ4e/9hBUukn5IbLIB8yNa9bXGPoiDe2qstLJH+Snaw0h7/9NqeuEcx5Pa2Zfj+zjbwFSyR/kh2sDzD+u3NtGRK68D7pr1tNDZ1gFGwRPoj2cEC8A0rf19aW1nLf7MLUsl/6kWSJvmvmrTPd3/9Dl1BaVzq/Z3WDCs3HtTuoMgAJD9YvmHllibW7W6NeyRDYuXru9nXntPuoMgAJD9YAL7h4Re3xj2KQQuBO5/fDCnFSmQgHAmWx1NvHmDttsa4RzIo3/zZNujQ1pXIQLkRLANYuOFf3nD27MJtje3csWozlJfmgoQixeBGsAB8w87GDh75yea4R9JvIfDFZ9dDLtAJzyKD4E6wANI+d6/azO/2uDX7/clfbOfpdQegxK6vKFJsbr2CDOAbrvvmrzh4pCvu0fTJb99p5tbv/U7zrkSGgHuvIs+wta2LTz3xCm1dyZ4Bv2n/YeY9/gpUpLQrKDIE3AsWQMrjp2+3cu3jv6QroVee2bT/MJd/8xXI5HSSs8gQcTNYAGmPl7c3s/jrv6Ajl6xZ8G8daufMr/6Ct1s6wXf3KRZJGrdfTWU+P9nezPyv/JTf70nGTPgXN+7nQ3/zImTyipXIEHP/FZXyWN/cyfyvruX7r+2K7WLK7dmAv171Jn/4xKvRu4HaDRQZcu4HC8D3yOQD/vjJ17h9+avsai3uKqW/3d3KJQ+t5gsvbItmsWsmu0hBGJatTOZR64HKh9AV8MUrpnHrRWfQUFNRsId6fVcrD/10K0+u3QkjyrRVJVJgpResHtmAhppyrjurntsWnMbU8TVUDsFcqObOHBv2tPLgT7fxg7eaIBtojpVIkZRusACsjba4rOHaqaNZOHUsF59Zz/zJo7D0bWqUBXJByItbGln95j5eeKuJX+8+HK1n5XuaXyVSRKUdrGMFFoIwCljKZ3ZDDRc3jGRmXRVjq9LHnVTtGdjenGFjUwfP7Wpj394jUZhSXhQq7fqJxGL4LB3gG/B9KPPBwrr9h1m3tw1CS69LQHhEB889A1XD52kSSbLh+Uo0HI2RiDhDR4tFxBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnDM9zCUWOZbv/Y0/480mZ45cXMr18ToaUgiXDiyVaJy3s/ggslKcYU5VmYkWK+ooUI9IedeWpD0yWATJByN6OPIG17O7MczAb0JLJQ2c+OrH+3Y/u71DIBk3BktIXdi/k6BlIe0yqLOPC00ZzXkMNH508iurKMqoq01SXpxhZkaYi5ZHqY1wOZwNCC22dWTK5gM6uPJnOHBsb21mzs4WNB9tZv+8wh3Ih5MIoln73umrSb24u4NeeI7bL4wxE2ouu/lworjwfnoHqdOEfxwJhCPloK+rDp49iyaxTmDl5NHMmjWb8iLLCj+EEGw62s3VvK5v3tPK9TY28+lbz8YtC6sIlfeJesNpztD5wJdUVaaxN/tBTvsfPN+zjom+8Uphotefo/IerSae8RD8fnjG0tHdRd9/zhYtWz5ZU2ufGqWNYMH0cN54/iTFVxQ/UybRm8vznm/tYs2E/j25shMNd3ZeH07LbH8S9XUJrSac8fM/gyk825Xt9O4Y7EKE7z0c6VaDnoTtUM8dUcu3Z4/nsR0+nYUw16QQv0FhbkeKGeRO5Yd5ElrV08uqOJr6+ZgfPv9Ma7Tqm9QZ+b9wLFtFhAKcUeMDRllVyX5w9hvxpCC10BYyoq+LbV05n0TmnUlvu3q/0xFGVTJzbwCfmNvD6rha+tWYHj659JzpYn/Zd+NEWjXs/XRFrIRNwTsNI/u+i6Vx/bkPcIxoycyeO4pFPzeW+q2by2Itb+NKandHFU3QpOUATR8U1+ZDKlM/Xr5vN6rsuKqlYHWvCyHL++uOzefPzF3HjzHHdl6tzbddi6ClY4gZrIZPnkzPG8cbdC7njY2dQU8h3XhNi5viRLL/1An5w07kQEoVrGCv9n7i4LwgBw/f/dB7XnTsx7tEUnQH+27kN7J9+Cku/+xr/um4/lKeG5bEtbWFJsuVCPjZhJBv+4uJhGatjnVKd5ju3XsDDH5/ZfT3N4beLqC0sSa5swJ/NncA//slcaofB7l9f+AaWXjqNMSPKWfJvv4+ileDpG0NNW1iSPBY4kuWLi6bxxM3nKVa9uOn8yfzktvnRDHkXznIYIgqWJIuNJoE+fsMcvnDlmXGPJtH+YPo41t75kWhC7jCJloIlyWGBwPL4J2Zx+8IpcY/GCR85fQw/XHJu97SHuEdTeAqWJEd7NorVRWfEPRKnXDlrPP909ZmQDeIeSsEpWJIMXQEPXT+b2xcqVgNx9x9M4/9cOBky+biHUlAKlsQvG3DPx07nrkumxj0Sp9139SwuOWN097y10qRgSbxyIdfNGMuXPj477pE4b3RlmkeunxOtolqix7MULIlPaKkZUcY3Pn1eopeCccnsU2v48uXTIV+ax7MULImHBfIhP771fOqqirAK6TDyvxdN54zRlSU51UHBknjkQ7502VTOnzw67pGUnDLP8NC1sxQskSGRD7n4tFruuXJm3CMpWYvOmsBlk2uj41klRMGS4rIWPI9Hrp9DWoetCqbcN9x7xZnQVVrHshQsKa6ugK8s+hBnn1oT90hK3sIPjeWPZtSV1FaWgiVFY62F6jLu+sPpcQ9lWCjzDbctOK2kFv1TsKRo8ha+e9McyjSFoWj+eN7EaLG/Elk7S8GSohldXc4n5w3vRfji8DcXnx5dOqwEKFhSNJ6Bcl39pegWnz2heysr7pEMnn57RErcnImjuGz8iJKYl6VgiQwD1849tSQOvitYIsPA4ln1JbH2u4IlMgzU1VSwYGKN87uFCpbIMFBbnmLx1DHOr5WlYIkME7OnjI0mwzlMwRIZJi6eOtb503QULJFhYlRFigmOH8dSsESGkZumjXF6K0vBEhlGFkwe7fR5hboGuJSU/e05Nuxr4+DhDB1dAYfbOghyAWAAi/E8RtRUUlNdxvT6Gs4ZPyLuIRfVuLpqSPvRaToOTstSsMRZ+9uzbNrdwtpth/h/W5t4ZVtTdPEF34tejMb0/qK0RFsZ3btGZ04Zzec/fCoXzqjnrPEji/lXKLrT66oZW+bRmO2JuFsULHFKZz5k055WHnxpG798u5ktbdlobpHvQYUP+P2+z417D/OZ/9iAqdrKtZNr+YvLpvHRD40d+sEnwKTaChoqUjR2BS72SsESd6xav4+vvbyNFVuawDfRqSa+Ab//kTpO933YfMgPtxzih5sP8fmPTOK+xbNK8oo+48dU80ZLBheLpYPukni/39vGxQ+tZvE3fsWK7c1Q7kPKG/pz4wzR/aY8Hly7k4a/e5GXtjYO7WMkwHmTa52d2qBgSWIFwKMvbuGcB1fzs3daoSod7foVmgHKfLoyeS59bC3/tWF/4R+ziM6pH+ns1AYFSxLrtuW/YemKjdFvaRwL/3kGUh6XP/kbXtx0oPiPXyDTx1Y5u5ifgiWJk8mH/NFjv+DJV3dDmR+92xcXz4C1XPf0a7zd1BHfOIZQZUUaKtxcgVTBkkTJhZZPPfEKL2w9FL2oksAztGTyXPvEK66fOwxARVmKsVVpXCyWgiWJ8lf/sY4fbWqMtqySJOXxuz2HeWL1trhHMmiVZSkmVWoLS2RQfrJxP195eXs8x6v6Iu1xx8pNHHb8asojK1JMqi5TsEQG6mB7lsuWvx5NWUjq9CBjIBvw0I83xT2SQalMeYyrcPNahQqWJMI//Ncm6Mgmf93xtMfXf7OHA4e74h7JoIwsT9gudx8pWBK7LQcO88Aru6KTcpPOM+xu6uClzW5Pc6iprdQWlshA/P0LmyGbT+6u4InSHk//amfcoxgUz/d0DEukv3Y0d/K9Nw8m90B7bzzDz/ceYfPB9rhHMmCT6tycPOrQb4mUopfX7+VIZy7eyaH9ZQwt7Vm27GqOeyQDVuZ72iUU6a/71+x0a+uqh2f49w0H4x7FgKWKcU5mAbg5aikJ25o62LGzJfnvDPbG9/jWG3vjHsWATR9b7eSKDQqWxOaljQeSN6O9rwzQnmVnaybukQyIg60CFCyJiQV++9ahaPE8V/keb+xujXsUA+JorxQsiUdTe5YVO1vd3B3s4Rt27WuLexQDMrG23MlqKVgSi86uHG8f6nA7WJ5hx8EjcY9iQEZVpvUuoUhfbdx/BPJh3MMYHGNY39RJp4N/DwdbBShYEpOf72h2+/gVgIE3mjrpyrm9eoNLFCyJxfYDR9zeHQQwhl1HsgSBe1tYrlKwJBatrZ1uzW7vjQEUrKJSsKTo2nMhjRmHTnb+IMawo7kz7lEMGwqWFF1rJkdTrkS2Sgx0ZHUMq1gULCm6I115mnJuXir9PTzDxgNuTm1wkYIlRdfZlWd/LqQ0igWBq3MEHKRgSdFlsoH7c7B6GOjULmHRKFhSdK6/OXgcY9ilg+5Fo2CJDFJJBTjhFCyJh17kMgAKlhRdPhdA3ipa0m8KlhRdrisHOv9OBkDBkuIzRltXMiAKlsggBa6uN+wgBUtkMDxoPuTu9Qldo2CJDIr2bYtJwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZTgbLM3GPoH+MKeyAC33/Q82t0ZYm115DPVJxD6DfjKE9kwcgtDGPpQ9SvkdnNl+4V6lnaM/kSKc8rCvPRy4AxyL7QQJrsdbSmQ3iHkqfeIboNeTgz8CwbKUDv+YnaM/hxKuzR8qDigL+2+Da85H2odyPexRDJ7DQmYt7FP1jDFSn4x5Fv7m3hQVOPtEFpecjXr6BEWVxj2JYcPIYlogMTwqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGR5CPewwiIicX5PHIZZxcKlVEhhFjIJfBI5eNeygiIieXy+KR63JrPXARGX6shVwXHl2dELpxtQ8RGabCALo68bAhZNp1HEtEksmYqFE2xMN40NGm3UIRSSZro0YZDw/IkM1qK0tEkqdn6yqbBch4YDfjGWg7pK0sEUkWa6M2eQawmz0w2zAe5HPQ3qKtLBFJBmOiJuVzYDzAbPOAXRgTfbHtEOSyipaIxMuYqEVth3i3T7DLA/sjgnwGDFigeV/3NAdFS0TiYKIGNe+LmoQhapT9UVSlmx/dg2EC1kb7jOWVUDcBRUtEis/Cob3Q1Xl068qyl6c+d2q0WoO1P8Tzo9saE92wab92DUWkuIyJ2tMTKwDPjxrFu8vLeM8Q5DvevYExkDkCjbshDBUuESksY6LWNO6O2nNsi4J8B3jPQE+wnv7zn4NdhfGPuQMvqlzjLsh0dB+lFxEZYsaLGtO4q3vL6pjWGB+wq6JGHbuAX87eR5jnuONWxkRvKTbthbaD0fEtbW2JyFAwpnue1cGoMfncCX0xEOajNnU7ukm17rkm5lx1Cp5//nETSHvuoKszmnEKUFbZ/XnFS0T6wxxtR3sLtBw4epbNiRtD0bGrx3jmrqeP+e4T3PzIOjz/rPddwaFnK2vEKCivgnR5dMfYo18XEYFjItQ9VSHXBV0dcKTlg/fYPB/CYD1PLZ197KdT730A727C4HsYbyw2fP8BHG6OHtRPRdEqK4dUefRnERGAIA/5Lsh2RbEK8kdD9X6xMh6EQSPGu/s9X+r1Gz798P8A7wk8TJ+2mN69jX13Q0tEJCrMMe/4nfT2BkIshLfw9F1P9np3vbr50U9i7Q/wPNPrlpaIyFAyHoShxZjreOpz/97bTfzePgnAG6s2cvaV+4AL8f1KHZsSkYLxfAjDJkL7eZYvXf5+Nzv5NtqSRxfh2W/g+VMIQ7TPJyJDx4DnQRhsJzR3sPxzL5zk1n108yNPA0u6S4jCJSID926oAJbz1NJP9+W7+j59/amln8YL5hMGPwYb4KU0iVRE+scY8FKADQiDH+MF8/saKxjozM8/fXgxofkzDJcAo/BTfrTSQ6h5WCJylDHRwfTonMAAaMHyEp79Nv9818p+392gB7TkqzfhhwuwdhqW0/C8GYqWiHSf0LwJw9sYs4XAW8vyP39mMHf5/wE/pJZJKs/o/AAAAABJRU5ErkJggg==" }</t>
+  </si>
+  <si>
+    <t>status=200||mediaId=(OPQA-AA01_mediaId)||entityId=(SYS_USER1)||entityType=profile||mediaType=image/png||context=1p-profile</t>
+  </si>
+  <si>
+    <t>{ "mediaId": "(OPQA-AA02_mediaId)", "mediaType" : "image/png", "base64Media": "data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAASwAAAEsCAYAAAB5fY51AAAABHNCSVQICAgIfAhkiAAAGYBJREFUeJzt3XuYFOWB7/HvW9U9V5gBBhxwAMVwEURBohgMRt2V9YKa5OhuPErcs15iPBv0PDlnZXWfk8c8m82um2fd9RKT+CTGVUyyu8nZTQRW18RoCCExxmgCchdE7gxzg5np6e6q9/xRM3JxlLl1V709v8/zjD7M9HS/9Ex/qap+6y3DYHzm2SpqU0vwgrngTcPaGXhmEtYO6m5FpAQYA6F9B2M2QbiF0H+d1vxyHr+mY8B3OaDvumfV9Rh7J5h5WFtLKm2wIdGHYiUi3YwB40Uf+ZzFmFawr2HN1/j7q77f77vr162XrboGa+/FMwvwfAgDBUpE+s4Y3m1HaNdizN/ywFXP9vnb+/xAy1Y8h192OTaEMAQUKhEZKANe95ZXkH2eB66+oo/fdRJ/ueoWLF/GT9UT5AY9TBGR4/hpCPL7MdzH3131xAfd9IODtWzl/cC9eH4ZYTCEIxQROUa0m5gF/pYHFt//fjfz3/cOlq34Aqmy+7HWx4YFGKGISDdrwRifVPoSLvyUZc13Xu7tZr0Ha9nK+0mV3U8+j45ViUjRhBZS6Uu58AbDmu+8dOKX37tL+JerbsHar2FMmd4BFJGiMwaszWLMnSce0/Lec2PLl/F8xUpE4mEtUYP48olfOj5Yy1Y8h5+q1wF2EYlVGICfqmfZiueO/fTRYC1bdQ1+2eWauiAiiRDkwC+7nGWrrun51NFgWXuv3g0UkUSJTve7t+ePUbDuWXU9nlkQzWAXEUmIMATPLOCeVddDT7CMvRPPR1MYRCRZbDSp1Ng7AQyfebaK0f5uDKP0zqCIJI4xYGmhOWhIUZtagg1r4x6TiEivrAVLLbWpJR5eMJdUemDrYomIFEMqbfCCuV60UqgOtotIgtkQ8KZ5WDtDwRKRRIumN8zwtAa7iCSeteCZSZ5iJSJOsLaXk59FRBJKwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOCMV9wBiYYHQHv3obdVVzxz/ISKxGz7BCkLIW8iHkPY597RRXDapltnjqjhlRNlxzfIMbG3qZP3BDla83cI7u9sACykPfA98BUwkDqUdrLA7UBhuPGscl8wYx8IZ9cwcV33Sb728+/+Pdf//17taeWndHlZuauTlHS1R1VImuiqtiBSFYdnK0rsKhQWyAWefUs31cyZw8/zJNNRVkR6CuHTkArYdOMJjP3uL7755gNaOLKT9wY9ZRE6q9IKVC8EzPHzVDG6YP5lx1WUFe6hNB47w+Oq3eHD1jiha2lUUKajSCVZooTPP0oWn8VeLZ1E/onChOtGGA0e44zuvsXpHC5SnQN0SKYjSCFY+5JTqMpb/9zksOrM+liEEFh57aSt3Pbe556KPsYxDpJS5Pw8rF3LpxBrWfO7C2GIF0d7g0kun8svPXhC9kxi6/++ASNK4HayugKun17Fq6UKmjhsR92gAuGBKHTuXXUJFVbr7HUoRGSruBisXcPWZY3n2jgVU+Mn6a0waVcmW/3URM8dWK1oiQyhZr/S+yoV8csY4/u3WC+IeyfuaOKqS5z5zAQ21Fdo9FBki7gUrsMypq+SbS+ZRkUr28CePqeL52+ZDNojmhonIoCT7FX8iC1jLv95+AWOqijdtYTDOmlDDM0vmatdQZAi4FaxswLc+MYvpCTnA3lc3njeZz86bEG1piciAuROsIOTchhpuWXhG3CMZkHuvmgXVZb2vDCEifeJGsCzgeXztutlxj2TAJo+u5FtXTIcubWWJDJQbwcqH3H52PRdMqYt7JINyy0enwMhyvWsoMkBuBItoFnkp+PYV06PzeESk35IfrCDk41PHMGNCTdwjGRKLzp5AQ3Vax7JEBiD5wcqF3PiRyZSVyMnEDTUVXHNWfbT6qYj0S/KDFcJVs0+NexRDasmHG7RbKDIAyQ5WYDl/6hhGpJM9zP6aWl/DpLFVOvgu0k/JLkE+5H/OnRD3KIZc/chyrplUo2CJ9FOyg5XymDJ+ZNyjKIgppypYIv2V3GBZqC73GVtTGfdICuKM+pEKlkg/JTdYWCaW+4yvLc1gTT9FwRLpr+QGy8L48hR1laV56cRZ9SP0TqFIPyU3WJT4ElIl/ZcTKYxEB0tE5FgKlog4Q8ESEWckOli2hA/0hNbqCtEi/ZTcYBk42BXQ1JmPeyQFsfFgu64OLdJPyQ0Whm2ZgF0tHXEPpCDe3NemYIn0U3KDZSCXDWhqy8Q9koJ4e/9hBUukn5IbLIB8yNa9bXGPoiDe2qstLJH+Snaw0h7/9NqeuEcx5Pa2Zfj+zjbwFSyR/kh2sDzD+u3NtGRK68D7pr1tNDZ1gFGwRPoj2cEC8A0rf19aW1nLf7MLUsl/6kWSJvmvmrTPd3/9Dl1BaVzq/Z3WDCs3HtTuoMgAJD9YvmHllibW7W6NeyRDYuXru9nXntPuoMgAJD9YAL7h4Re3xj2KQQuBO5/fDCnFSmQgHAmWx1NvHmDttsa4RzIo3/zZNujQ1pXIQLkRLANYuOFf3nD27MJtje3csWozlJfmgoQixeBGsAB8w87GDh75yea4R9JvIfDFZ9dDLtAJzyKD4E6wANI+d6/azO/2uDX7/clfbOfpdQegxK6vKFJsbr2CDOAbrvvmrzh4pCvu0fTJb99p5tbv/U7zrkSGgHuvIs+wta2LTz3xCm1dyZ4Bv2n/YeY9/gpUpLQrKDIE3AsWQMrjp2+3cu3jv6QroVee2bT/MJd/8xXI5HSSs8gQcTNYAGmPl7c3s/jrv6Ajl6xZ8G8daufMr/6Ct1s6wXf3KRZJGrdfTWU+P9nezPyv/JTf70nGTPgXN+7nQ3/zImTyipXIEHP/FZXyWN/cyfyvruX7r+2K7WLK7dmAv171Jn/4xKvRu4HaDRQZcu4HC8D3yOQD/vjJ17h9+avsai3uKqW/3d3KJQ+t5gsvbItmsWsmu0hBGJatTOZR64HKh9AV8MUrpnHrRWfQUFNRsId6fVcrD/10K0+u3QkjyrRVJVJgpResHtmAhppyrjurntsWnMbU8TVUDsFcqObOHBv2tPLgT7fxg7eaIBtojpVIkZRusACsjba4rOHaqaNZOHUsF59Zz/zJo7D0bWqUBXJByItbGln95j5eeKuJX+8+HK1n5XuaXyVSRKUdrGMFFoIwCljKZ3ZDDRc3jGRmXRVjq9LHnVTtGdjenGFjUwfP7Wpj394jUZhSXhQq7fqJxGL4LB3gG/B9KPPBwrr9h1m3tw1CS69LQHhEB889A1XD52kSSbLh+Uo0HI2RiDhDR4tFxBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnDM9zCUWOZbv/Y0/480mZ45cXMr18ToaUgiXDiyVaJy3s/ggslKcYU5VmYkWK+ooUI9IedeWpD0yWATJByN6OPIG17O7MczAb0JLJQ2c+OrH+3Y/u71DIBk3BktIXdi/k6BlIe0yqLOPC00ZzXkMNH508iurKMqoq01SXpxhZkaYi5ZHqY1wOZwNCC22dWTK5gM6uPJnOHBsb21mzs4WNB9tZv+8wh3Ih5MIoln73umrSb24u4NeeI7bL4wxE2ouu/lworjwfnoHqdOEfxwJhCPloK+rDp49iyaxTmDl5NHMmjWb8iLLCj+EEGw62s3VvK5v3tPK9TY28+lbz8YtC6sIlfeJesNpztD5wJdUVaaxN/tBTvsfPN+zjom+8Uphotefo/IerSae8RD8fnjG0tHdRd9/zhYtWz5ZU2ufGqWNYMH0cN54/iTFVxQ/UybRm8vznm/tYs2E/j25shMNd3ZeH07LbH8S9XUJrSac8fM/gyk825Xt9O4Y7EKE7z0c6VaDnoTtUM8dUcu3Z4/nsR0+nYUw16QQv0FhbkeKGeRO5Yd5ElrV08uqOJr6+ZgfPv9Ma7Tqm9QZ+b9wLFtFhAKcUeMDRllVyX5w9hvxpCC10BYyoq+LbV05n0TmnUlvu3q/0xFGVTJzbwCfmNvD6rha+tWYHj659JzpYn/Zd+NEWjXs/XRFrIRNwTsNI/u+i6Vx/bkPcIxoycyeO4pFPzeW+q2by2Itb+NKandHFU3QpOUATR8U1+ZDKlM/Xr5vN6rsuKqlYHWvCyHL++uOzefPzF3HjzHHdl6tzbddi6ClY4gZrIZPnkzPG8cbdC7njY2dQU8h3XhNi5viRLL/1An5w07kQEoVrGCv9n7i4LwgBw/f/dB7XnTsx7tEUnQH+27kN7J9+Cku/+xr/um4/lKeG5bEtbWFJsuVCPjZhJBv+4uJhGatjnVKd5ju3XsDDH5/ZfT3N4beLqC0sSa5swJ/NncA//slcaofB7l9f+AaWXjqNMSPKWfJvv4+ileDpG0NNW1iSPBY4kuWLi6bxxM3nKVa9uOn8yfzktvnRDHkXznIYIgqWJIuNJoE+fsMcvnDlmXGPJtH+YPo41t75kWhC7jCJloIlyWGBwPL4J2Zx+8IpcY/GCR85fQw/XHJu97SHuEdTeAqWJEd7NorVRWfEPRKnXDlrPP909ZmQDeIeSsEpWJIMXQEPXT+b2xcqVgNx9x9M4/9cOBky+biHUlAKlsQvG3DPx07nrkumxj0Sp9139SwuOWN097y10qRgSbxyIdfNGMuXPj477pE4b3RlmkeunxOtolqix7MULIlPaKkZUcY3Pn1eopeCccnsU2v48uXTIV+ax7MULImHBfIhP771fOqqirAK6TDyvxdN54zRlSU51UHBknjkQ7502VTOnzw67pGUnDLP8NC1sxQskSGRD7n4tFruuXJm3CMpWYvOmsBlk2uj41klRMGS4rIWPI9Hrp9DWoetCqbcN9x7xZnQVVrHshQsKa6ugK8s+hBnn1oT90hK3sIPjeWPZtSV1FaWgiVFY62F6jLu+sPpcQ9lWCjzDbctOK2kFv1TsKRo8ha+e9McyjSFoWj+eN7EaLG/Elk7S8GSohldXc4n5w3vRfji8DcXnx5dOqwEKFhSNJ6Bcl39pegWnz2heysr7pEMnn57RErcnImjuGz8iJKYl6VgiQwD1849tSQOvitYIsPA4ln1JbH2u4IlMgzU1VSwYGKN87uFCpbIMFBbnmLx1DHOr5WlYIkME7OnjI0mwzlMwRIZJi6eOtb503QULJFhYlRFigmOH8dSsESGkZumjXF6K0vBEhlGFkwe7fR5hboGuJSU/e05Nuxr4+DhDB1dAYfbOghyAWAAi/E8RtRUUlNdxvT6Gs4ZPyLuIRfVuLpqSPvRaToOTstSsMRZ+9uzbNrdwtpth/h/W5t4ZVtTdPEF34tejMb0/qK0RFsZ3btGZ04Zzec/fCoXzqjnrPEji/lXKLrT66oZW+bRmO2JuFsULHFKZz5k055WHnxpG798u5ktbdlobpHvQYUP+P2+z417D/OZ/9iAqdrKtZNr+YvLpvHRD40d+sEnwKTaChoqUjR2BS72SsESd6xav4+vvbyNFVuawDfRqSa+Ab//kTpO933YfMgPtxzih5sP8fmPTOK+xbNK8oo+48dU80ZLBheLpYPukni/39vGxQ+tZvE3fsWK7c1Q7kPKG/pz4wzR/aY8Hly7k4a/e5GXtjYO7WMkwHmTa52d2qBgSWIFwKMvbuGcB1fzs3daoSod7foVmgHKfLoyeS59bC3/tWF/4R+ziM6pH+ns1AYFSxLrtuW/YemKjdFvaRwL/3kGUh6XP/kbXtx0oPiPXyDTx1Y5u5ifgiWJk8mH/NFjv+DJV3dDmR+92xcXz4C1XPf0a7zd1BHfOIZQZUUaKtxcgVTBkkTJhZZPPfEKL2w9FL2oksAztGTyXPvEK66fOwxARVmKsVVpXCyWgiWJ8lf/sY4fbWqMtqySJOXxuz2HeWL1trhHMmiVZSkmVWoLS2RQfrJxP195eXs8x6v6Iu1xx8pNHHb8asojK1JMqi5TsEQG6mB7lsuWvx5NWUjq9CBjIBvw0I83xT2SQalMeYyrcPNahQqWJMI//Ncm6Mgmf93xtMfXf7OHA4e74h7JoIwsT9gudx8pWBK7LQcO88Aru6KTcpPOM+xu6uClzW5Pc6iprdQWlshA/P0LmyGbT+6u4InSHk//amfcoxgUz/d0DEukv3Y0d/K9Nw8m90B7bzzDz/ceYfPB9rhHMmCT6tycPOrQb4mUopfX7+VIZy7eyaH9ZQwt7Vm27GqOeyQDVuZ72iUU6a/71+x0a+uqh2f49w0H4x7FgKWKcU5mAbg5aikJ25o62LGzJfnvDPbG9/jWG3vjHsWATR9b7eSKDQqWxOaljQeSN6O9rwzQnmVnaybukQyIg60CFCyJiQV++9ahaPE8V/keb+xujXsUA+JorxQsiUdTe5YVO1vd3B3s4Rt27WuLexQDMrG23MlqKVgSi86uHG8f6nA7WJ5hx8EjcY9iQEZVpvUuoUhfbdx/BPJh3MMYHGNY39RJp4N/DwdbBShYEpOf72h2+/gVgIE3mjrpyrm9eoNLFCyJxfYDR9zeHQQwhl1HsgSBe1tYrlKwJBatrZ1uzW7vjQEUrKJSsKTo2nMhjRmHTnb+IMawo7kz7lEMGwqWFF1rJkdTrkS2Sgx0ZHUMq1gULCm6I115mnJuXir9PTzDxgNuTm1wkYIlRdfZlWd/LqQ0igWBq3MEHKRgSdFlsoH7c7B6GOjULmHRKFhSdK6/OXgcY9ilg+5Fo2CJDFJJBTjhFCyJh17kMgAKlhRdPhdA3ipa0m8KlhRdrisHOv9OBkDBkuIzRltXMiAKlsggBa6uN+wgBUtkMDxoPuTu9Qldo2CJDIr2bYtJwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZTgbLM3GPoH+MKeyAC33/Q82t0ZYm115DPVJxD6DfjKE9kwcgtDGPpQ9SvkdnNl+4V6lnaM/kSKc8rCvPRy4AxyL7QQJrsdbSmQ3iHkqfeIboNeTgz8CwbKUDv+YnaM/hxKuzR8qDigL+2+Da85H2odyPexRDJ7DQmYt7FP1jDFSn4x5Fv7m3hQVOPtEFpecjXr6BEWVxj2JYcPIYlogMTwqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGR5CPewwiIicX5PHIZZxcKlVEhhFjIJfBI5eNeygiIieXy+KR63JrPXARGX6shVwXHl2dELpxtQ8RGabCALo68bAhZNp1HEtEksmYqFE2xMN40NGm3UIRSSZro0YZDw/IkM1qK0tEkqdn6yqbBch4YDfjGWg7pK0sEUkWa6M2eQawmz0w2zAe5HPQ3qKtLBFJBmOiJuVzYDzAbPOAXRgTfbHtEOSyipaIxMuYqEVth3i3T7DLA/sjgnwGDFigeV/3NAdFS0TiYKIGNe+LmoQhapT9UVSlmx/dg2EC1kb7jOWVUDcBRUtEis/Cob3Q1Xl068qyl6c+d2q0WoO1P8Tzo9saE92wab92DUWkuIyJ2tMTKwDPjxrFu8vLeM8Q5DvevYExkDkCjbshDBUuESksY6LWNO6O2nNsi4J8B3jPQE+wnv7zn4NdhfGPuQMvqlzjLsh0dB+lFxEZYsaLGtO4q3vL6pjWGB+wq6JGHbuAX87eR5jnuONWxkRvKTbthbaD0fEtbW2JyFAwpnue1cGoMfncCX0xEOajNnU7ukm17rkm5lx1Cp5//nETSHvuoKszmnEKUFbZ/XnFS0T6wxxtR3sLtBw4epbNiRtD0bGrx3jmrqeP+e4T3PzIOjz/rPddwaFnK2vEKCivgnR5dMfYo18XEYFjItQ9VSHXBV0dcKTlg/fYPB/CYD1PLZ197KdT730A727C4HsYbyw2fP8BHG6OHtRPRdEqK4dUefRnERGAIA/5Lsh2RbEK8kdD9X6xMh6EQSPGu/s9X+r1Gz798P8A7wk8TJ+2mN69jX13Q0tEJCrMMe/4nfT2BkIshLfw9F1P9np3vbr50U9i7Q/wPNPrlpaIyFAyHoShxZjreOpz/97bTfzePgnAG6s2cvaV+4AL8f1KHZsSkYLxfAjDJkL7eZYvXf5+Nzv5NtqSRxfh2W/g+VMIQ7TPJyJDx4DnQRhsJzR3sPxzL5zk1n108yNPA0u6S4jCJSID926oAJbz1NJP9+W7+j59/amln8YL5hMGPwYb4KU0iVRE+scY8FKADQiDH+MF8/saKxjozM8/fXgxofkzDJcAo/BTfrTSQ6h5WCJylDHRwfTonMAAaMHyEp79Nv9818p+392gB7TkqzfhhwuwdhqW0/C8GYqWiHSf0LwJw9sYs4XAW8vyP39mMHf5/wE/pJZJKs/o/AAAAABJRU5ErkJggg==" }</t>
+  </si>
+  <si>
+    <t>{ "mediaId": "(OPQA-AA02_mediaId)", "mediaType" : "image/png", "pathPrefix" : "stable-pics1", "base64Media": "data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAMgAAADLCAYAAAArzNwwAAAAGXRFWHRTb2Z0d2FyZQBBZG9iZSBJbWFnZVJlYWR5ccllPAAADylJREFUeNrsnb1y20gWhRvwuso1ienM2VCRNxsqm0xUttGYfAJR2WYys8kkPYHIJxAZTW0karKNTGWTGcrWkaFM2XKSqZlysNtXurBhivjvBvrnnCoUbYmkgO7++tzb3WgIAUEQBEEQBClWgCJoR98NfurJlwH/t89HWi9Tv090s+OrYj5I0R/RrxuULgCxBYKk4Q/l8X0KhL7mPx3JY8Ovd/wKeABI544w5F7/gF97hp1mAg050RrQAJA2gHjLr31LLyViWG4kLCvULABpAsWAYTjakR+4ohU7zEoCE6PWAUgZKAiIkcUu0cRdloAFgOwKnyaOO0VVrVOwbACIn2Ak4dMEPOQm+hSGzSUoEQDxwy0ofDr1MIRS4ioSlAUAcROMd/I4EeYNx9omyk/OfQi/AoABNQy/5vKYuQpKADAgVaBISM4AiB1wnAGM7kIvl3KUwDEwKPm+QPJtRDJPoKwBiBlgEBCX4nHWGzJH5CRTm/OT0JFw6gPgMFITeXySdTSBg7QPxoBdAzPf9oRdx7YtYXlmsWv8Io/XaHfWiMLgyfPXb/76fP/xNziIvlzjCq5hvVbsJsbnJqFFcEw41wAc9mvEuYnxeeMzS+CgXIPCqhdoW87oBYdcgQy51gixEFJBFoZcgcFwEBTvBWbDfVHEkBi1pD40FI4k3wAc/uihQzQtLwkNhIOWilyivXipHkMyQZKenYz/E+3Ee41MSd4DQ8DosWuM0DaglBYyJzn22kEYDkrGh2gP0HZeIp2kL53k2ktAUnBgGBcyEpJngAMCJIYBAjggWyDpapgXcEB1NOGRTncdhC/wH6hrqIGT9KST/Ns5QBiOCeoYaqgfJSR3EhLty1LCFuF4BzgghbrkTTq0KmgJDrqQK9QppFi0+vdQ5wLHoAU4sCoX0qlYHvu6lsqHmuHosXMADkiX+jqjE905yKXAJm6Qfg15FbhyaRvF4p1HsDIXaks0snX7+f7jf4zPQfiml/eoM6iDpH1f5d5boQY4kqXrENS2lLc9HTkI8o78Hm4mj7E8DpND9njk5K/4/1PxuKdtjOKqnY+cGRliYb4jU9TYKz8WgHd1oXD1QNj9bPYutK9ifiRQCAfZ2yeBId1tx5iqel5G6rntJ4ClUJEs9/2mX6JsFOv56ze0Vy5W6H7VQyglK0nZPrSf7z/e07628pjL8qZl33+Kx/2J0Sk91WsV97UrcRCMWj1xjXGbD49hZ6HHWY/gLE+012RUK1BQOdR7fUDFPGjNcHS2QyBvmXMkcI//lzqR9XHYWYglbexngd1ISLQDx1ha+p9dngQtAZfHkpaDc8jre/jVbzKB2MhBeJQFOyAasD1Njrufisen/fosCrFqLWhsOg9yCjjMhINEDUIeNK9yyLmRty5St5Oo7SBIzM2GIyOR9/mRdRtO2Ct1FE0c5NRzOGgSamrLyfKk2SGft4+iSKfyit9aDgL30H8nm2Yn8fkGtkrDvnUdxHf3mNsIR8pJxh7XXaW2W9lB4B4ilo1sz/aL4BuMfB3dKu0ioW4CHdS5Q9fh68hW6TZcyUHgHm64R6o+zzzu8F6VGdGq6iBHnrvHyrHrmXlcl6XCy9KA8Kz5xHNAli5dDPegK0/r8kR1DnLiORwbW0euCnTtaX32yjwLsQogvruHqxNsa4/r9EQJIEya72uuYhcvioc7fR3NGvDEaWMH8T05J93BHf1zkUJAUhsHQJCLGjV1ENwM5b5uPL72Xt5jFMoAcoL2Azmuo1qAcALTR/lBrodZfPdlZQdBeAX5omEdQN6i3LzQDyiC3W09zAmvKLTCRnBfdeByoorq3R0thVUtBwIgrpYBr1YvDQjCq2/Vd/jaEClkmAIcxHNAipZa+J6HhDmFBtvdnZfBPRx20u3h3hDu4b2LYAQrp+1nAXKAcvKmt0VnmFPHcJBq6gF653WQCwjH2cg/ditGESDEQo+yWwtVj1IzTDNU7ROTGACQ6po6el3nqNon6ucBglGNp1p3+dQonXL1ulTlZXAQCMpJ1MM8e4G+CIMWntZ3mJWcQH64qqOrA7SFWOgpsxuSq5AAkJyOYxuQIYrGOxdBned0HCHKoXrihuvyFxAM8frX08JBKgCCHCSnwFxLaPP2g4J2J+lQvi4cux7seVYQeoaeJKKqNCqzZb4l7nGG8Kq6gyDE8sBF+K65U1QlQiwd6jmQiyBSACBoYDlCaFWyjABIgwQO5w8HgRzrgTn/gIMAEL0hlsV5COAAIGhoOcLj9ABIK7Juko3DK8yeAxCEWRl6h2oDIG3Kmsk2dg8sLQEgrSrz0V0GaiKwUqKKNgCkuXo2hC1YWlJLEQBRlKxbkIu8g3uoCbFiFEktFzG2d2Z44R4ApNv4ftfjuwzRJaoHOYgRDdG0hF2eD4VWQ1RNLd3CQdSKQpkLg+AYCPfugOw8xLpDkTQOtSYGwEFOdoXqaKSdo1jYyLi5LrrcZI7heC+wIZyWHCRCuTTWQwPtcOiXwircMajJQZCDqIPkqu2kXf49GrGaoPibK3ksRLj1QwCiToO2nIRAlMd7wKHWPXY5CMIs9ZB80JmTMIAExxDFrUxxHiBwET05yUQDHHRvxwfkHMp1mwfILcqntjY5kNBEopK8hFyDvks8DuVijVXLIdYa5VMbjkN57OeAQj3+J9rVsA4onGucsWvk3Rm4EBiyVwJIsKsS5Mt/UUbV4fgj+jXiMhxw794v+Aw15GXyuYJQ6m2JJJy+81h+34rP4RLhV/W6lOX3KhMQrpBPAhNNteDY6miuSibPMfda6fD2JTfussk3fX6cHonkc7gUuA+9ilayDMdFgGA8vZzW3GPHOb0/hUS6l5ufy3M4yzmHIZ/DEFVWrSyzVvPeoJxKhTKHRXNHXNh7mnI7+s69PDj4HOh91Cueo+pKlakocpABJ4LQUzDm8pglM60Vk2xVPfmKzoMbftVz6PM5IELY3ZkEhYAgD1ELRkYHdMS5QdkyphxjyTFyrOAcElDoHDBUzO5BUUFZQJCHPCbPS1Vg5MAyYFC+59dNKmEnl4h0/X0+B6rnt0jmxVSW86wsIBPh7+2a1Chp+HXh00Wndl488jSh398ejQwKCsun+ZA4FdvHwnNxCDZhWHwItWNZ73vbPwwKCsn1RXAbhuKaJtcQgudGE667ykK2gePtH/6t4EPXDhYKoKgoDjUXnC+dOJqbXu/6YZGDkLV+cqQAVpxXAAp1ucqJcGMpyzfLS0oDwoVh+3LqFY9OxGjaWmChCMP2Wfqd4RWpzL5Yc4uTbprpHgMOreFXMncwFfauIF5m/aIMIDaGJHTO+3VmmqHaoND8AS31t+2O1DivnYQlLjxZlm2TXY51TqxBmW3lwbUt61SXeb8su/XotS3OkRVLQq1B8rCQ0yInWTQGhEd+TI/jk4qBzIHEhg41VuEgNiTr5wirjIIksiA0Xxa9oQogC2HuKEW8vcgMMkJTw9vMShkg3DubmnzhRiBzQ62FzW0mdKAhxr6turVMJobmpTv7sGKPEBvYIyzRBo12ERPbzLxsvlrnCVOmuQjcw3yZ1IkRGKXz1dDyHmGFZSRWuMhamDNNMK8y2ln3GYWmuMg1mp81MmGAp5J71AbEEBfZIDlHmKXTPZo4iAkuskabsyrMijoOs+Kq7tEIEHaRLiFBeIUwq1KHXmelRdPnpM9EdzOluDPQPnXVqUV1w/FGgDCR044uGOuu7AuzugqLa7fRUMFFLzrIB5B/IMwqq0UTMMOuCa0pbK5tr9qsu8YRjhJAeISizYQdDmKv2ryR6rhpKB6oPJuWdkCh/GMf7cxeyXbyvzZCufSDcLoOsb4QC/eADKhDZXc0KgWkpVALT+FFmKU9tNLlIMkTlSKLCxfSL52d3ELl7pmhppMcC00TiEVPhIW8dpBYKB5RDTU14lhTPoL8wwFp7OSU74cWaiwEsrmZhh4CQqKelXcoBy/UWQLyhKeKC+IO7coZqezsFrpufQhbKIixwsJAiOWOVHV2kc7dNLUDwjGhqqQdCxQRYm270KHOk2zDQZKk7FjR90BuaKPg89o3KQ/bKg1O2ptAAjgckoLObtxGhxm2XCiUSNWdaUd4hUQ90XFb95aEbZcIz7TXGXGAgwCQBI5FWycYdlEqPOpQ9SJ/R3vyHpDjtneyCbsqmRqQwEHc053JcHQKSA1IkIO4p43JcHQOSEVIAIh7ikyGwwhAUpDMCt6DEMs/HXe9e2ZoSknwuq3MeZLvBj9N0F6c01FOtDA2YWvZwLQSYxAu5NHb8WsqsCn2xLJbso6pbq/kMcyA49CUiCEwtABp44f3GZBEQtPSZqiVuiUoLuXRz6jbsUmPtAhNLERu/HsZSdwDPAi5rITjjDu+XXCs2Dlik845MLxAexxuZcGwEgpv0Ie01WOfXWOY8ZZzXmFhnAJLCjgvL9kwJNjM2sy6eydfTnPqbtzhnr1uAJLKSy5F9sZ0K07gYzRLY+rrIsc11tyxGV1fz2wp8M/3H++fv37zL/nPF/L4ccdb/k6hmHzPX/K9v6GJdhcWyzr4Wf7zl4xcIwmpjmU9GR8aB5ZWwojdpJfxlojdZI0m23oofJoDhnUjkIHFldFjSEY5b7PCxh0AY8hgDHPeZmwi7iQgW5VzmdNrkRZcQQBFbdn3Rf7olJWu4RQgKTdJRksEQGkFDCrrSc7bNlzWM5uvNXCw4i4Kwi6AojeUIs1EzYdmAhCzKpJylDnmUEol3yei+NkvzuV8geMVO2JH6Re8lSqUHnS/gKt848YnHEb1SoBx7uKoYeBJZU9E/vBjWuQm9LjilW9LWDiXG5V0C6fB8AqQGqFXkmQSLDcuw5KC4m2J3C3dicx9mGfyCpBUoxikwgdRoVEksMQOXD91Ekei/DMlkw7Dq8ENLwHZ6j2TBLRf4aMxhxcETGT6GH8KiAN+7VX4OF3b3MeQ03tAdoRfRxxm9Cp+fMMN6YZf466g4esg2H9gdxjW+JqY3WLp+41pAGR3I0vH5L0GXxWl4Pk99X9RJ35nx0tCoj4fL/ln/YoumBVCXWPYG4BUheWAYelr/nOx+Lrb4KAhnGUBXsMpAIgqWPpbsXzfskuIUqHgCndiApA2gBnwcdBSr1/FjQiGW3aJCEAAEBOg6aWg6TE4ukKmTSqvuU1CNNwHA0Bsh2i49aM8eBIIvggAQBAEQRAEQRbr/wIMAB2nwEL3kwxHAAAAAElFTkSuQmCC" }</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to update media with invalid media ID for profile context by Entity ID using base64 API and check the error status</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to update media with invalid Entity ID for profile context using base64 API and check the error status</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to update media with invalid media ID for profile context using base64 API and check the error status</t>
+  </si>
+  <si>
+    <t>OPQA-SS01</t>
+  </si>
+  <si>
+    <t>Verify that user is able to create media for profile context using Streaming API</t>
+  </si>
+  <si>
+    <t>/internal/media</t>
+  </si>
+  <si>
+    <t>Cache-Control=no-cache||Content-Type=multipart/form-data; boundary=----WebKitFormBoundary7MA4YWxkTrZu0gW</t>
+  </si>
+  <si>
+    <t>src/test/resources/media/LinkedIn.png</t>
+  </si>
+  <si>
+    <t>status=201||entityId=(SYS_USER1)||entityType=profile||mediaType=image/png||context=1p-profile</t>
+  </si>
+  <si>
+    <t>OPQA-SS02</t>
+  </si>
+  <si>
+    <t>Verify that user is able to update his own media for profile context by media ID using Streaming API</t>
+  </si>
+  <si>
+    <t>/internal/media/(OPQA-SS01_mediaId)</t>
+  </si>
+  <si>
+    <t>src/test/resources/media/kPl0TGN.jpg</t>
+  </si>
+  <si>
+    <t>status=200||mediaId=(OPQA-SS01_mediaId)||entityId=(SYS_USER1)||entityType=profile||mediaType=image/jpeg||context=1p-profile</t>
+  </si>
+  <si>
+    <t>OPQA-SS03</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to update media with invalid media ID for profile context using Streaming API and check the error status</t>
+  </si>
+  <si>
+    <t>/internal/media/0f28b7f1-2bee-4178-ad9f-3d5e68d167</t>
+  </si>
+  <si>
+    <t>OPQA-SS04</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to update media with invalid Entity ID for profile context using Streaming API and check the error status</t>
+  </si>
+  <si>
+    <t>/internal/media/1p-profile/profile/(SYS_USER1)A</t>
+  </si>
+  <si>
+    <t>OPQA-SS05</t>
+  </si>
+  <si>
+    <t>Verify that user is able to update his own media for profile context by Entity ID using Streaming API</t>
+  </si>
+  <si>
+    <t>/internal/media/1p-profile/profile/(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>src/test/resources/media/8mb-artwork.jpg</t>
+  </si>
+  <si>
+    <t>OPQA-AA17_1</t>
   </si>
 </sst>
 </file>
@@ -673,15 +742,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="H17" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="53.140625" style="5" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="49.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -806,7 +875,7 @@
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
@@ -816,13 +885,13 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="6" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>19</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -831,13 +900,13 @@
         <v>33</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>11</v>
@@ -847,11 +916,11 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="K5" s="1"/>
     </row>
@@ -860,7 +929,7 @@
         <v>36</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
@@ -876,26 +945,26 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="240">
       <c r="A7" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>11</v>
@@ -911,13 +980,13 @@
         <v>19</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="K7" s="8"/>
     </row>
     <row r="8" spans="1:12" ht="240">
       <c r="A8" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>34</v>
@@ -926,7 +995,7 @@
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>11</v>
@@ -936,28 +1005,28 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="6" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>25</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:12" ht="240">
       <c r="A9" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>11</v>
@@ -967,28 +1036,28 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="6" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>25</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="31.5">
       <c r="A10" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>0</v>
@@ -1005,16 +1074,16 @@
     </row>
     <row r="11" spans="1:12" ht="47.25">
       <c r="A11" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>59</v>
-      </c>
       <c r="C11" t="s">
         <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>0</v>
@@ -1032,16 +1101,16 @@
     </row>
     <row r="12" spans="1:12" ht="31.5">
       <c r="A12" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>0</v>
@@ -1049,7 +1118,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="4"/>
       <c r="I12" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>14</v>
@@ -1058,16 +1127,16 @@
     </row>
     <row r="13" spans="1:12" s="10" customFormat="1" ht="47.25">
       <c r="A13" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>0</v>
@@ -1076,7 +1145,7 @@
       <c r="G13"/>
       <c r="H13"/>
       <c r="I13" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>17</v>
@@ -1086,82 +1155,82 @@
     </row>
     <row r="14" spans="1:12" ht="47.25">
       <c r="A14" s="8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="47.25">
       <c r="A15" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
         <v>65</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" t="s">
-        <v>70</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="47.25">
       <c r="A16" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H16"/>
       <c r="I16" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>14</v>
@@ -1169,16 +1238,16 @@
     </row>
     <row r="17" spans="1:11" ht="31.5">
       <c r="A17" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
         <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>18</v>
@@ -1194,16 +1263,16 @@
     </row>
     <row r="18" spans="1:11" ht="31.5">
       <c r="A18" s="8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
         <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>18</v>
@@ -1219,16 +1288,16 @@
     </row>
     <row r="19" spans="1:11" ht="47.25">
       <c r="A19" s="8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>18</v>
@@ -1246,16 +1315,16 @@
     </row>
     <row r="20" spans="1:11" ht="47.25">
       <c r="A20" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
         <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>18</v>
@@ -1267,6 +1336,180 @@
       </c>
       <c r="J20" s="4" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="45">
+      <c r="A21" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="45">
+      <c r="A22" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="47.25">
+      <c r="A23" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="47.25">
+      <c r="A24" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="K24" s="8"/>
+    </row>
+    <row r="25" spans="1:11" ht="45">
+      <c r="A25" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" ht="31.5">
+      <c r="A26" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="5"/>
+      <c r="H26"/>
+      <c r="I26" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1280,7 +1523,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Created and updated Profile & Media test cases.
</commit_message>
<xml_diff>
--- a/src/test/test-data/MediaTestData.xlsx
+++ b/src/test/test-data/MediaTestData.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UC196992\Git\1p-api-automation\src\test\test-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="126">
   <si>
     <t>GET</t>
   </si>
@@ -74,9 +79,6 @@
     <t>DELETE</t>
   </si>
   <si>
-    <t>OPQA-AA01</t>
-  </si>
-  <si>
     <t>Verify that user is able to create media for profile context using base64 API</t>
   </si>
   <si>
@@ -92,9 +94,6 @@
     <t>mediaId</t>
   </si>
   <si>
-    <t>OPQA-AA02</t>
-  </si>
-  <si>
     <t>Verify that user is able to create media with custom path prefix for profile context using base64 API</t>
   </si>
   <si>
@@ -107,30 +106,15 @@
     <t>status=201||entityId=(SYS_USER1)||entityType=profile||mediaType=image/jpeg||context=1p-profile</t>
   </si>
   <si>
-    <t>OPQA-AA03</t>
-  </si>
-  <si>
-    <t>{ "mediaId": "(OPQA-AA01_mediaId)", "base64Media": "data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAASwAAAEsCAYAAAB5fY51AAAABHNCSVQICAgIfAhkiAAAGYBJREFUeJzt3XuYFOWB7/HvW9U9V5gBBhxwAMVwEURBohgMRt2V9YKa5OhuPErcs15iPBv0PDlnZXWfk8c8m82um2fd9RKT+CTGVUyyu8nZTQRW18RoCCExxmgCchdE7gxzg5np6e6q9/xRM3JxlLl1V709v8/zjD7M9HS/9Ex/qap+6y3DYHzm2SpqU0vwgrngTcPaGXhmEtYO6m5FpAQYA6F9B2M2QbiF0H+d1vxyHr+mY8B3OaDvumfV9Rh7J5h5WFtLKm2wIdGHYiUi3YwB40Uf+ZzFmFawr2HN1/j7q77f77vr162XrboGa+/FMwvwfAgDBUpE+s4Y3m1HaNdizN/ywFXP9vnb+/xAy1Y8h192OTaEMAQUKhEZKANe95ZXkH2eB66+oo/fdRJ/ueoWLF/GT9UT5AY9TBGR4/hpCPL7MdzH3131xAfd9IODtWzl/cC9eH4ZYTCEIxQROUa0m5gF/pYHFt//fjfz3/cOlq34Aqmy+7HWx4YFGKGISDdrwRifVPoSLvyUZc13Xu7tZr0Ha9nK+0mV3U8+j45ViUjRhBZS6Uu58AbDmu+8dOKX37tL+JerbsHar2FMmd4BFJGiMwaszWLMnSce0/Lec2PLl/F8xUpE4mEtUYP48olfOj5Yy1Y8h5+q1wF2EYlVGICfqmfZiueO/fTRYC1bdQ1+2eWauiAiiRDkwC+7nGWrrun51NFgWXuv3g0UkUSJTve7t+ePUbDuWXU9nlkQzWAXEUmIMATPLOCeVddDT7CMvRPPR1MYRCRZbDSp1Ng7AQyfebaK0f5uDKP0zqCIJI4xYGmhOWhIUZtagg1r4x6TiEivrAVLLbWpJR5eMJdUemDrYomIFEMqbfCCuV60UqgOtotIgtkQ8KZ5WDtDwRKRRIumN8zwtAa7iCSeteCZSZ5iJSJOsLaXk59FRBJKwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOCMV9wBiYYHQHv3obdVVzxz/ISKxGz7BCkLIW8iHkPY597RRXDapltnjqjhlRNlxzfIMbG3qZP3BDla83cI7u9sACykPfA98BUwkDqUdrLA7UBhuPGscl8wYx8IZ9cwcV33Sb728+/+Pdf//17taeWndHlZuauTlHS1R1VImuiqtiBSFYdnK0rsKhQWyAWefUs31cyZw8/zJNNRVkR6CuHTkArYdOMJjP3uL7755gNaOLKT9wY9ZRE6q9IKVC8EzPHzVDG6YP5lx1WUFe6hNB47w+Oq3eHD1jiha2lUUKajSCVZooTPP0oWn8VeLZ1E/onChOtGGA0e44zuvsXpHC5SnQN0SKYjSCFY+5JTqMpb/9zksOrM+liEEFh57aSt3Pbe556KPsYxDpJS5Pw8rF3LpxBrWfO7C2GIF0d7g0kun8svPXhC9kxi6/++ASNK4HayugKun17Fq6UKmjhsR92gAuGBKHTuXXUJFVbr7HUoRGSruBisXcPWZY3n2jgVU+Mn6a0waVcmW/3URM8dWK1oiQyhZr/S+yoV8csY4/u3WC+IeyfuaOKqS5z5zAQ21Fdo9FBki7gUrsMypq+SbS+ZRkUr28CePqeL52+ZDNojmhonIoCT7FX8iC1jLv95+AWOqijdtYTDOmlDDM0vmatdQZAi4FaxswLc+MYvpCTnA3lc3njeZz86bEG1piciAuROsIOTchhpuWXhG3CMZkHuvmgXVZb2vDCEifeJGsCzgeXztutlxj2TAJo+u5FtXTIcubWWJDJQbwcqH3H52PRdMqYt7JINyy0enwMhyvWsoMkBuBItoFnkp+PYV06PzeESk35IfrCDk41PHMGNCTdwjGRKLzp5AQ3Vax7JEBiD5wcqF3PiRyZSVyMnEDTUVXHNWfbT6qYj0S/KDFcJVs0+NexRDasmHG7RbKDIAyQ5WYDl/6hhGpJM9zP6aWl/DpLFVOvgu0k/JLkE+5H/OnRD3KIZc/chyrplUo2CJ9FOyg5XymDJ+ZNyjKIgppypYIv2V3GBZqC73GVtTGfdICuKM+pEKlkg/JTdYWCaW+4yvLc1gTT9FwRLpr+QGy8L48hR1laV56cRZ9SP0TqFIPyU3WJT4ElIl/ZcTKYxEB0tE5FgKlog4Q8ESEWckOli2hA/0hNbqCtEi/ZTcYBk42BXQ1JmPeyQFsfFgu64OLdJPyQ0Whm2ZgF0tHXEPpCDe3NemYIn0U3KDZSCXDWhqy8Q9koJ4e/9hBUukn5IbLIB8yNa9bXGPoiDe2qstLJH+Snaw0h7/9NqeuEcx5Pa2Zfj+zjbwFSyR/kh2sDzD+u3NtGRK68D7pr1tNDZ1gFGwRPoj2cEC8A0rf19aW1nLf7MLUsl/6kWSJvmvmrTPd3/9Dl1BaVzq/Z3WDCs3HtTuoMgAJD9YvmHllibW7W6NeyRDYuXru9nXntPuoMgAJD9YAL7h4Re3xj2KQQuBO5/fDCnFSmQgHAmWx1NvHmDttsa4RzIo3/zZNujQ1pXIQLkRLANYuOFf3nD27MJtje3csWozlJfmgoQixeBGsAB8w87GDh75yea4R9JvIfDFZ9dDLtAJzyKD4E6wANI+d6/azO/2uDX7/clfbOfpdQegxK6vKFJsbr2CDOAbrvvmrzh4pCvu0fTJb99p5tbv/U7zrkSGgHuvIs+wta2LTz3xCm1dyZ4Bv2n/YeY9/gpUpLQrKDIE3AsWQMrjp2+3cu3jv6QroVee2bT/MJd/8xXI5HSSs8gQcTNYAGmPl7c3s/jrv6Ajl6xZ8G8daufMr/6Ct1s6wXf3KRZJGrdfTWU+P9nezPyv/JTf70nGTPgXN+7nQ3/zImTyipXIEHP/FZXyWN/cyfyvruX7r+2K7WLK7dmAv171Jn/4xKvRu4HaDRQZcu4HC8D3yOQD/vjJ17h9+avsai3uKqW/3d3KJQ+t5gsvbItmsWsmu0hBGJatTOZR64HKh9AV8MUrpnHrRWfQUFNRsId6fVcrD/10K0+u3QkjyrRVJVJgpResHtmAhppyrjurntsWnMbU8TVUDsFcqObOHBv2tPLgT7fxg7eaIBtojpVIkZRusACsjba4rOHaqaNZOHUsF59Zz/zJo7D0bWqUBXJByItbGln95j5eeKuJX+8+HK1n5XuaXyVSRKUdrGMFFoIwCljKZ3ZDDRc3jGRmXRVjq9LHnVTtGdjenGFjUwfP7Wpj394jUZhSXhQq7fqJxGL4LB3gG/B9KPPBwrr9h1m3tw1CS69LQHhEB889A1XD52kSSbLh+Uo0HI2RiDhDR4tFxBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnDM9zCUWOZbv/Y0/480mZ45cXMr18ToaUgiXDiyVaJy3s/ggslKcYU5VmYkWK+ooUI9IedeWpD0yWATJByN6OPIG17O7MczAb0JLJQ2c+OrH+3Y/u71DIBk3BktIXdi/k6BlIe0yqLOPC00ZzXkMNH508iurKMqoq01SXpxhZkaYi5ZHqY1wOZwNCC22dWTK5gM6uPJnOHBsb21mzs4WNB9tZv+8wh3Ih5MIoln73umrSb24u4NeeI7bL4wxE2ouu/lworjwfnoHqdOEfxwJhCPloK+rDp49iyaxTmDl5NHMmjWb8iLLCj+EEGw62s3VvK5v3tPK9TY28+lbz8YtC6sIlfeJesNpztD5wJdUVaaxN/tBTvsfPN+zjom+8Uphotefo/IerSae8RD8fnjG0tHdRd9/zhYtWz5ZU2ufGqWNYMH0cN54/iTFVxQ/UybRm8vznm/tYs2E/j25shMNd3ZeH07LbH8S9XUJrSac8fM/gyk825Xt9O4Y7EKE7z0c6VaDnoTtUM8dUcu3Z4/nsR0+nYUw16QQv0FhbkeKGeRO5Yd5ElrV08uqOJr6+ZgfPv9Ma7Tqm9QZ+b9wLFtFhAKcUeMDRllVyX5w9hvxpCC10BYyoq+LbV05n0TmnUlvu3q/0xFGVTJzbwCfmNvD6rha+tWYHj659JzpYn/Zd+NEWjXs/XRFrIRNwTsNI/u+i6Vx/bkPcIxoycyeO4pFPzeW+q2by2Itb+NKandHFU3QpOUATR8U1+ZDKlM/Xr5vN6rsuKqlYHWvCyHL++uOzefPzF3HjzHHdl6tzbddi6ClY4gZrIZPnkzPG8cbdC7njY2dQU8h3XhNi5viRLL/1An5w07kQEoVrGCv9n7i4LwgBw/f/dB7XnTsx7tEUnQH+27kN7J9+Cku/+xr/um4/lKeG5bEtbWFJsuVCPjZhJBv+4uJhGatjnVKd5ju3XsDDH5/ZfT3N4beLqC0sSa5swJ/NncA//slcaofB7l9f+AaWXjqNMSPKWfJvv4+ileDpG0NNW1iSPBY4kuWLi6bxxM3nKVa9uOn8yfzktvnRDHkXznIYIgqWJIuNJoE+fsMcvnDlmXGPJtH+YPo41t75kWhC7jCJloIlyWGBwPL4J2Zx+8IpcY/GCR85fQw/XHJu97SHuEdTeAqWJEd7NorVRWfEPRKnXDlrPP909ZmQDeIeSsEpWJIMXQEPXT+b2xcqVgNx9x9M4/9cOBky+biHUlAKlsQvG3DPx07nrkumxj0Sp9139SwuOWN097y10qRgSbxyIdfNGMuXPj477pE4b3RlmkeunxOtolqix7MULIlPaKkZUcY3Pn1eopeCccnsU2v48uXTIV+ax7MULImHBfIhP771fOqqirAK6TDyvxdN54zRlSU51UHBknjkQ7502VTOnzw67pGUnDLP8NC1sxQskSGRD7n4tFruuXJm3CMpWYvOmsBlk2uj41klRMGS4rIWPI9Hrp9DWoetCqbcN9x7xZnQVVrHshQsKa6ugK8s+hBnn1oT90hK3sIPjeWPZtSV1FaWgiVFY62F6jLu+sPpcQ9lWCjzDbctOK2kFv1TsKRo8ha+e9McyjSFoWj+eN7EaLG/Elk7S8GSohldXc4n5w3vRfji8DcXnx5dOqwEKFhSNJ6Bcl39pegWnz2heysr7pEMnn57RErcnImjuGz8iJKYl6VgiQwD1849tSQOvitYIsPA4ln1JbH2u4IlMgzU1VSwYGKN87uFCpbIMFBbnmLx1DHOr5WlYIkME7OnjI0mwzlMwRIZJi6eOtb503QULJFhYlRFigmOH8dSsESGkZumjXF6K0vBEhlGFkwe7fR5hboGuJSU/e05Nuxr4+DhDB1dAYfbOghyAWAAi/E8RtRUUlNdxvT6Gs4ZPyLuIRfVuLpqSPvRaToOTstSsMRZ+9uzbNrdwtpth/h/W5t4ZVtTdPEF34tejMb0/qK0RFsZ3btGZ04Zzec/fCoXzqjnrPEji/lXKLrT66oZW+bRmO2JuFsULHFKZz5k055WHnxpG798u5ktbdlobpHvQYUP+P2+z417D/OZ/9iAqdrKtZNr+YvLpvHRD40d+sEnwKTaChoqUjR2BS72SsESd6xav4+vvbyNFVuawDfRqSa+Ab//kTpO933YfMgPtxzih5sP8fmPTOK+xbNK8oo+48dU80ZLBheLpYPukni/39vGxQ+tZvE3fsWK7c1Q7kPKG/pz4wzR/aY8Hly7k4a/e5GXtjYO7WMkwHmTa52d2qBgSWIFwKMvbuGcB1fzs3daoSod7foVmgHKfLoyeS59bC3/tWF/4R+ziM6pH+ns1AYFSxLrtuW/YemKjdFvaRwL/3kGUh6XP/kbXtx0oPiPXyDTx1Y5u5ifgiWJk8mH/NFjv+DJV3dDmR+92xcXz4C1XPf0a7zd1BHfOIZQZUUaKtxcgVTBkkTJhZZPPfEKL2w9FL2oksAztGTyXPvEK66fOwxARVmKsVVpXCyWgiWJ8lf/sY4fbWqMtqySJOXxuz2HeWL1trhHMmiVZSkmVWoLS2RQfrJxP195eXs8x6v6Iu1xx8pNHHb8asojK1JMqi5TsEQG6mB7lsuWvx5NWUjq9CBjIBvw0I83xT2SQalMeYyrcPNahQqWJMI//Ncm6Mgmf93xtMfXf7OHA4e74h7JoIwsT9gudx8pWBK7LQcO88Aru6KTcpPOM+xu6uClzW5Pc6iprdQWlshA/P0LmyGbT+6u4InSHk//amfcoxgUz/d0DEukv3Y0d/K9Nw8m90B7bzzDz/ceYfPB9rhHMmCT6tycPOrQb4mUopfX7+VIZy7eyaH9ZQwt7Vm27GqOeyQDVuZ72iUU6a/71+x0a+uqh2f49w0H4x7FgKWKcU5mAbg5aikJ25o62LGzJfnvDPbG9/jWG3vjHsWATR9b7eSKDQqWxOaljQeSN6O9rwzQnmVnaybukQyIg60CFCyJiQV++9ahaPE8V/keb+xujXsUA+JorxQsiUdTe5YVO1vd3B3s4Rt27WuLexQDMrG23MlqKVgSi86uHG8f6nA7WJ5hx8EjcY9iQEZVpvUuoUhfbdx/BPJh3MMYHGNY39RJp4N/DwdbBShYEpOf72h2+/gVgIE3mjrpyrm9eoNLFCyJxfYDR9zeHQQwhl1HsgSBe1tYrlKwJBatrZ1uzW7vjQEUrKJSsKTo2nMhjRmHTnb+IMawo7kz7lEMGwqWFF1rJkdTrkS2Sgx0ZHUMq1gULCm6I115mnJuXir9PTzDxgNuTm1wkYIlRdfZlWd/LqQ0igWBq3MEHKRgSdFlsoH7c7B6GOjULmHRKFhSdK6/OXgcY9ilg+5Fo2CJDFJJBTjhFCyJh17kMgAKlhRdPhdA3ipa0m8KlhRdrisHOv9OBkDBkuIzRltXMiAKlsggBa6uN+wgBUtkMDxoPuTu9Qldo2CJDIr2bYtJwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZTgbLM3GPoH+MKeyAC33/Q82t0ZYm115DPVJxD6DfjKE9kwcgtDGPpQ9SvkdnNl+4V6lnaM/kSKc8rCvPRy4AxyL7QQJrsdbSmQ3iHkqfeIboNeTgz8CwbKUDv+YnaM/hxKuzR8qDigL+2+Da85H2odyPexRDJ7DQmYt7FP1jDFSn4x5Fv7m3hQVOPtEFpecjXr6BEWVxj2JYcPIYlogMTwqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGR5CPewwiIicX5PHIZZxcKlVEhhFjIJfBI5eNeygiIieXy+KR63JrPXARGX6shVwXHl2dELpxtQ8RGabCALo68bAhZNp1HEtEksmYqFE2xMN40NGm3UIRSSZro0YZDw/IkM1qK0tEkqdn6yqbBch4YDfjGWg7pK0sEUkWa6M2eQawmz0w2zAe5HPQ3qKtLBFJBmOiJuVzYDzAbPOAXRgTfbHtEOSyipaIxMuYqEVth3i3T7DLA/sjgnwGDFigeV/3NAdFS0TiYKIGNe+LmoQhapT9UVSlmx/dg2EC1kb7jOWVUDcBRUtEis/Cob3Q1Xl068qyl6c+d2q0WoO1P8Tzo9saE92wab92DUWkuIyJ2tMTKwDPjxrFu8vLeM8Q5DvevYExkDkCjbshDBUuESksY6LWNO6O2nNsi4J8B3jPQE+wnv7zn4NdhfGPuQMvqlzjLsh0dB+lFxEZYsaLGtO4q3vL6pjWGB+wq6JGHbuAX87eR5jnuONWxkRvKTbthbaD0fEtbW2JyFAwpnue1cGoMfncCX0xEOajNnU7ukm17rkm5lx1Cp5//nETSHvuoKszmnEKUFbZ/XnFS0T6wxxtR3sLtBw4epbNiRtD0bGrx3jmrqeP+e4T3PzIOjz/rPddwaFnK2vEKCivgnR5dMfYo18XEYFjItQ9VSHXBV0dcKTlg/fYPB/CYD1PLZ197KdT730A727C4HsYbyw2fP8BHG6OHtRPRdEqK4dUefRnERGAIA/5Lsh2RbEK8kdD9X6xMh6EQSPGu/s9X+r1Gz798P8A7wk8TJ+2mN69jX13Q0tEJCrMMe/4nfT2BkIshLfw9F1P9np3vbr50U9i7Q/wPNPrlpaIyFAyHoShxZjreOpz/97bTfzePgnAG6s2cvaV+4AL8f1KHZsSkYLxfAjDJkL7eZYvXf5+Nzv5NtqSRxfh2W/g+VMIQ7TPJyJDx4DnQRhsJzR3sPxzL5zk1n108yNPA0u6S4jCJSID926oAJbz1NJP9+W7+j59/amln8YL5hMGPwYb4KU0iVRE+scY8FKADQiDH+MF8/saKxjozM8/fXgxofkzDJcAo/BTfrTSQ6h5WCJylDHRwfTonMAAaMHyEp79Nv9818p+392gB7TkqzfhhwuwdhqW0/C8GYqWiHSf0LwJw9sYs4XAW8vyP39mMHf5/wE/pJZJKs/o/AAAAABJRU5ErkJggg==" }</t>
-  </si>
-  <si>
     <t>Verify that user is able to update his own media for profile context by media ID using base64 API</t>
   </si>
   <si>
-    <t>OPQA-AA04</t>
-  </si>
-  <si>
     <t>Verify that user is able to update his own media for profile context by Entity ID using base64 API</t>
   </si>
   <si>
     <t>/internal/media/1p-profile/profile/(SYS_USER1)/base64</t>
   </si>
   <si>
-    <t>OPQA-AA05</t>
-  </si>
-  <si>
-    <t>/internal/media/(OPQA-AA01_mediaId)/base64</t>
-  </si>
-  <si>
     <t>/internal/media/0f28b7f1-2bee-4178-ad9f-3d5e68d167/base64</t>
   </si>
   <si>
@@ -140,39 +124,12 @@
     <t>/internal/media/1p-profile/profile/(SYS_USER2)/base64</t>
   </si>
   <si>
-    <t>OPQA-AA06</t>
-  </si>
-  <si>
-    <t>OPQA-AA07</t>
-  </si>
-  <si>
-    <t>status=200||mediaId=(OPQA-AA02_mediaId)||entityId=(SYS_USER2)||entityType=profile||mediaType=image/png||context=1p-profile</t>
-  </si>
-  <si>
     <t>Verify that user is able to update his own media with custom pathPrefix for profile context by Entity ID using base64 API</t>
   </si>
   <si>
     <t>/internal/media/1p-profile/profile/(SYS_USER1)A/base64</t>
   </si>
   <si>
-    <t>OPQA-AA08</t>
-  </si>
-  <si>
-    <t>OPQA-AA09</t>
-  </si>
-  <si>
-    <t>/media/(OPQA-AA01_mediaId)</t>
-  </si>
-  <si>
-    <t>OPQA-AA10</t>
-  </si>
-  <si>
-    <t>/media/(OPQA-AA01_mediaId)A</t>
-  </si>
-  <si>
-    <t>OPQA-AA11</t>
-  </si>
-  <si>
     <t>Verify that for the given valid Entity ID, media is retunred by using GET Media by Entity ID/Type API</t>
   </si>
   <si>
@@ -185,66 +142,30 @@
     <t>/media/1p-profile/profile/(SYS_USER2)</t>
   </si>
   <si>
-    <t>OPQA-AA12</t>
-  </si>
-  <si>
-    <t>Verify that for the given invalid Entity ID, media is not retunred and error thrown by using GET Media by Entity ID/Type API</t>
-  </si>
-  <si>
-    <t>OPQA-AA13</t>
-  </si>
-  <si>
     <t>Verify that for the given valid Entity ID, filters with isRedirect for getting media is working as expected using GET Media by Entity ID/Type API</t>
   </si>
   <si>
-    <t>OPQA-AA14</t>
-  </si>
-  <si>
     <t>Verify that for the given valid Media ID, filters with isRedirect for getting media is working as expected using GET Media by Media ID API</t>
   </si>
   <si>
-    <t>OPQA-AA15</t>
-  </si>
-  <si>
     <t>Verify that for the given valid Media ID, filters with height &amp; width for getting media is working as expected using GET Media by Media ID API</t>
   </si>
   <si>
     <t>?width=200&amp;height=300</t>
   </si>
   <si>
-    <t>/media/(OPQA-AA02_mediaId)</t>
-  </si>
-  <si>
     <t>?isRedirect=false</t>
   </si>
   <si>
-    <t>OPQA-AA16</t>
-  </si>
-  <si>
-    <t>/internal/media/(OPQA-AA01_mediaId)</t>
-  </si>
-  <si>
-    <t>OPQA-AA17</t>
-  </si>
-  <si>
     <t>Verify that user is able to delete his own media by using Delete Media by Media ID API</t>
   </si>
   <si>
     <t>/internal/media/1p-profile/profile/(SYS_USER2)</t>
   </si>
   <si>
-    <t>OPQA-AA18</t>
-  </si>
-  <si>
     <t>Verify that for the given invalid Media ID, media is not able to delete and error thrown by using Delete Media by Media ID API</t>
   </si>
   <si>
-    <t>/internal/media/(OPQA-AA01_mediaId)A</t>
-  </si>
-  <si>
-    <t>OPQA-AA19</t>
-  </si>
-  <si>
     <t>Verify that user can't delete the deleted media again and error thrown by using Delete Media by Entity ID/Type API</t>
   </si>
   <si>
@@ -257,18 +178,6 @@
     <t>/media/1p-profile/profile/(SYS_USER2)A</t>
   </si>
   <si>
-    <t>{ "mediaId": "(OPQA-AA01_mediaId)", "mediaType" : "image/png", "base64Media": "data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAASwAAAEsCAYAAAB5fY51AAAABHNCSVQICAgIfAhkiAAAGYBJREFUeJzt3XuYFOWB7/HvW9U9V5gBBhxwAMVwEURBohgMRt2V9YKa5OhuPErcs15iPBv0PDlnZXWfk8c8m82um2fd9RKT+CTGVUyyu8nZTQRW18RoCCExxmgCchdE7gxzg5np6e6q9/xRM3JxlLl1V709v8/zjD7M9HS/9Ex/qap+6y3DYHzm2SpqU0vwgrngTcPaGXhmEtYO6m5FpAQYA6F9B2M2QbiF0H+d1vxyHr+mY8B3OaDvumfV9Rh7J5h5WFtLKm2wIdGHYiUi3YwB40Uf+ZzFmFawr2HN1/j7q77f77vr162XrboGa+/FMwvwfAgDBUpE+s4Y3m1HaNdizN/ywFXP9vnb+/xAy1Y8h192OTaEMAQUKhEZKANe95ZXkH2eB66+oo/fdRJ/ueoWLF/GT9UT5AY9TBGR4/hpCPL7MdzH3131xAfd9IODtWzl/cC9eH4ZYTCEIxQROUa0m5gF/pYHFt//fjfz3/cOlq34Aqmy+7HWx4YFGKGISDdrwRifVPoSLvyUZc13Xu7tZr0Ha9nK+0mV3U8+j45ViUjRhBZS6Uu58AbDmu+8dOKX37tL+JerbsHar2FMmd4BFJGiMwaszWLMnSce0/Lec2PLl/F8xUpE4mEtUYP48olfOj5Yy1Y8h5+q1wF2EYlVGICfqmfZiueO/fTRYC1bdQ1+2eWauiAiiRDkwC+7nGWrrun51NFgWXuv3g0UkUSJTve7t+ePUbDuWXU9nlkQzWAXEUmIMATPLOCeVddDT7CMvRPPR1MYRCRZbDSp1Ng7AQyfebaK0f5uDKP0zqCIJI4xYGmhOWhIUZtagg1r4x6TiEivrAVLLbWpJR5eMJdUemDrYomIFEMqbfCCuV60UqgOtotIgtkQ8KZ5WDtDwRKRRIumN8zwtAa7iCSeteCZSZ5iJSJOsLaXk59FRBJKwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOCMV9wBiYYHQHv3obdVVzxz/ISKxGz7BCkLIW8iHkPY597RRXDapltnjqjhlRNlxzfIMbG3qZP3BDla83cI7u9sACykPfA98BUwkDqUdrLA7UBhuPGscl8wYx8IZ9cwcV33Sb728+/+Pdf//17taeWndHlZuauTlHS1R1VImuiqtiBSFYdnK0rsKhQWyAWefUs31cyZw8/zJNNRVkR6CuHTkArYdOMJjP3uL7755gNaOLKT9wY9ZRE6q9IKVC8EzPHzVDG6YP5lx1WUFe6hNB47w+Oq3eHD1jiha2lUUKajSCVZooTPP0oWn8VeLZ1E/onChOtGGA0e44zuvsXpHC5SnQN0SKYjSCFY+5JTqMpb/9zksOrM+liEEFh57aSt3Pbe556KPsYxDpJS5Pw8rF3LpxBrWfO7C2GIF0d7g0kun8svPXhC9kxi6/++ASNK4HayugKun17Fq6UKmjhsR92gAuGBKHTuXXUJFVbr7HUoRGSruBisXcPWZY3n2jgVU+Mn6a0waVcmW/3URM8dWK1oiQyhZr/S+yoV8csY4/u3WC+IeyfuaOKqS5z5zAQ21Fdo9FBki7gUrsMypq+SbS+ZRkUr28CePqeL52+ZDNojmhonIoCT7FX8iC1jLv95+AWOqijdtYTDOmlDDM0vmatdQZAi4FaxswLc+MYvpCTnA3lc3njeZz86bEG1piciAuROsIOTchhpuWXhG3CMZkHuvmgXVZb2vDCEifeJGsCzgeXztutlxj2TAJo+u5FtXTIcubWWJDJQbwcqH3H52PRdMqYt7JINyy0enwMhyvWsoMkBuBItoFnkp+PYV06PzeESk35IfrCDk41PHMGNCTdwjGRKLzp5AQ3Vax7JEBiD5wcqF3PiRyZSVyMnEDTUVXHNWfbT6qYj0S/KDFcJVs0+NexRDasmHG7RbKDIAyQ5WYDl/6hhGpJM9zP6aWl/DpLFVOvgu0k/JLkE+5H/OnRD3KIZc/chyrplUo2CJ9FOyg5XymDJ+ZNyjKIgppypYIv2V3GBZqC73GVtTGfdICuKM+pEKlkg/JTdYWCaW+4yvLc1gTT9FwRLpr+QGy8L48hR1laV56cRZ9SP0TqFIPyU3WJT4ElIl/ZcTKYxEB0tE5FgKlog4Q8ESEWckOli2hA/0hNbqCtEi/ZTcYBk42BXQ1JmPeyQFsfFgu64OLdJPyQ0Whm2ZgF0tHXEPpCDe3NemYIn0U3KDZSCXDWhqy8Q9koJ4e/9hBUukn5IbLIB8yNa9bXGPoiDe2qstLJH+Snaw0h7/9NqeuEcx5Pa2Zfj+zjbwFSyR/kh2sDzD+u3NtGRK68D7pr1tNDZ1gFGwRPoj2cEC8A0rf19aW1nLf7MLUsl/6kWSJvmvmrTPd3/9Dl1BaVzq/Z3WDCs3HtTuoMgAJD9YvmHllibW7W6NeyRDYuXru9nXntPuoMgAJD9YAL7h4Re3xj2KQQuBO5/fDCnFSmQgHAmWx1NvHmDttsa4RzIo3/zZNujQ1pXIQLkRLANYuOFf3nD27MJtje3csWozlJfmgoQixeBGsAB8w87GDh75yea4R9JvIfDFZ9dDLtAJzyKD4E6wANI+d6/azO/2uDX7/clfbOfpdQegxK6vKFJsbr2CDOAbrvvmrzh4pCvu0fTJb99p5tbv/U7zrkSGgHuvIs+wta2LTz3xCm1dyZ4Bv2n/YeY9/gpUpLQrKDIE3AsWQMrjp2+3cu3jv6QroVee2bT/MJd/8xXI5HSSs8gQcTNYAGmPl7c3s/jrv6Ajl6xZ8G8daufMr/6Ct1s6wXf3KRZJGrdfTWU+P9nezPyv/JTf70nGTPgXN+7nQ3/zImTyipXIEHP/FZXyWN/cyfyvruX7r+2K7WLK7dmAv171Jn/4xKvRu4HaDRQZcu4HC8D3yOQD/vjJ17h9+avsai3uKqW/3d3KJQ+t5gsvbItmsWsmu0hBGJatTOZR64HKh9AV8MUrpnHrRWfQUFNRsId6fVcrD/10K0+u3QkjyrRVJVJgpResHtmAhppyrjurntsWnMbU8TVUDsFcqObOHBv2tPLgT7fxg7eaIBtojpVIkZRusACsjba4rOHaqaNZOHUsF59Zz/zJo7D0bWqUBXJByItbGln95j5eeKuJX+8+HK1n5XuaXyVSRKUdrGMFFoIwCljKZ3ZDDRc3jGRmXRVjq9LHnVTtGdjenGFjUwfP7Wpj394jUZhSXhQq7fqJxGL4LB3gG/B9KPPBwrr9h1m3tw1CS69LQHhEB889A1XD52kSSbLh+Uo0HI2RiDhDR4tFxBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnDM9zCUWOZbv/Y0/480mZ45cXMr18ToaUgiXDiyVaJy3s/ggslKcYU5VmYkWK+ooUI9IedeWpD0yWATJByN6OPIG17O7MczAb0JLJQ2c+OrH+3Y/u71DIBk3BktIXdi/k6BlIe0yqLOPC00ZzXkMNH508iurKMqoq01SXpxhZkaYi5ZHqY1wOZwNCC22dWTK5gM6uPJnOHBsb21mzs4WNB9tZv+8wh3Ih5MIoln73umrSb24u4NeeI7bL4wxE2ouu/lworjwfnoHqdOEfxwJhCPloK+rDp49iyaxTmDl5NHMmjWb8iLLCj+EEGw62s3VvK5v3tPK9TY28+lbz8YtC6sIlfeJesNpztD5wJdUVaaxN/tBTvsfPN+zjom+8Uphotefo/IerSae8RD8fnjG0tHdRd9/zhYtWz5ZU2ufGqWNYMH0cN54/iTFVxQ/UybRm8vznm/tYs2E/j25shMNd3ZeH07LbH8S9XUJrSac8fM/gyk825Xt9O4Y7EKE7z0c6VaDnoTtUM8dUcu3Z4/nsR0+nYUw16QQv0FhbkeKGeRO5Yd5ElrV08uqOJr6+ZgfPv9Ma7Tqm9QZ+b9wLFtFhAKcUeMDRllVyX5w9hvxpCC10BYyoq+LbV05n0TmnUlvu3q/0xFGVTJzbwCfmNvD6rha+tWYHj659JzpYn/Zd+NEWjXs/XRFrIRNwTsNI/u+i6Vx/bkPcIxoycyeO4pFPzeW+q2by2Itb+NKandHFU3QpOUATR8U1+ZDKlM/Xr5vN6rsuKqlYHWvCyHL++uOzefPzF3HjzHHdl6tzbddi6ClY4gZrIZPnkzPG8cbdC7njY2dQU8h3XhNi5viRLL/1An5w07kQEoVrGCv9n7i4LwgBw/f/dB7XnTsx7tEUnQH+27kN7J9+Cku/+xr/um4/lKeG5bEtbWFJsuVCPjZhJBv+4uJhGatjnVKd5ju3XsDDH5/ZfT3N4beLqC0sSa5swJ/NncA//slcaofB7l9f+AaWXjqNMSPKWfJvv4+ileDpG0NNW1iSPBY4kuWLi6bxxM3nKVa9uOn8yfzktvnRDHkXznIYIgqWJIuNJoE+fsMcvnDlmXGPJtH+YPo41t75kWhC7jCJloIlyWGBwPL4J2Zx+8IpcY/GCR85fQw/XHJu97SHuEdTeAqWJEd7NorVRWfEPRKnXDlrPP909ZmQDeIeSsEpWJIMXQEPXT+b2xcqVgNx9x9M4/9cOBky+biHUlAKlsQvG3DPx07nrkumxj0Sp9139SwuOWN097y10qRgSbxyIdfNGMuXPj477pE4b3RlmkeunxOtolqix7MULIlPaKkZUcY3Pn1eopeCccnsU2v48uXTIV+ax7MULImHBfIhP771fOqqirAK6TDyvxdN54zRlSU51UHBknjkQ7502VTOnzw67pGUnDLP8NC1sxQskSGRD7n4tFruuXJm3CMpWYvOmsBlk2uj41klRMGS4rIWPI9Hrp9DWoetCqbcN9x7xZnQVVrHshQsKa6ugK8s+hBnn1oT90hK3sIPjeWPZtSV1FaWgiVFY62F6jLu+sPpcQ9lWCjzDbctOK2kFv1TsKRo8ha+e9McyjSFoWj+eN7EaLG/Elk7S8GSohldXc4n5w3vRfji8DcXnx5dOqwEKFhSNJ6Bcl39pegWnz2heysr7pEMnn57RErcnImjuGz8iJKYl6VgiQwD1849tSQOvitYIsPA4ln1JbH2u4IlMgzU1VSwYGKN87uFCpbIMFBbnmLx1DHOr5WlYIkME7OnjI0mwzlMwRIZJi6eOtb503QULJFhYlRFigmOH8dSsESGkZumjXF6K0vBEhlGFkwe7fR5hboGuJSU/e05Nuxr4+DhDB1dAYfbOghyAWAAi/E8RtRUUlNdxvT6Gs4ZPyLuIRfVuLpqSPvRaToOTstSsMRZ+9uzbNrdwtpth/h/W5t4ZVtTdPEF34tejMb0/qK0RFsZ3btGZ04Zzec/fCoXzqjnrPEji/lXKLrT66oZW+bRmO2JuFsULHFKZz5k055WHnxpG798u5ktbdlobpHvQYUP+P2+z417D/OZ/9iAqdrKtZNr+YvLpvHRD40d+sEnwKTaChoqUjR2BS72SsESd6xav4+vvbyNFVuawDfRqSa+Ab//kTpO933YfMgPtxzih5sP8fmPTOK+xbNK8oo+48dU80ZLBheLpYPukni/39vGxQ+tZvE3fsWK7c1Q7kPKG/pz4wzR/aY8Hly7k4a/e5GXtjYO7WMkwHmTa52d2qBgSWIFwKMvbuGcB1fzs3daoSod7foVmgHKfLoyeS59bC3/tWF/4R+ziM6pH+ns1AYFSxLrtuW/YemKjdFvaRwL/3kGUh6XP/kbXtx0oPiPXyDTx1Y5u5ifgiWJk8mH/NFjv+DJV3dDmR+92xcXz4C1XPf0a7zd1BHfOIZQZUUaKtxcgVTBkkTJhZZPPfEKL2w9FL2oksAztGTyXPvEK66fOwxARVmKsVVpXCyWgiWJ8lf/sY4fbWqMtqySJOXxuz2HeWL1trhHMmiVZSkmVWoLS2RQfrJxP195eXs8x6v6Iu1xx8pNHHb8asojK1JMqi5TsEQG6mB7lsuWvx5NWUjq9CBjIBvw0I83xT2SQalMeYyrcPNahQqWJMI//Ncm6Mgmf93xtMfXf7OHA4e74h7JoIwsT9gudx8pWBK7LQcO88Aru6KTcpPOM+xu6uClzW5Pc6iprdQWlshA/P0LmyGbT+6u4InSHk//amfcoxgUz/d0DEukv3Y0d/K9Nw8m90B7bzzDz/ceYfPB9rhHMmCT6tycPOrQb4mUopfX7+VIZy7eyaH9ZQwt7Vm27GqOeyQDVuZ72iUU6a/71+x0a+uqh2f49w0H4x7FgKWKcU5mAbg5aikJ25o62LGzJfnvDPbG9/jWG3vjHsWATR9b7eSKDQqWxOaljQeSN6O9rwzQnmVnaybukQyIg60CFCyJiQV++9ahaPE8V/keb+xujXsUA+JorxQsiUdTe5YVO1vd3B3s4Rt27WuLexQDMrG23MlqKVgSi86uHG8f6nA7WJ5hx8EjcY9iQEZVpvUuoUhfbdx/BPJh3MMYHGNY39RJp4N/DwdbBShYEpOf72h2+/gVgIE3mjrpyrm9eoNLFCyJxfYDR9zeHQQwhl1HsgSBe1tYrlKwJBatrZ1uzW7vjQEUrKJSsKTo2nMhjRmHTnb+IMawo7kz7lEMGwqWFF1rJkdTrkS2Sgx0ZHUMq1gULCm6I115mnJuXir9PTzDxgNuTm1wkYIlRdfZlWd/LqQ0igWBq3MEHKRgSdFlsoH7c7B6GOjULmHRKFhSdK6/OXgcY9ilg+5Fo2CJDFJJBTjhFCyJh17kMgAKlhRdPhdA3ipa0m8KlhRdrisHOv9OBkDBkuIzRltXMiAKlsggBa6uN+wgBUtkMDxoPuTu9Qldo2CJDIr2bYtJwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZTgbLM3GPoH+MKeyAC33/Q82t0ZYm115DPVJxD6DfjKE9kwcgtDGPpQ9SvkdnNl+4V6lnaM/kSKc8rCvPRy4AxyL7QQJrsdbSmQ3iHkqfeIboNeTgz8CwbKUDv+YnaM/hxKuzR8qDigL+2+Da85H2odyPexRDJ7DQmYt7FP1jDFSn4x5Fv7m3hQVOPtEFpecjXr6BEWVxj2JYcPIYlogMTwqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGR5CPewwiIicX5PHIZZxcKlVEhhFjIJfBI5eNeygiIieXy+KR63JrPXARGX6shVwXHl2dELpxtQ8RGabCALo68bAhZNp1HEtEksmYqFE2xMN40NGm3UIRSSZro0YZDw/IkM1qK0tEkqdn6yqbBch4YDfjGWg7pK0sEUkWa6M2eQawmz0w2zAe5HPQ3qKtLBFJBmOiJuVzYDzAbPOAXRgTfbHtEOSyipaIxMuYqEVth3i3T7DLA/sjgnwGDFigeV/3NAdFS0TiYKIGNe+LmoQhapT9UVSlmx/dg2EC1kb7jOWVUDcBRUtEis/Cob3Q1Xl068qyl6c+d2q0WoO1P8Tzo9saE92wab92DUWkuIyJ2tMTKwDPjxrFu8vLeM8Q5DvevYExkDkCjbshDBUuESksY6LWNO6O2nNsi4J8B3jPQE+wnv7zn4NdhfGPuQMvqlzjLsh0dB+lFxEZYsaLGtO4q3vL6pjWGB+wq6JGHbuAX87eR5jnuONWxkRvKTbthbaD0fEtbW2JyFAwpnue1cGoMfncCX0xEOajNnU7ukm17rkm5lx1Cp5//nETSHvuoKszmnEKUFbZ/XnFS0T6wxxtR3sLtBw4epbNiRtD0bGrx3jmrqeP+e4T3PzIOjz/rPddwaFnK2vEKCivgnR5dMfYo18XEYFjItQ9VSHXBV0dcKTlg/fYPB/CYD1PLZ197KdT730A727C4HsYbyw2fP8BHG6OHtRPRdEqK4dUefRnERGAIA/5Lsh2RbEK8kdD9X6xMh6EQSPGu/s9X+r1Gz798P8A7wk8TJ+2mN69jX13Q0tEJCrMMe/4nfT2BkIshLfw9F1P9np3vbr50U9i7Q/wPNPrlpaIyFAyHoShxZjreOpz/97bTfzePgnAG6s2cvaV+4AL8f1KHZsSkYLxfAjDJkL7eZYvXf5+Nzv5NtqSRxfh2W/g+VMIQ7TPJyJDx4DnQRhsJzR3sPxzL5zk1n108yNPA0u6S4jCJSID926oAJbz1NJP9+W7+j59/amln8YL5hMGPwYb4KU0iVRE+scY8FKADQiDH+MF8/saKxjozM8/fXgxofkzDJcAo/BTfrTSQ6h5WCJylDHRwfTonMAAaMHyEp79Nv9818p+392gB7TkqzfhhwuwdhqW0/C8GYqWiHSf0LwJw9sYs4XAW8vyP39mMHf5/wE/pJZJKs/o/AAAAABJRU5ErkJggg==" }</t>
-  </si>
-  <si>
-    <t>status=200||mediaId=(OPQA-AA01_mediaId)||entityId=(SYS_USER1)||entityType=profile||mediaType=image/png||context=1p-profile</t>
-  </si>
-  <si>
-    <t>{ "mediaId": "(OPQA-AA02_mediaId)", "mediaType" : "image/png", "base64Media": "data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAASwAAAEsCAYAAAB5fY51AAAABHNCSVQICAgIfAhkiAAAGYBJREFUeJzt3XuYFOWB7/HvW9U9V5gBBhxwAMVwEURBohgMRt2V9YKa5OhuPErcs15iPBv0PDlnZXWfk8c8m82um2fd9RKT+CTGVUyyu8nZTQRW18RoCCExxmgCchdE7gxzg5np6e6q9/xRM3JxlLl1V709v8/zjD7M9HS/9Ex/qap+6y3DYHzm2SpqU0vwgrngTcPaGXhmEtYO6m5FpAQYA6F9B2M2QbiF0H+d1vxyHr+mY8B3OaDvumfV9Rh7J5h5WFtLKm2wIdGHYiUi3YwB40Uf+ZzFmFawr2HN1/j7q77f77vr162XrboGa+/FMwvwfAgDBUpE+s4Y3m1HaNdizN/ywFXP9vnb+/xAy1Y8h192OTaEMAQUKhEZKANe95ZXkH2eB66+oo/fdRJ/ueoWLF/GT9UT5AY9TBGR4/hpCPL7MdzH3131xAfd9IODtWzl/cC9eH4ZYTCEIxQROUa0m5gF/pYHFt//fjfz3/cOlq34Aqmy+7HWx4YFGKGISDdrwRifVPoSLvyUZc13Xu7tZr0Ha9nK+0mV3U8+j45ViUjRhBZS6Uu58AbDmu+8dOKX37tL+JerbsHar2FMmd4BFJGiMwaszWLMnSce0/Lec2PLl/F8xUpE4mEtUYP48olfOj5Yy1Y8h5+q1wF2EYlVGICfqmfZiueO/fTRYC1bdQ1+2eWauiAiiRDkwC+7nGWrrun51NFgWXuv3g0UkUSJTve7t+ePUbDuWXU9nlkQzWAXEUmIMATPLOCeVddDT7CMvRPPR1MYRCRZbDSp1Ng7AQyfebaK0f5uDKP0zqCIJI4xYGmhOWhIUZtagg1r4x6TiEivrAVLLbWpJR5eMJdUemDrYomIFEMqbfCCuV60UqgOtotIgtkQ8KZ5WDtDwRKRRIumN8zwtAa7iCSeteCZSZ5iJSJOsLaXk59FRBJKwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOCMV9wBiYYHQHv3obdVVzxz/ISKxGz7BCkLIW8iHkPY597RRXDapltnjqjhlRNlxzfIMbG3qZP3BDla83cI7u9sACykPfA98BUwkDqUdrLA7UBhuPGscl8wYx8IZ9cwcV33Sb728+/+Pdf//17taeWndHlZuauTlHS1R1VImuiqtiBSFYdnK0rsKhQWyAWefUs31cyZw8/zJNNRVkR6CuHTkArYdOMJjP3uL7755gNaOLKT9wY9ZRE6q9IKVC8EzPHzVDG6YP5lx1WUFe6hNB47w+Oq3eHD1jiha2lUUKajSCVZooTPP0oWn8VeLZ1E/onChOtGGA0e44zuvsXpHC5SnQN0SKYjSCFY+5JTqMpb/9zksOrM+liEEFh57aSt3Pbe556KPsYxDpJS5Pw8rF3LpxBrWfO7C2GIF0d7g0kun8svPXhC9kxi6/++ASNK4HayugKun17Fq6UKmjhsR92gAuGBKHTuXXUJFVbr7HUoRGSruBisXcPWZY3n2jgVU+Mn6a0waVcmW/3URM8dWK1oiQyhZr/S+yoV8csY4/u3WC+IeyfuaOKqS5z5zAQ21Fdo9FBki7gUrsMypq+SbS+ZRkUr28CePqeL52+ZDNojmhonIoCT7FX8iC1jLv95+AWOqijdtYTDOmlDDM0vmatdQZAi4FaxswLc+MYvpCTnA3lc3njeZz86bEG1piciAuROsIOTchhpuWXhG3CMZkHuvmgXVZb2vDCEifeJGsCzgeXztutlxj2TAJo+u5FtXTIcubWWJDJQbwcqH3H52PRdMqYt7JINyy0enwMhyvWsoMkBuBItoFnkp+PYV06PzeESk35IfrCDk41PHMGNCTdwjGRKLzp5AQ3Vax7JEBiD5wcqF3PiRyZSVyMnEDTUVXHNWfbT6qYj0S/KDFcJVs0+NexRDasmHG7RbKDIAyQ5WYDl/6hhGpJM9zP6aWl/DpLFVOvgu0k/JLkE+5H/OnRD3KIZc/chyrplUo2CJ9FOyg5XymDJ+ZNyjKIgppypYIv2V3GBZqC73GVtTGfdICuKM+pEKlkg/JTdYWCaW+4yvLc1gTT9FwRLpr+QGy8L48hR1laV56cRZ9SP0TqFIPyU3WJT4ElIl/ZcTKYxEB0tE5FgKlog4Q8ESEWckOli2hA/0hNbqCtEi/ZTcYBk42BXQ1JmPeyQFsfFgu64OLdJPyQ0Whm2ZgF0tHXEPpCDe3NemYIn0U3KDZSCXDWhqy8Q9koJ4e/9hBUukn5IbLIB8yNa9bXGPoiDe2qstLJH+Snaw0h7/9NqeuEcx5Pa2Zfj+zjbwFSyR/kh2sDzD+u3NtGRK68D7pr1tNDZ1gFGwRPoj2cEC8A0rf19aW1nLf7MLUsl/6kWSJvmvmrTPd3/9Dl1BaVzq/Z3WDCs3HtTuoMgAJD9YvmHllibW7W6NeyRDYuXru9nXntPuoMgAJD9YAL7h4Re3xj2KQQuBO5/fDCnFSmQgHAmWx1NvHmDttsa4RzIo3/zZNujQ1pXIQLkRLANYuOFf3nD27MJtje3csWozlJfmgoQixeBGsAB8w87GDh75yea4R9JvIfDFZ9dDLtAJzyKD4E6wANI+d6/azO/2uDX7/clfbOfpdQegxK6vKFJsbr2CDOAbrvvmrzh4pCvu0fTJb99p5tbv/U7zrkSGgHuvIs+wta2LTz3xCm1dyZ4Bv2n/YeY9/gpUpLQrKDIE3AsWQMrjp2+3cu3jv6QroVee2bT/MJd/8xXI5HSSs8gQcTNYAGmPl7c3s/jrv6Ajl6xZ8G8daufMr/6Ct1s6wXf3KRZJGrdfTWU+P9nezPyv/JTf70nGTPgXN+7nQ3/zImTyipXIEHP/FZXyWN/cyfyvruX7r+2K7WLK7dmAv171Jn/4xKvRu4HaDRQZcu4HC8D3yOQD/vjJ17h9+avsai3uKqW/3d3KJQ+t5gsvbItmsWsmu0hBGJatTOZR64HKh9AV8MUrpnHrRWfQUFNRsId6fVcrD/10K0+u3QkjyrRVJVJgpResHtmAhppyrjurntsWnMbU8TVUDsFcqObOHBv2tPLgT7fxg7eaIBtojpVIkZRusACsjba4rOHaqaNZOHUsF59Zz/zJo7D0bWqUBXJByItbGln95j5eeKuJX+8+HK1n5XuaXyVSRKUdrGMFFoIwCljKZ3ZDDRc3jGRmXRVjq9LHnVTtGdjenGFjUwfP7Wpj394jUZhSXhQq7fqJxGL4LB3gG/B9KPPBwrr9h1m3tw1CS69LQHhEB889A1XD52kSSbLh+Uo0HI2RiDhDR4tFxBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnDM9zCUWOZbv/Y0/480mZ45cXMr18ToaUgiXDiyVaJy3s/ggslKcYU5VmYkWK+ooUI9IedeWpD0yWATJByN6OPIG17O7MczAb0JLJQ2c+OrH+3Y/u71DIBk3BktIXdi/k6BlIe0yqLOPC00ZzXkMNH508iurKMqoq01SXpxhZkaYi5ZHqY1wOZwNCC22dWTK5gM6uPJnOHBsb21mzs4WNB9tZv+8wh3Ih5MIoln73umrSb24u4NeeI7bL4wxE2ouu/lworjwfnoHqdOEfxwJhCPloK+rDp49iyaxTmDl5NHMmjWb8iLLCj+EEGw62s3VvK5v3tPK9TY28+lbz8YtC6sIlfeJesNpztD5wJdUVaaxN/tBTvsfPN+zjom+8Uphotefo/IerSae8RD8fnjG0tHdRd9/zhYtWz5ZU2ufGqWNYMH0cN54/iTFVxQ/UybRm8vznm/tYs2E/j25shMNd3ZeH07LbH8S9XUJrSac8fM/gyk825Xt9O4Y7EKE7z0c6VaDnoTtUM8dUcu3Z4/nsR0+nYUw16QQv0FhbkeKGeRO5Yd5ElrV08uqOJr6+ZgfPv9Ma7Tqm9QZ+b9wLFtFhAKcUeMDRllVyX5w9hvxpCC10BYyoq+LbV05n0TmnUlvu3q/0xFGVTJzbwCfmNvD6rha+tWYHj659JzpYn/Zd+NEWjXs/XRFrIRNwTsNI/u+i6Vx/bkPcIxoycyeO4pFPzeW+q2by2Itb+NKandHFU3QpOUATR8U1+ZDKlM/Xr5vN6rsuKqlYHWvCyHL++uOzefPzF3HjzHHdl6tzbddi6ClY4gZrIZPnkzPG8cbdC7njY2dQU8h3XhNi5viRLL/1An5w07kQEoVrGCv9n7i4LwgBw/f/dB7XnTsx7tEUnQH+27kN7J9+Cku/+xr/um4/lKeG5bEtbWFJsuVCPjZhJBv+4uJhGatjnVKd5ju3XsDDH5/ZfT3N4beLqC0sSa5swJ/NncA//slcaofB7l9f+AaWXjqNMSPKWfJvv4+ileDpG0NNW1iSPBY4kuWLi6bxxM3nKVa9uOn8yfzktvnRDHkXznIYIgqWJIuNJoE+fsMcvnDlmXGPJtH+YPo41t75kWhC7jCJloIlyWGBwPL4J2Zx+8IpcY/GCR85fQw/XHJu97SHuEdTeAqWJEd7NorVRWfEPRKnXDlrPP909ZmQDeIeSsEpWJIMXQEPXT+b2xcqVgNx9x9M4/9cOBky+biHUlAKlsQvG3DPx07nrkumxj0Sp9139SwuOWN097y10qRgSbxyIdfNGMuXPj477pE4b3RlmkeunxOtolqix7MULIlPaKkZUcY3Pn1eopeCccnsU2v48uXTIV+ax7MULImHBfIhP771fOqqirAK6TDyvxdN54zRlSU51UHBknjkQ7502VTOnzw67pGUnDLP8NC1sxQskSGRD7n4tFruuXJm3CMpWYvOmsBlk2uj41klRMGS4rIWPI9Hrp9DWoetCqbcN9x7xZnQVVrHshQsKa6ugK8s+hBnn1oT90hK3sIPjeWPZtSV1FaWgiVFY62F6jLu+sPpcQ9lWCjzDbctOK2kFv1TsKRo8ha+e9McyjSFoWj+eN7EaLG/Elk7S8GSohldXc4n5w3vRfji8DcXnx5dOqwEKFhSNJ6Bcl39pegWnz2heysr7pEMnn57RErcnImjuGz8iJKYl6VgiQwD1849tSQOvitYIsPA4ln1JbH2u4IlMgzU1VSwYGKN87uFCpbIMFBbnmLx1DHOr5WlYIkME7OnjI0mwzlMwRIZJi6eOtb503QULJFhYlRFigmOH8dSsESGkZumjXF6K0vBEhlGFkwe7fR5hboGuJSU/e05Nuxr4+DhDB1dAYfbOghyAWAAi/E8RtRUUlNdxvT6Gs4ZPyLuIRfVuLpqSPvRaToOTstSsMRZ+9uzbNrdwtpth/h/W5t4ZVtTdPEF34tejMb0/qK0RFsZ3btGZ04Zzec/fCoXzqjnrPEji/lXKLrT66oZW+bRmO2JuFsULHFKZz5k055WHnxpG798u5ktbdlobpHvQYUP+P2+z417D/OZ/9iAqdrKtZNr+YvLpvHRD40d+sEnwKTaChoqUjR2BS72SsESd6xav4+vvbyNFVuawDfRqSa+Ab//kTpO933YfMgPtxzih5sP8fmPTOK+xbNK8oo+48dU80ZLBheLpYPukni/39vGxQ+tZvE3fsWK7c1Q7kPKG/pz4wzR/aY8Hly7k4a/e5GXtjYO7WMkwHmTa52d2qBgSWIFwKMvbuGcB1fzs3daoSod7foVmgHKfLoyeS59bC3/tWF/4R+ziM6pH+ns1AYFSxLrtuW/YemKjdFvaRwL/3kGUh6XP/kbXtx0oPiPXyDTx1Y5u5ifgiWJk8mH/NFjv+DJV3dDmR+92xcXz4C1XPf0a7zd1BHfOIZQZUUaKtxcgVTBkkTJhZZPPfEKL2w9FL2oksAztGTyXPvEK66fOwxARVmKsVVpXCyWgiWJ8lf/sY4fbWqMtqySJOXxuz2HeWL1trhHMmiVZSkmVWoLS2RQfrJxP195eXs8x6v6Iu1xx8pNHHb8asojK1JMqi5TsEQG6mB7lsuWvx5NWUjq9CBjIBvw0I83xT2SQalMeYyrcPNahQqWJMI//Ncm6Mgmf93xtMfXf7OHA4e74h7JoIwsT9gudx8pWBK7LQcO88Aru6KTcpPOM+xu6uClzW5Pc6iprdQWlshA/P0LmyGbT+6u4InSHk//amfcoxgUz/d0DEukv3Y0d/K9Nw8m90B7bzzDz/ceYfPB9rhHMmCT6tycPOrQb4mUopfX7+VIZy7eyaH9ZQwt7Vm27GqOeyQDVuZ72iUU6a/71+x0a+uqh2f49w0H4x7FgKWKcU5mAbg5aikJ25o62LGzJfnvDPbG9/jWG3vjHsWATR9b7eSKDQqWxOaljQeSN6O9rwzQnmVnaybukQyIg60CFCyJiQV++9ahaPE8V/keb+xujXsUA+JorxQsiUdTe5YVO1vd3B3s4Rt27WuLexQDMrG23MlqKVgSi86uHG8f6nA7WJ5hx8EjcY9iQEZVpvUuoUhfbdx/BPJh3MMYHGNY39RJp4N/DwdbBShYEpOf72h2+/gVgIE3mjrpyrm9eoNLFCyJxfYDR9zeHQQwhl1HsgSBe1tYrlKwJBatrZ1uzW7vjQEUrKJSsKTo2nMhjRmHTnb+IMawo7kz7lEMGwqWFF1rJkdTrkS2Sgx0ZHUMq1gULCm6I115mnJuXir9PTzDxgNuTm1wkYIlRdfZlWd/LqQ0igWBq3MEHKRgSdFlsoH7c7B6GOjULmHRKFhSdK6/OXgcY9ilg+5Fo2CJDFJJBTjhFCyJh17kMgAKlhRdPhdA3ipa0m8KlhRdrisHOv9OBkDBkuIzRltXMiAKlsggBa6uN+wgBUtkMDxoPuTu9Qldo2CJDIr2bYtJwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZTgbLM3GPoH+MKeyAC33/Q82t0ZYm115DPVJxD6DfjKE9kwcgtDGPpQ9SvkdnNl+4V6lnaM/kSKc8rCvPRy4AxyL7QQJrsdbSmQ3iHkqfeIboNeTgz8CwbKUDv+YnaM/hxKuzR8qDigL+2+Da85H2odyPexRDJ7DQmYt7FP1jDFSn4x5Fv7m3hQVOPtEFpecjXr6BEWVxj2JYcPIYlogMTwqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGR5CPewwiIicX5PHIZZxcKlVEhhFjIJfBI5eNeygiIieXy+KR63JrPXARGX6shVwXHl2dELpxtQ8RGabCALo68bAhZNp1HEtEksmYqFE2xMN40NGm3UIRSSZro0YZDw/IkM1qK0tEkqdn6yqbBch4YDfjGWg7pK0sEUkWa6M2eQawmz0w2zAe5HPQ3qKtLBFJBmOiJuVzYDzAbPOAXRgTfbHtEOSyipaIxMuYqEVth3i3T7DLA/sjgnwGDFigeV/3NAdFS0TiYKIGNe+LmoQhapT9UVSlmx/dg2EC1kb7jOWVUDcBRUtEis/Cob3Q1Xl068qyl6c+d2q0WoO1P8Tzo9saE92wab92DUWkuIyJ2tMTKwDPjxrFu8vLeM8Q5DvevYExkDkCjbshDBUuESksY6LWNO6O2nNsi4J8B3jPQE+wnv7zn4NdhfGPuQMvqlzjLsh0dB+lFxEZYsaLGtO4q3vL6pjWGB+wq6JGHbuAX87eR5jnuONWxkRvKTbthbaD0fEtbW2JyFAwpnue1cGoMfncCX0xEOajNnU7ukm17rkm5lx1Cp5//nETSHvuoKszmnEKUFbZ/XnFS0T6wxxtR3sLtBw4epbNiRtD0bGrx3jmrqeP+e4T3PzIOjz/rPddwaFnK2vEKCivgnR5dMfYo18XEYFjItQ9VSHXBV0dcKTlg/fYPB/CYD1PLZ197KdT730A727C4HsYbyw2fP8BHG6OHtRPRdEqK4dUefRnERGAIA/5Lsh2RbEK8kdD9X6xMh6EQSPGu/s9X+r1Gz798P8A7wk8TJ+2mN69jX13Q0tEJCrMMe/4nfT2BkIshLfw9F1P9np3vbr50U9i7Q/wPNPrlpaIyFAyHoShxZjreOpz/97bTfzePgnAG6s2cvaV+4AL8f1KHZsSkYLxfAjDJkL7eZYvXf5+Nzv5NtqSRxfh2W/g+VMIQ7TPJyJDx4DnQRhsJzR3sPxzL5zk1n108yNPA0u6S4jCJSID926oAJbz1NJP9+W7+j59/amln8YL5hMGPwYb4KU0iVRE+scY8FKADQiDH+MF8/saKxjozM8/fXgxofkzDJcAo/BTfrTSQ6h5WCJylDHRwfTonMAAaMHyEp79Nv9818p+392gB7TkqzfhhwuwdhqW0/C8GYqWiHSf0LwJw9sYs4XAW8vyP39mMHf5/wE/pJZJKs/o/AAAAABJRU5ErkJggg==" }</t>
-  </si>
-  <si>
-    <t>{ "mediaId": "(OPQA-AA02_mediaId)", "mediaType" : "image/png", "pathPrefix" : "stable-pics1", "base64Media": "data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAMgAAADLCAYAAAArzNwwAAAAGXRFWHRTb2Z0d2FyZQBBZG9iZSBJbWFnZVJlYWR5ccllPAAADylJREFUeNrsnb1y20gWhRvwuso1ienM2VCRNxsqm0xUttGYfAJR2WYys8kkPYHIJxAZTW0karKNTGWTGcrWkaFM2XKSqZlysNtXurBhivjvBvrnnCoUbYmkgO7++tzb3WgIAUEQBEEQBClWgCJoR98NfurJlwH/t89HWi9Tv090s+OrYj5I0R/RrxuULgCxBYKk4Q/l8X0KhL7mPx3JY8Ovd/wKeABI544w5F7/gF97hp1mAg050RrQAJA2gHjLr31LLyViWG4kLCvULABpAsWAYTjakR+4ohU7zEoCE6PWAUgZKAiIkcUu0cRdloAFgOwKnyaOO0VVrVOwbACIn2Ak4dMEPOQm+hSGzSUoEQDxwy0ofDr1MIRS4ioSlAUAcROMd/I4EeYNx9omyk/OfQi/AoABNQy/5vKYuQpKADAgVaBISM4AiB1wnAGM7kIvl3KUwDEwKPm+QPJtRDJPoKwBiBlgEBCX4nHWGzJH5CRTm/OT0JFw6gPgMFITeXySdTSBg7QPxoBdAzPf9oRdx7YtYXlmsWv8Io/XaHfWiMLgyfPXb/76fP/xNziIvlzjCq5hvVbsJsbnJqFFcEw41wAc9mvEuYnxeeMzS+CgXIPCqhdoW87oBYdcgQy51gixEFJBFoZcgcFwEBTvBWbDfVHEkBi1pD40FI4k3wAc/uihQzQtLwkNhIOWilyivXipHkMyQZKenYz/E+3Ee41MSd4DQ8DosWuM0DaglBYyJzn22kEYDkrGh2gP0HZeIp2kL53k2ktAUnBgGBcyEpJngAMCJIYBAjggWyDpapgXcEB1NOGRTncdhC/wH6hrqIGT9KST/Ns5QBiOCeoYaqgfJSR3EhLty1LCFuF4BzgghbrkTTq0KmgJDrqQK9QppFi0+vdQ5wLHoAU4sCoX0qlYHvu6lsqHmuHosXMADkiX+jqjE905yKXAJm6Qfg15FbhyaRvF4p1HsDIXaks0snX7+f7jf4zPQfiml/eoM6iDpH1f5d5boQY4kqXrENS2lLc9HTkI8o78Hm4mj7E8DpND9njk5K/4/1PxuKdtjOKqnY+cGRliYb4jU9TYKz8WgHd1oXD1QNj9bPYutK9ifiRQCAfZ2yeBId1tx5iqel5G6rntJ4ClUJEs9/2mX6JsFOv56ze0Vy5W6H7VQyglK0nZPrSf7z/e07628pjL8qZl33+Kx/2J0Sk91WsV97UrcRCMWj1xjXGbD49hZ6HHWY/gLE+012RUK1BQOdR7fUDFPGjNcHS2QyBvmXMkcI//lzqR9XHYWYglbexngd1ISLQDx1ha+p9dngQtAZfHkpaDc8jre/jVbzKB2MhBeJQFOyAasD1Njrufisen/fosCrFqLWhsOg9yCjjMhINEDUIeNK9yyLmRty5St5Oo7SBIzM2GIyOR9/mRdRtO2Ct1FE0c5NRzOGgSamrLyfKk2SGft4+iSKfyit9aDgL30H8nm2Yn8fkGtkrDvnUdxHf3mNsIR8pJxh7XXaW2W9lB4B4ilo1sz/aL4BuMfB3dKu0ioW4CHdS5Q9fh68hW6TZcyUHgHm64R6o+zzzu8F6VGdGq6iBHnrvHyrHrmXlcl6XCy9KA8Kz5xHNAli5dDPegK0/r8kR1DnLiORwbW0euCnTtaX32yjwLsQogvruHqxNsa4/r9EQJIEya72uuYhcvioc7fR3NGvDEaWMH8T05J93BHf1zkUJAUhsHQJCLGjV1ENwM5b5uPL72Xt5jFMoAcoL2Azmuo1qAcALTR/lBrodZfPdlZQdBeAX5omEdQN6i3LzQDyiC3W09zAmvKLTCRnBfdeByoorq3R0thVUtBwIgrpYBr1YvDQjCq2/Vd/jaEClkmAIcxHNAipZa+J6HhDmFBtvdnZfBPRx20u3h3hDu4b2LYAQrp+1nAXKAcvKmt0VnmFPHcJBq6gF653WQCwjH2cg/ditGESDEQo+yWwtVj1IzTDNU7ROTGACQ6po6el3nqNon6ucBglGNp1p3+dQonXL1ulTlZXAQCMpJ1MM8e4G+CIMWntZ3mJWcQH64qqOrA7SFWOgpsxuSq5AAkJyOYxuQIYrGOxdBned0HCHKoXrihuvyFxAM8frX08JBKgCCHCSnwFxLaPP2g4J2J+lQvi4cux7seVYQeoaeJKKqNCqzZb4l7nGG8Kq6gyDE8sBF+K65U1QlQiwd6jmQiyBSACBoYDlCaFWyjABIgwQO5w8HgRzrgTn/gIMAEL0hlsV5COAAIGhoOcLj9ABIK7Juko3DK8yeAxCEWRl6h2oDIG3Kmsk2dg8sLQEgrSrz0V0GaiKwUqKKNgCkuXo2hC1YWlJLEQBRlKxbkIu8g3uoCbFiFEktFzG2d2Z44R4ApNv4ftfjuwzRJaoHOYgRDdG0hF2eD4VWQ1RNLd3CQdSKQpkLg+AYCPfugOw8xLpDkTQOtSYGwEFOdoXqaKSdo1jYyLi5LrrcZI7heC+wIZyWHCRCuTTWQwPtcOiXwircMajJQZCDqIPkqu2kXf49GrGaoPibK3ksRLj1QwCiToO2nIRAlMd7wKHWPXY5CMIs9ZB80JmTMIAExxDFrUxxHiBwET05yUQDHHRvxwfkHMp1mwfILcqntjY5kNBEopK8hFyDvks8DuVijVXLIdYa5VMbjkN57OeAQj3+J9rVsA4onGucsWvk3Rm4EBiyVwJIsKsS5Mt/UUbV4fgj+jXiMhxw794v+Aw15GXyuYJQ6m2JJJy+81h+34rP4RLhV/W6lOX3KhMQrpBPAhNNteDY6miuSibPMfda6fD2JTfussk3fX6cHonkc7gUuA+9ilayDMdFgGA8vZzW3GPHOb0/hUS6l5ufy3M4yzmHIZ/DEFVWrSyzVvPeoJxKhTKHRXNHXNh7mnI7+s69PDj4HOh91Cueo+pKlakocpABJ4LQUzDm8pglM60Vk2xVPfmKzoMbftVz6PM5IELY3ZkEhYAgD1ELRkYHdMS5QdkyphxjyTFyrOAcElDoHDBUzO5BUUFZQJCHPCbPS1Vg5MAyYFC+59dNKmEnl4h0/X0+B6rnt0jmxVSW86wsIBPh7+2a1Chp+HXh00Wndl488jSh398ejQwKCsun+ZA4FdvHwnNxCDZhWHwItWNZ73vbPwwKCsn1RXAbhuKaJtcQgudGE667ykK2gePtH/6t4EPXDhYKoKgoDjUXnC+dOJqbXu/6YZGDkLV+cqQAVpxXAAp1ucqJcGMpyzfLS0oDwoVh+3LqFY9OxGjaWmChCMP2Wfqd4RWpzL5Yc4uTbprpHgMOreFXMncwFfauIF5m/aIMIDaGJHTO+3VmmqHaoND8AS31t+2O1DivnYQlLjxZlm2TXY51TqxBmW3lwbUt61SXeb8su/XotS3OkRVLQq1B8rCQ0yInWTQGhEd+TI/jk4qBzIHEhg41VuEgNiTr5wirjIIksiA0Xxa9oQogC2HuKEW8vcgMMkJTw9vMShkg3DubmnzhRiBzQ62FzW0mdKAhxr6turVMJobmpTv7sGKPEBvYIyzRBo12ERPbzLxsvlrnCVOmuQjcw3yZ1IkRGKXz1dDyHmGFZSRWuMhamDNNMK8y2ln3GYWmuMg1mp81MmGAp5J71AbEEBfZIDlHmKXTPZo4iAkuskabsyrMijoOs+Kq7tEIEHaRLiFBeIUwq1KHXmelRdPnpM9EdzOluDPQPnXVqUV1w/FGgDCR044uGOuu7AuzugqLa7fRUMFFLzrIB5B/IMwqq0UTMMOuCa0pbK5tr9qsu8YRjhJAeISizYQdDmKv2ryR6rhpKB6oPJuWdkCh/GMf7cxeyXbyvzZCufSDcLoOsb4QC/eADKhDZXc0KgWkpVALT+FFmKU9tNLlIMkTlSKLCxfSL52d3ELl7pmhppMcC00TiEVPhIW8dpBYKB5RDTU14lhTPoL8wwFp7OSU74cWaiwEsrmZhh4CQqKelXcoBy/UWQLyhKeKC+IO7coZqezsFrpufQhbKIixwsJAiOWOVHV2kc7dNLUDwjGhqqQdCxQRYm270KHOk2zDQZKk7FjR90BuaKPg89o3KQ/bKg1O2ptAAjgckoLObtxGhxm2XCiUSNWdaUd4hUQ90XFb95aEbZcIz7TXGXGAgwCQBI5FWycYdlEqPOpQ9SJ/R3vyHpDjtneyCbsqmRqQwEHc053JcHQKSA1IkIO4p43JcHQOSEVIAIh7ikyGwwhAUpDMCt6DEMs/HXe9e2ZoSknwuq3MeZLvBj9N0F6c01FOtDA2YWvZwLQSYxAu5NHb8WsqsCn2xLJbso6pbq/kMcyA49CUiCEwtABp44f3GZBEQtPSZqiVuiUoLuXRz6jbsUmPtAhNLERu/HsZSdwDPAi5rITjjDu+XXCs2Dlik845MLxAexxuZcGwEgpv0Ie01WOfXWOY8ZZzXmFhnAJLCjgvL9kwJNjM2sy6eydfTnPqbtzhnr1uAJLKSy5F9sZ0K07gYzRLY+rrIsc11tyxGV1fz2wp8M/3H++fv37zL/nPF/L4ccdb/k6hmHzPX/K9v6GJdhcWyzr4Wf7zl4xcIwmpjmU9GR8aB5ZWwojdpJfxlojdZI0m23oofJoDhnUjkIHFldFjSEY5b7PCxh0AY8hgDHPeZmwi7iQgW5VzmdNrkRZcQQBFbdn3Rf7olJWu4RQgKTdJRksEQGkFDCrrSc7bNlzWM5uvNXCw4i4Kwi6AojeUIs1EzYdmAhCzKpJylDnmUEol3yei+NkvzuV8geMVO2JH6Re8lSqUHnS/gKt848YnHEb1SoBx7uKoYeBJZU9E/vBjWuQm9LjilW9LWDiXG5V0C6fB8AqQGqFXkmQSLDcuw5KC4m2J3C3dicx9mGfyCpBUoxikwgdRoVEksMQOXD91Ekei/DMlkw7Dq8ENLwHZ6j2TBLRf4aMxhxcETGT6GH8KiAN+7VX4OF3b3MeQ03tAdoRfRxxm9Cp+fMMN6YZf466g4esg2H9gdxjW+JqY3WLp+41pAGR3I0vH5L0GXxWl4Pk99X9RJ35nx0tCoj4fL/ln/YoumBVCXWPYG4BUheWAYelr/nOx+Lrb4KAhnGUBXsMpAIgqWPpbsXzfskuIUqHgCndiApA2gBnwcdBSr1/FjQiGW3aJCEAAEBOg6aWg6TE4ukKmTSqvuU1CNNwHA0Bsh2i49aM8eBIIvggAQBAEQRAEQRbr/wIMAB2nwEL3kwxHAAAAAElFTkSuQmCC" }</t>
-  </si>
-  <si>
     <t>Verify that user is not able to update media with invalid media ID for profile context by Entity ID using base64 API and check the error status</t>
   </si>
   <si>
@@ -278,9 +187,6 @@
     <t>Verify that user is not able to update media with invalid media ID for profile context using base64 API and check the error status</t>
   </si>
   <si>
-    <t>OPQA-SS01</t>
-  </si>
-  <si>
     <t>Verify that user is able to create media for profile context using Streaming API</t>
   </si>
   <si>
@@ -296,42 +202,24 @@
     <t>status=201||entityId=(SYS_USER1)||entityType=profile||mediaType=image/png||context=1p-profile</t>
   </si>
   <si>
-    <t>OPQA-SS02</t>
-  </si>
-  <si>
     <t>Verify that user is able to update his own media for profile context by media ID using Streaming API</t>
   </si>
   <si>
-    <t>/internal/media/(OPQA-SS01_mediaId)</t>
-  </si>
-  <si>
     <t>src/test/resources/media/kPl0TGN.jpg</t>
   </si>
   <si>
-    <t>status=200||mediaId=(OPQA-SS01_mediaId)||entityId=(SYS_USER1)||entityType=profile||mediaType=image/jpeg||context=1p-profile</t>
-  </si>
-  <si>
-    <t>OPQA-SS03</t>
-  </si>
-  <si>
     <t>Verify that user is not able to update media with invalid media ID for profile context using Streaming API and check the error status</t>
   </si>
   <si>
     <t>/internal/media/0f28b7f1-2bee-4178-ad9f-3d5e68d167</t>
   </si>
   <si>
-    <t>OPQA-SS04</t>
-  </si>
-  <si>
     <t>Verify that user is not able to update media with invalid Entity ID for profile context using Streaming API and check the error status</t>
   </si>
   <si>
     <t>/internal/media/1p-profile/profile/(SYS_USER1)A</t>
   </si>
   <si>
-    <t>OPQA-SS05</t>
-  </si>
-  <si>
     <t>Verify that user is able to update his own media for profile context by Entity ID using Streaming API</t>
   </si>
   <si>
@@ -341,14 +229,182 @@
     <t>src/test/resources/media/8mb-artwork.jpg</t>
   </si>
   <si>
-    <t>OPQA-AA17_1</t>
+    <t>Verify that for the given invalid Entity ID, default media is retunred and no error thrown by using GET Media by Entity ID/Type API</t>
+  </si>
+  <si>
+    <t>Verify that GET Bulk media by Entity API is working as expected for multiple truids.</t>
+  </si>
+  <si>
+    <t>mediaId||mediaStorageLocation||mediaUrl</t>
+  </si>
+  <si>
+    <t>Verify that GET Bulk media by Entity API is working as expected for single truid.</t>
+  </si>
+  <si>
+    <t>src/test/resources/media/Neon1Profile.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that separate media with existing location API is works as expected  </t>
+  </si>
+  <si>
+    <t>/internal/media/existing</t>
+  </si>
+  <si>
+    <t>/media/1p-profile/profile/bulk</t>
+  </si>
+  <si>
+    <t>?id=(SYS_USER3)</t>
+  </si>
+  <si>
+    <t>status=200||entityId=(SYS_USER3)</t>
+  </si>
+  <si>
+    <t>?id=(SYS_USER1)&amp;id=(SYS_USER3)</t>
+  </si>
+  <si>
+    <t>OPQA-5252</t>
+  </si>
+  <si>
+    <t>/internal/media/(OPQA-5252_mediaId)/base64</t>
+  </si>
+  <si>
+    <t>{ "mediaId": "(OPQA-5252_mediaId)", "mediaType" : "image/png", "base64Media": "data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAASwAAAEsCAYAAAB5fY51AAAABHNCSVQICAgIfAhkiAAAGYBJREFUeJzt3XuYFOWB7/HvW9U9V5gBBhxwAMVwEURBohgMRt2V9YKa5OhuPErcs15iPBv0PDlnZXWfk8c8m82um2fd9RKT+CTGVUyyu8nZTQRW18RoCCExxmgCchdE7gxzg5np6e6q9/xRM3JxlLl1V709v8/zjD7M9HS/9Ex/qap+6y3DYHzm2SpqU0vwgrngTcPaGXhmEtYO6m5FpAQYA6F9B2M2QbiF0H+d1vxyHr+mY8B3OaDvumfV9Rh7J5h5WFtLKm2wIdGHYiUi3YwB40Uf+ZzFmFawr2HN1/j7q77f77vr162XrboGa+/FMwvwfAgDBUpE+s4Y3m1HaNdizN/ywFXP9vnb+/xAy1Y8h192OTaEMAQUKhEZKANe95ZXkH2eB66+oo/fdRJ/ueoWLF/GT9UT5AY9TBGR4/hpCPL7MdzH3131xAfd9IODtWzl/cC9eH4ZYTCEIxQROUa0m5gF/pYHFt//fjfz3/cOlq34Aqmy+7HWx4YFGKGISDdrwRifVPoSLvyUZc13Xu7tZr0Ha9nK+0mV3U8+j45ViUjRhBZS6Uu58AbDmu+8dOKX37tL+JerbsHar2FMmd4BFJGiMwaszWLMnSce0/Lec2PLl/F8xUpE4mEtUYP48olfOj5Yy1Y8h5+q1wF2EYlVGICfqmfZiueO/fTRYC1bdQ1+2eWauiAiiRDkwC+7nGWrrun51NFgWXuv3g0UkUSJTve7t+ePUbDuWXU9nlkQzWAXEUmIMATPLOCeVddDT7CMvRPPR1MYRCRZbDSp1Ng7AQyfebaK0f5uDKP0zqCIJI4xYGmhOWhIUZtagg1r4x6TiEivrAVLLbWpJR5eMJdUemDrYomIFEMqbfCCuV60UqgOtotIgtkQ8KZ5WDtDwRKRRIumN8zwtAa7iCSeteCZSZ5iJSJOsLaXk59FRBJKwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOCMV9wBiYYHQHv3obdVVzxz/ISKxGz7BCkLIW8iHkPY597RRXDapltnjqjhlRNlxzfIMbG3qZP3BDla83cI7u9sACykPfA98BUwkDqUdrLA7UBhuPGscl8wYx8IZ9cwcV33Sb728+/+Pdf//17taeWndHlZuauTlHS1R1VImuiqtiBSFYdnK0rsKhQWyAWefUs31cyZw8/zJNNRVkR6CuHTkArYdOMJjP3uL7755gNaOLKT9wY9ZRE6q9IKVC8EzPHzVDG6YP5lx1WUFe6hNB47w+Oq3eHD1jiha2lUUKajSCVZooTPP0oWn8VeLZ1E/onChOtGGA0e44zuvsXpHC5SnQN0SKYjSCFY+5JTqMpb/9zksOrM+liEEFh57aSt3Pbe556KPsYxDpJS5Pw8rF3LpxBrWfO7C2GIF0d7g0kun8svPXhC9kxi6/++ASNK4HayugKun17Fq6UKmjhsR92gAuGBKHTuXXUJFVbr7HUoRGSruBisXcPWZY3n2jgVU+Mn6a0waVcmW/3URM8dWK1oiQyhZr/S+yoV8csY4/u3WC+IeyfuaOKqS5z5zAQ21Fdo9FBki7gUrsMypq+SbS+ZRkUr28CePqeL52+ZDNojmhonIoCT7FX8iC1jLv95+AWOqijdtYTDOmlDDM0vmatdQZAi4FaxswLc+MYvpCTnA3lc3njeZz86bEG1piciAuROsIOTchhpuWXhG3CMZkHuvmgXVZb2vDCEifeJGsCzgeXztutlxj2TAJo+u5FtXTIcubWWJDJQbwcqH3H52PRdMqYt7JINyy0enwMhyvWsoMkBuBItoFnkp+PYV06PzeESk35IfrCDk41PHMGNCTdwjGRKLzp5AQ3Vax7JEBiD5wcqF3PiRyZSVyMnEDTUVXHNWfbT6qYj0S/KDFcJVs0+NexRDasmHG7RbKDIAyQ5WYDl/6hhGpJM9zP6aWl/DpLFVOvgu0k/JLkE+5H/OnRD3KIZc/chyrplUo2CJ9FOyg5XymDJ+ZNyjKIgppypYIv2V3GBZqC73GVtTGfdICuKM+pEKlkg/JTdYWCaW+4yvLc1gTT9FwRLpr+QGy8L48hR1laV56cRZ9SP0TqFIPyU3WJT4ElIl/ZcTKYxEB0tE5FgKlog4Q8ESEWckOli2hA/0hNbqCtEi/ZTcYBk42BXQ1JmPeyQFsfFgu64OLdJPyQ0Whm2ZgF0tHXEPpCDe3NemYIn0U3KDZSCXDWhqy8Q9koJ4e/9hBUukn5IbLIB8yNa9bXGPoiDe2qstLJH+Snaw0h7/9NqeuEcx5Pa2Zfj+zjbwFSyR/kh2sDzD+u3NtGRK68D7pr1tNDZ1gFGwRPoj2cEC8A0rf19aW1nLf7MLUsl/6kWSJvmvmrTPd3/9Dl1BaVzq/Z3WDCs3HtTuoMgAJD9YvmHllibW7W6NeyRDYuXru9nXntPuoMgAJD9YAL7h4Re3xj2KQQuBO5/fDCnFSmQgHAmWx1NvHmDttsa4RzIo3/zZNujQ1pXIQLkRLANYuOFf3nD27MJtje3csWozlJfmgoQixeBGsAB8w87GDh75yea4R9JvIfDFZ9dDLtAJzyKD4E6wANI+d6/azO/2uDX7/clfbOfpdQegxK6vKFJsbr2CDOAbrvvmrzh4pCvu0fTJb99p5tbv/U7zrkSGgHuvIs+wta2LTz3xCm1dyZ4Bv2n/YeY9/gpUpLQrKDIE3AsWQMrjp2+3cu3jv6QroVee2bT/MJd/8xXI5HSSs8gQcTNYAGmPl7c3s/jrv6Ajl6xZ8G8daufMr/6Ct1s6wXf3KRZJGrdfTWU+P9nezPyv/JTf70nGTPgXN+7nQ3/zImTyipXIEHP/FZXyWN/cyfyvruX7r+2K7WLK7dmAv171Jn/4xKvRu4HaDRQZcu4HC8D3yOQD/vjJ17h9+avsai3uKqW/3d3KJQ+t5gsvbItmsWsmu0hBGJatTOZR64HKh9AV8MUrpnHrRWfQUFNRsId6fVcrD/10K0+u3QkjyrRVJVJgpResHtmAhppyrjurntsWnMbU8TVUDsFcqObOHBv2tPLgT7fxg7eaIBtojpVIkZRusACsjba4rOHaqaNZOHUsF59Zz/zJo7D0bWqUBXJByItbGln95j5eeKuJX+8+HK1n5XuaXyVSRKUdrGMFFoIwCljKZ3ZDDRc3jGRmXRVjq9LHnVTtGdjenGFjUwfP7Wpj394jUZhSXhQq7fqJxGL4LB3gG/B9KPPBwrr9h1m3tw1CS69LQHhEB889A1XD52kSSbLh+Uo0HI2RiDhDR4tFxBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnDM9zCUWOZbv/Y0/480mZ45cXMr18ToaUgiXDiyVaJy3s/ggslKcYU5VmYkWK+ooUI9IedeWpD0yWATJByN6OPIG17O7MczAb0JLJQ2c+OrH+3Y/u71DIBk3BktIXdi/k6BlIe0yqLOPC00ZzXkMNH508iurKMqoq01SXpxhZkaYi5ZHqY1wOZwNCC22dWTK5gM6uPJnOHBsb21mzs4WNB9tZv+8wh3Ih5MIoln73umrSb24u4NeeI7bL4wxE2ouu/lworjwfnoHqdOEfxwJhCPloK+rDp49iyaxTmDl5NHMmjWb8iLLCj+EEGw62s3VvK5v3tPK9TY28+lbz8YtC6sIlfeJesNpztD5wJdUVaaxN/tBTvsfPN+zjom+8Uphotefo/IerSae8RD8fnjG0tHdRd9/zhYtWz5ZU2ufGqWNYMH0cN54/iTFVxQ/UybRm8vznm/tYs2E/j25shMNd3ZeH07LbH8S9XUJrSac8fM/gyk825Xt9O4Y7EKE7z0c6VaDnoTtUM8dUcu3Z4/nsR0+nYUw16QQv0FhbkeKGeRO5Yd5ElrV08uqOJr6+ZgfPv9Ma7Tqm9QZ+b9wLFtFhAKcUeMDRllVyX5w9hvxpCC10BYyoq+LbV05n0TmnUlvu3q/0xFGVTJzbwCfmNvD6rha+tWYHj659JzpYn/Zd+NEWjXs/XRFrIRNwTsNI/u+i6Vx/bkPcIxoycyeO4pFPzeW+q2by2Itb+NKandHFU3QpOUATR8U1+ZDKlM/Xr5vN6rsuKqlYHWvCyHL++uOzefPzF3HjzHHdl6tzbddi6ClY4gZrIZPnkzPG8cbdC7njY2dQU8h3XhNi5viRLL/1An5w07kQEoVrGCv9n7i4LwgBw/f/dB7XnTsx7tEUnQH+27kN7J9+Cku/+xr/um4/lKeG5bEtbWFJsuVCPjZhJBv+4uJhGatjnVKd5ju3XsDDH5/ZfT3N4beLqC0sSa5swJ/NncA//slcaofB7l9f+AaWXjqNMSPKWfJvv4+ileDpG0NNW1iSPBY4kuWLi6bxxM3nKVa9uOn8yfzktvnRDHkXznIYIgqWJIuNJoE+fsMcvnDlmXGPJtH+YPo41t75kWhC7jCJloIlyWGBwPL4J2Zx+8IpcY/GCR85fQw/XHJu97SHuEdTeAqWJEd7NorVRWfEPRKnXDlrPP909ZmQDeIeSsEpWJIMXQEPXT+b2xcqVgNx9x9M4/9cOBky+biHUlAKlsQvG3DPx07nrkumxj0Sp9139SwuOWN097y10qRgSbxyIdfNGMuXPj477pE4b3RlmkeunxOtolqix7MULIlPaKkZUcY3Pn1eopeCccnsU2v48uXTIV+ax7MULImHBfIhP771fOqqirAK6TDyvxdN54zRlSU51UHBknjkQ7502VTOnzw67pGUnDLP8NC1sxQskSGRD7n4tFruuXJm3CMpWYvOmsBlk2uj41klRMGS4rIWPI9Hrp9DWoetCqbcN9x7xZnQVVrHshQsKa6ugK8s+hBnn1oT90hK3sIPjeWPZtSV1FaWgiVFY62F6jLu+sPpcQ9lWCjzDbctOK2kFv1TsKRo8ha+e9McyjSFoWj+eN7EaLG/Elk7S8GSohldXc4n5w3vRfji8DcXnx5dOqwEKFhSNJ6Bcl39pegWnz2heysr7pEMnn57RErcnImjuGz8iJKYl6VgiQwD1849tSQOvitYIsPA4ln1JbH2u4IlMgzU1VSwYGKN87uFCpbIMFBbnmLx1DHOr5WlYIkME7OnjI0mwzlMwRIZJi6eOtb503QULJFhYlRFigmOH8dSsESGkZumjXF6K0vBEhlGFkwe7fR5hboGuJSU/e05Nuxr4+DhDB1dAYfbOghyAWAAi/E8RtRUUlNdxvT6Gs4ZPyLuIRfVuLpqSPvRaToOTstSsMRZ+9uzbNrdwtpth/h/W5t4ZVtTdPEF34tejMb0/qK0RFsZ3btGZ04Zzec/fCoXzqjnrPEji/lXKLrT66oZW+bRmO2JuFsULHFKZz5k055WHnxpG798u5ktbdlobpHvQYUP+P2+z417D/OZ/9iAqdrKtZNr+YvLpvHRD40d+sEnwKTaChoqUjR2BS72SsESd6xav4+vvbyNFVuawDfRqSa+Ab//kTpO933YfMgPtxzih5sP8fmPTOK+xbNK8oo+48dU80ZLBheLpYPukni/39vGxQ+tZvE3fsWK7c1Q7kPKG/pz4wzR/aY8Hly7k4a/e5GXtjYO7WMkwHmTa52d2qBgSWIFwKMvbuGcB1fzs3daoSod7foVmgHKfLoyeS59bC3/tWF/4R+ziM6pH+ns1AYFSxLrtuW/YemKjdFvaRwL/3kGUh6XP/kbXtx0oPiPXyDTx1Y5u5ifgiWJk8mH/NFjv+DJV3dDmR+92xcXz4C1XPf0a7zd1BHfOIZQZUUaKtxcgVTBkkTJhZZPPfEKL2w9FL2oksAztGTyXPvEK66fOwxARVmKsVVpXCyWgiWJ8lf/sY4fbWqMtqySJOXxuz2HeWL1trhHMmiVZSkmVWoLS2RQfrJxP195eXs8x6v6Iu1xx8pNHHb8asojK1JMqi5TsEQG6mB7lsuWvx5NWUjq9CBjIBvw0I83xT2SQalMeYyrcPNahQqWJMI//Ncm6Mgmf93xtMfXf7OHA4e74h7JoIwsT9gudx8pWBK7LQcO88Aru6KTcpPOM+xu6uClzW5Pc6iprdQWlshA/P0LmyGbT+6u4InSHk//amfcoxgUz/d0DEukv3Y0d/K9Nw8m90B7bzzDz/ceYfPB9rhHMmCT6tycPOrQb4mUopfX7+VIZy7eyaH9ZQwt7Vm27GqOeyQDVuZ72iUU6a/71+x0a+uqh2f49w0H4x7FgKWKcU5mAbg5aikJ25o62LGzJfnvDPbG9/jWG3vjHsWATR9b7eSKDQqWxOaljQeSN6O9rwzQnmVnaybukQyIg60CFCyJiQV++9ahaPE8V/keb+xujXsUA+JorxQsiUdTe5YVO1vd3B3s4Rt27WuLexQDMrG23MlqKVgSi86uHG8f6nA7WJ5hx8EjcY9iQEZVpvUuoUhfbdx/BPJh3MMYHGNY39RJp4N/DwdbBShYEpOf72h2+/gVgIE3mjrpyrm9eoNLFCyJxfYDR9zeHQQwhl1HsgSBe1tYrlKwJBatrZ1uzW7vjQEUrKJSsKTo2nMhjRmHTnb+IMawo7kz7lEMGwqWFF1rJkdTrkS2Sgx0ZHUMq1gULCm6I115mnJuXir9PTzDxgNuTm1wkYIlRdfZlWd/LqQ0igWBq3MEHKRgSdFlsoH7c7B6GOjULmHRKFhSdK6/OXgcY9ilg+5Fo2CJDFJJBTjhFCyJh17kMgAKlhRdPhdA3ipa0m8KlhRdrisHOv9OBkDBkuIzRltXMiAKlsggBa6uN+wgBUtkMDxoPuTu9Qldo2CJDIr2bYtJwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZTgbLM3GPoH+MKeyAC33/Q82t0ZYm115DPVJxD6DfjKE9kwcgtDGPpQ9SvkdnNl+4V6lnaM/kSKc8rCvPRy4AxyL7QQJrsdbSmQ3iHkqfeIboNeTgz8CwbKUDv+YnaM/hxKuzR8qDigL+2+Da85H2odyPexRDJ7DQmYt7FP1jDFSn4x5Fv7m3hQVOPtEFpecjXr6BEWVxj2JYcPIYlogMTwqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGR5CPewwiIicX5PHIZZxcKlVEhhFjIJfBI5eNeygiIieXy+KR63JrPXARGX6shVwXHl2dELpxtQ8RGabCALo68bAhZNp1HEtEksmYqFE2xMN40NGm3UIRSSZro0YZDw/IkM1qK0tEkqdn6yqbBch4YDfjGWg7pK0sEUkWa6M2eQawmz0w2zAe5HPQ3qKtLBFJBmOiJuVzYDzAbPOAXRgTfbHtEOSyipaIxMuYqEVth3i3T7DLA/sjgnwGDFigeV/3NAdFS0TiYKIGNe+LmoQhapT9UVSlmx/dg2EC1kb7jOWVUDcBRUtEis/Cob3Q1Xl068qyl6c+d2q0WoO1P8Tzo9saE92wab92DUWkuIyJ2tMTKwDPjxrFu8vLeM8Q5DvevYExkDkCjbshDBUuESksY6LWNO6O2nNsi4J8B3jPQE+wnv7zn4NdhfGPuQMvqlzjLsh0dB+lFxEZYsaLGtO4q3vL6pjWGB+wq6JGHbuAX87eR5jnuONWxkRvKTbthbaD0fEtbW2JyFAwpnue1cGoMfncCX0xEOajNnU7ukm17rkm5lx1Cp5//nETSHvuoKszmnEKUFbZ/XnFS0T6wxxtR3sLtBw4epbNiRtD0bGrx3jmrqeP+e4T3PzIOjz/rPddwaFnK2vEKCivgnR5dMfYo18XEYFjItQ9VSHXBV0dcKTlg/fYPB/CYD1PLZ197KdT730A727C4HsYbyw2fP8BHG6OHtRPRdEqK4dUefRnERGAIA/5Lsh2RbEK8kdD9X6xMh6EQSPGu/s9X+r1Gz798P8A7wk8TJ+2mN69jX13Q0tEJCrMMe/4nfT2BkIshLfw9F1P9np3vbr50U9i7Q/wPNPrlpaIyFAyHoShxZjreOpz/97bTfzePgnAG6s2cvaV+4AL8f1KHZsSkYLxfAjDJkL7eZYvXf5+Nzv5NtqSRxfh2W/g+VMIQ7TPJyJDx4DnQRhsJzR3sPxzL5zk1n108yNPA0u6S4jCJSID926oAJbz1NJP9+W7+j59/amln8YL5hMGPwYb4KU0iVRE+scY8FKADQiDH+MF8/saKxjozM8/fXgxofkzDJcAo/BTfrTSQ6h5WCJylDHRwfTonMAAaMHyEp79Nv9818p+392gB7TkqzfhhwuwdhqW0/C8GYqWiHSf0LwJw9sYs4XAW8vyP39mMHf5/wE/pJZJKs/o/AAAAABJRU5ErkJggg==" }</t>
+  </si>
+  <si>
+    <t>status=200||mediaId=(OPQA-5252_mediaId)||entityId=(SYS_USER1)||entityType=profile||mediaType=image/png||context=1p-profile</t>
+  </si>
+  <si>
+    <t>{ "mediaId": "(OPQA-5252_mediaId)", "base64Media": "data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAASwAAAEsCAYAAAB5fY51AAAABHNCSVQICAgIfAhkiAAAGYBJREFUeJzt3XuYFOWB7/HvW9U9V5gBBhxwAMVwEURBohgMRt2V9YKa5OhuPErcs15iPBv0PDlnZXWfk8c8m82um2fd9RKT+CTGVUyyu8nZTQRW18RoCCExxmgCchdE7gxzg5np6e6q9/xRM3JxlLl1V709v8/zjD7M9HS/9Ex/qap+6y3DYHzm2SpqU0vwgrngTcPaGXhmEtYO6m5FpAQYA6F9B2M2QbiF0H+d1vxyHr+mY8B3OaDvumfV9Rh7J5h5WFtLKm2wIdGHYiUi3YwB40Uf+ZzFmFawr2HN1/j7q77f77vr162XrboGa+/FMwvwfAgDBUpE+s4Y3m1HaNdizN/ywFXP9vnb+/xAy1Y8h192OTaEMAQUKhEZKANe95ZXkH2eB66+oo/fdRJ/ueoWLF/GT9UT5AY9TBGR4/hpCPL7MdzH3131xAfd9IODtWzl/cC9eH4ZYTCEIxQROUa0m5gF/pYHFt//fjfz3/cOlq34Aqmy+7HWx4YFGKGISDdrwRifVPoSLvyUZc13Xu7tZr0Ha9nK+0mV3U8+j45ViUjRhBZS6Uu58AbDmu+8dOKX37tL+JerbsHar2FMmd4BFJGiMwaszWLMnSce0/Lec2PLl/F8xUpE4mEtUYP48olfOj5Yy1Y8h5+q1wF2EYlVGICfqmfZiueO/fTRYC1bdQ1+2eWauiAiiRDkwC+7nGWrrun51NFgWXuv3g0UkUSJTve7t+ePUbDuWXU9nlkQzWAXEUmIMATPLOCeVddDT7CMvRPPR1MYRCRZbDSp1Ng7AQyfebaK0f5uDKP0zqCIJI4xYGmhOWhIUZtagg1r4x6TiEivrAVLLbWpJR5eMJdUemDrYomIFEMqbfCCuV60UqgOtotIgtkQ8KZ5WDtDwRKRRIumN8zwtAa7iCSeteCZSZ5iJSJOsLaXk59FRBJKwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOCMV9wBiYYHQHv3obdVVzxz/ISKxGz7BCkLIW8iHkPY597RRXDapltnjqjhlRNlxzfIMbG3qZP3BDla83cI7u9sACykPfA98BUwkDqUdrLA7UBhuPGscl8wYx8IZ9cwcV33Sb728+/+Pdf//17taeWndHlZuauTlHS1R1VImuiqtiBSFYdnK0rsKhQWyAWefUs31cyZw8/zJNNRVkR6CuHTkArYdOMJjP3uL7755gNaOLKT9wY9ZRE6q9IKVC8EzPHzVDG6YP5lx1WUFe6hNB47w+Oq3eHD1jiha2lUUKajSCVZooTPP0oWn8VeLZ1E/onChOtGGA0e44zuvsXpHC5SnQN0SKYjSCFY+5JTqMpb/9zksOrM+liEEFh57aSt3Pbe556KPsYxDpJS5Pw8rF3LpxBrWfO7C2GIF0d7g0kun8svPXhC9kxi6/++ASNK4HayugKun17Fq6UKmjhsR92gAuGBKHTuXXUJFVbr7HUoRGSruBisXcPWZY3n2jgVU+Mn6a0waVcmW/3URM8dWK1oiQyhZr/S+yoV8csY4/u3WC+IeyfuaOKqS5z5zAQ21Fdo9FBki7gUrsMypq+SbS+ZRkUr28CePqeL52+ZDNojmhonIoCT7FX8iC1jLv95+AWOqijdtYTDOmlDDM0vmatdQZAi4FaxswLc+MYvpCTnA3lc3njeZz86bEG1piciAuROsIOTchhpuWXhG3CMZkHuvmgXVZb2vDCEifeJGsCzgeXztutlxj2TAJo+u5FtXTIcubWWJDJQbwcqH3H52PRdMqYt7JINyy0enwMhyvWsoMkBuBItoFnkp+PYV06PzeESk35IfrCDk41PHMGNCTdwjGRKLzp5AQ3Vax7JEBiD5wcqF3PiRyZSVyMnEDTUVXHNWfbT6qYj0S/KDFcJVs0+NexRDasmHG7RbKDIAyQ5WYDl/6hhGpJM9zP6aWl/DpLFVOvgu0k/JLkE+5H/OnRD3KIZc/chyrplUo2CJ9FOyg5XymDJ+ZNyjKIgppypYIv2V3GBZqC73GVtTGfdICuKM+pEKlkg/JTdYWCaW+4yvLc1gTT9FwRLpr+QGy8L48hR1laV56cRZ9SP0TqFIPyU3WJT4ElIl/ZcTKYxEB0tE5FgKlog4Q8ESEWckOli2hA/0hNbqCtEi/ZTcYBk42BXQ1JmPeyQFsfFgu64OLdJPyQ0Whm2ZgF0tHXEPpCDe3NemYIn0U3KDZSCXDWhqy8Q9koJ4e/9hBUukn5IbLIB8yNa9bXGPoiDe2qstLJH+Snaw0h7/9NqeuEcx5Pa2Zfj+zjbwFSyR/kh2sDzD+u3NtGRK68D7pr1tNDZ1gFGwRPoj2cEC8A0rf19aW1nLf7MLUsl/6kWSJvmvmrTPd3/9Dl1BaVzq/Z3WDCs3HtTuoMgAJD9YvmHllibW7W6NeyRDYuXru9nXntPuoMgAJD9YAL7h4Re3xj2KQQuBO5/fDCnFSmQgHAmWx1NvHmDttsa4RzIo3/zZNujQ1pXIQLkRLANYuOFf3nD27MJtje3csWozlJfmgoQixeBGsAB8w87GDh75yea4R9JvIfDFZ9dDLtAJzyKD4E6wANI+d6/azO/2uDX7/clfbOfpdQegxK6vKFJsbr2CDOAbrvvmrzh4pCvu0fTJb99p5tbv/U7zrkSGgHuvIs+wta2LTz3xCm1dyZ4Bv2n/YeY9/gpUpLQrKDIE3AsWQMrjp2+3cu3jv6QroVee2bT/MJd/8xXI5HSSs8gQcTNYAGmPl7c3s/jrv6Ajl6xZ8G8daufMr/6Ct1s6wXf3KRZJGrdfTWU+P9nezPyv/JTf70nGTPgXN+7nQ3/zImTyipXIEHP/FZXyWN/cyfyvruX7r+2K7WLK7dmAv171Jn/4xKvRu4HaDRQZcu4HC8D3yOQD/vjJ17h9+avsai3uKqW/3d3KJQ+t5gsvbItmsWsmu0hBGJatTOZR64HKh9AV8MUrpnHrRWfQUFNRsId6fVcrD/10K0+u3QkjyrRVJVJgpResHtmAhppyrjurntsWnMbU8TVUDsFcqObOHBv2tPLgT7fxg7eaIBtojpVIkZRusACsjba4rOHaqaNZOHUsF59Zz/zJo7D0bWqUBXJByItbGln95j5eeKuJX+8+HK1n5XuaXyVSRKUdrGMFFoIwCljKZ3ZDDRc3jGRmXRVjq9LHnVTtGdjenGFjUwfP7Wpj394jUZhSXhQq7fqJxGL4LB3gG/B9KPPBwrr9h1m3tw1CS69LQHhEB889A1XD52kSSbLh+Uo0HI2RiDhDR4tFxBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnDM9zCUWOZbv/Y0/480mZ45cXMr18ToaUgiXDiyVaJy3s/ggslKcYU5VmYkWK+ooUI9IedeWpD0yWATJByN6OPIG17O7MczAb0JLJQ2c+OrH+3Y/u71DIBk3BktIXdi/k6BlIe0yqLOPC00ZzXkMNH508iurKMqoq01SXpxhZkaYi5ZHqY1wOZwNCC22dWTK5gM6uPJnOHBsb21mzs4WNB9tZv+8wh3Ih5MIoln73umrSb24u4NeeI7bL4wxE2ouu/lworjwfnoHqdOEfxwJhCPloK+rDp49iyaxTmDl5NHMmjWb8iLLCj+EEGw62s3VvK5v3tPK9TY28+lbz8YtC6sIlfeJesNpztD5wJdUVaaxN/tBTvsfPN+zjom+8Uphotefo/IerSae8RD8fnjG0tHdRd9/zhYtWz5ZU2ufGqWNYMH0cN54/iTFVxQ/UybRm8vznm/tYs2E/j25shMNd3ZeH07LbH8S9XUJrSac8fM/gyk825Xt9O4Y7EKE7z0c6VaDnoTtUM8dUcu3Z4/nsR0+nYUw16QQv0FhbkeKGeRO5Yd5ElrV08uqOJr6+ZgfPv9Ma7Tqm9QZ+b9wLFtFhAKcUeMDRllVyX5w9hvxpCC10BYyoq+LbV05n0TmnUlvu3q/0xFGVTJzbwCfmNvD6rha+tWYHj659JzpYn/Zd+NEWjXs/XRFrIRNwTsNI/u+i6Vx/bkPcIxoycyeO4pFPzeW+q2by2Itb+NKandHFU3QpOUATR8U1+ZDKlM/Xr5vN6rsuKqlYHWvCyHL++uOzefPzF3HjzHHdl6tzbddi6ClY4gZrIZPnkzPG8cbdC7njY2dQU8h3XhNi5viRLL/1An5w07kQEoVrGCv9n7i4LwgBw/f/dB7XnTsx7tEUnQH+27kN7J9+Cku/+xr/um4/lKeG5bEtbWFJsuVCPjZhJBv+4uJhGatjnVKd5ju3XsDDH5/ZfT3N4beLqC0sSa5swJ/NncA//slcaofB7l9f+AaWXjqNMSPKWfJvv4+ileDpG0NNW1iSPBY4kuWLi6bxxM3nKVa9uOn8yfzktvnRDHkXznIYIgqWJIuNJoE+fsMcvnDlmXGPJtH+YPo41t75kWhC7jCJloIlyWGBwPL4J2Zx+8IpcY/GCR85fQw/XHJu97SHuEdTeAqWJEd7NorVRWfEPRKnXDlrPP909ZmQDeIeSsEpWJIMXQEPXT+b2xcqVgNx9x9M4/9cOBky+biHUlAKlsQvG3DPx07nrkumxj0Sp9139SwuOWN097y10qRgSbxyIdfNGMuXPj477pE4b3RlmkeunxOtolqix7MULIlPaKkZUcY3Pn1eopeCccnsU2v48uXTIV+ax7MULImHBfIhP771fOqqirAK6TDyvxdN54zRlSU51UHBknjkQ7502VTOnzw67pGUnDLP8NC1sxQskSGRD7n4tFruuXJm3CMpWYvOmsBlk2uj41klRMGS4rIWPI9Hrp9DWoetCqbcN9x7xZnQVVrHshQsKa6ugK8s+hBnn1oT90hK3sIPjeWPZtSV1FaWgiVFY62F6jLu+sPpcQ9lWCjzDbctOK2kFv1TsKRo8ha+e9McyjSFoWj+eN7EaLG/Elk7S8GSohldXc4n5w3vRfji8DcXnx5dOqwEKFhSNJ6Bcl39pegWnz2heysr7pEMnn57RErcnImjuGz8iJKYl6VgiQwD1849tSQOvitYIsPA4ln1JbH2u4IlMgzU1VSwYGKN87uFCpbIMFBbnmLx1DHOr5WlYIkME7OnjI0mwzlMwRIZJi6eOtb503QULJFhYlRFigmOH8dSsESGkZumjXF6K0vBEhlGFkwe7fR5hboGuJSU/e05Nuxr4+DhDB1dAYfbOghyAWAAi/E8RtRUUlNdxvT6Gs4ZPyLuIRfVuLpqSPvRaToOTstSsMRZ+9uzbNrdwtpth/h/W5t4ZVtTdPEF34tejMb0/qK0RFsZ3btGZ04Zzec/fCoXzqjnrPEji/lXKLrT66oZW+bRmO2JuFsULHFKZz5k055WHnxpG798u5ktbdlobpHvQYUP+P2+z417D/OZ/9iAqdrKtZNr+YvLpvHRD40d+sEnwKTaChoqUjR2BS72SsESd6xav4+vvbyNFVuawDfRqSa+Ab//kTpO933YfMgPtxzih5sP8fmPTOK+xbNK8oo+48dU80ZLBheLpYPukni/39vGxQ+tZvE3fsWK7c1Q7kPKG/pz4wzR/aY8Hly7k4a/e5GXtjYO7WMkwHmTa52d2qBgSWIFwKMvbuGcB1fzs3daoSod7foVmgHKfLoyeS59bC3/tWF/4R+ziM6pH+ns1AYFSxLrtuW/YemKjdFvaRwL/3kGUh6XP/kbXtx0oPiPXyDTx1Y5u5ifgiWJk8mH/NFjv+DJV3dDmR+92xcXz4C1XPf0a7zd1BHfOIZQZUUaKtxcgVTBkkTJhZZPPfEKL2w9FL2oksAztGTyXPvEK66fOwxARVmKsVVpXCyWgiWJ8lf/sY4fbWqMtqySJOXxuz2HeWL1trhHMmiVZSkmVWoLS2RQfrJxP195eXs8x6v6Iu1xx8pNHHb8asojK1JMqi5TsEQG6mB7lsuWvx5NWUjq9CBjIBvw0I83xT2SQalMeYyrcPNahQqWJMI//Ncm6Mgmf93xtMfXf7OHA4e74h7JoIwsT9gudx8pWBK7LQcO88Aru6KTcpPOM+xu6uClzW5Pc6iprdQWlshA/P0LmyGbT+6u4InSHk//amfcoxgUz/d0DEukv3Y0d/K9Nw8m90B7bzzDz/ceYfPB9rhHMmCT6tycPOrQb4mUopfX7+VIZy7eyaH9ZQwt7Vm27GqOeyQDVuZ72iUU6a/71+x0a+uqh2f49w0H4x7FgKWKcU5mAbg5aikJ25o62LGzJfnvDPbG9/jWG3vjHsWATR9b7eSKDQqWxOaljQeSN6O9rwzQnmVnaybukQyIg60CFCyJiQV++9ahaPE8V/keb+xujXsUA+JorxQsiUdTe5YVO1vd3B3s4Rt27WuLexQDMrG23MlqKVgSi86uHG8f6nA7WJ5hx8EjcY9iQEZVpvUuoUhfbdx/BPJh3MMYHGNY39RJp4N/DwdbBShYEpOf72h2+/gVgIE3mjrpyrm9eoNLFCyJxfYDR9zeHQQwhl1HsgSBe1tYrlKwJBatrZ1uzW7vjQEUrKJSsKTo2nMhjRmHTnb+IMawo7kz7lEMGwqWFF1rJkdTrkS2Sgx0ZHUMq1gULCm6I115mnJuXir9PTzDxgNuTm1wkYIlRdfZlWd/LqQ0igWBq3MEHKRgSdFlsoH7c7B6GOjULmHRKFhSdK6/OXgcY9ilg+5Fo2CJDFJJBTjhFCyJh17kMgAKlhRdPhdA3ipa0m8KlhRdrisHOv9OBkDBkuIzRltXMiAKlsggBa6uN+wgBUtkMDxoPuTu9Qldo2CJDIr2bYtJwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZTgbLM3GPoH+MKeyAC33/Q82t0ZYm115DPVJxD6DfjKE9kwcgtDGPpQ9SvkdnNl+4V6lnaM/kSKc8rCvPRy4AxyL7QQJrsdbSmQ3iHkqfeIboNeTgz8CwbKUDv+YnaM/hxKuzR8qDigL+2+Da85H2odyPexRDJ7DQmYt7FP1jDFSn4x5Fv7m3hQVOPtEFpecjXr6BEWVxj2JYcPIYlogMTwqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGR5CPewwiIicX5PHIZZxcKlVEhhFjIJfBI5eNeygiIieXy+KR63JrPXARGX6shVwXHl2dELpxtQ8RGabCALo68bAhZNp1HEtEksmYqFE2xMN40NGm3UIRSSZro0YZDw/IkM1qK0tEkqdn6yqbBch4YDfjGWg7pK0sEUkWa6M2eQawmz0w2zAe5HPQ3qKtLBFJBmOiJuVzYDzAbPOAXRgTfbHtEOSyipaIxMuYqEVth3i3T7DLA/sjgnwGDFigeV/3NAdFS0TiYKIGNe+LmoQhapT9UVSlmx/dg2EC1kb7jOWVUDcBRUtEis/Cob3Q1Xl068qyl6c+d2q0WoO1P8Tzo9saE92wab92DUWkuIyJ2tMTKwDPjxrFu8vLeM8Q5DvevYExkDkCjbshDBUuESksY6LWNO6O2nNsi4J8B3jPQE+wnv7zn4NdhfGPuQMvqlzjLsh0dB+lFxEZYsaLGtO4q3vL6pjWGB+wq6JGHbuAX87eR5jnuONWxkRvKTbthbaD0fEtbW2JyFAwpnue1cGoMfncCX0xEOajNnU7ukm17rkm5lx1Cp5//nETSHvuoKszmnEKUFbZ/XnFS0T6wxxtR3sLtBw4epbNiRtD0bGrx3jmrqeP+e4T3PzIOjz/rPddwaFnK2vEKCivgnR5dMfYo18XEYFjItQ9VSHXBV0dcKTlg/fYPB/CYD1PLZ197KdT730A727C4HsYbyw2fP8BHG6OHtRPRdEqK4dUefRnERGAIA/5Lsh2RbEK8kdD9X6xMh6EQSPGu/s9X+r1Gz798P8A7wk8TJ+2mN69jX13Q0tEJCrMMe/4nfT2BkIshLfw9F1P9np3vbr50U9i7Q/wPNPrlpaIyFAyHoShxZjreOpz/97bTfzePgnAG6s2cvaV+4AL8f1KHZsSkYLxfAjDJkL7eZYvXf5+Nzv5NtqSRxfh2W/g+VMIQ7TPJyJDx4DnQRhsJzR3sPxzL5zk1n108yNPA0u6S4jCJSID926oAJbz1NJP9+W7+j59/amln8YL5hMGPwYb4KU0iVRE+scY8FKADQiDH+MF8/saKxjozM8/fXgxofkzDJcAo/BTfrTSQ6h5WCJylDHRwfTonMAAaMHyEp79Nv9818p+392gB7TkqzfhhwuwdhqW0/C8GYqWiHSf0LwJw9sYs4XAW8vyP39mMHf5/wE/pJZJKs/o/AAAAABJRU5ErkJggg==" }</t>
+  </si>
+  <si>
+    <t>/media/(OPQA-5252_mediaId)</t>
+  </si>
+  <si>
+    <t>/media/(OPQA-5252_mediaId)A</t>
+  </si>
+  <si>
+    <t>/internal/media/(OPQA-5252_mediaId)</t>
+  </si>
+  <si>
+    <t>/internal/media/(OPQA-5252_mediaId)A</t>
+  </si>
+  <si>
+    <t>OPQA-5253</t>
+  </si>
+  <si>
+    <t>{ "mediaId": "(OPQA-5253_mediaId)", "mediaType" : "image/png", "base64Media": "data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAASwAAAEsCAYAAAB5fY51AAAABHNCSVQICAgIfAhkiAAAGYBJREFUeJzt3XuYFOWB7/HvW9U9V5gBBhxwAMVwEURBohgMRt2V9YKa5OhuPErcs15iPBv0PDlnZXWfk8c8m82um2fd9RKT+CTGVUyyu8nZTQRW18RoCCExxmgCchdE7gxzg5np6e6q9/xRM3JxlLl1V709v8/zjD7M9HS/9Ex/qap+6y3DYHzm2SpqU0vwgrngTcPaGXhmEtYO6m5FpAQYA6F9B2M2QbiF0H+d1vxyHr+mY8B3OaDvumfV9Rh7J5h5WFtLKm2wIdGHYiUi3YwB40Uf+ZzFmFawr2HN1/j7q77f77vr162XrboGa+/FMwvwfAgDBUpE+s4Y3m1HaNdizN/ywFXP9vnb+/xAy1Y8h192OTaEMAQUKhEZKANe95ZXkH2eB66+oo/fdRJ/ueoWLF/GT9UT5AY9TBGR4/hpCPL7MdzH3131xAfd9IODtWzl/cC9eH4ZYTCEIxQROUa0m5gF/pYHFt//fjfz3/cOlq34Aqmy+7HWx4YFGKGISDdrwRifVPoSLvyUZc13Xu7tZr0Ha9nK+0mV3U8+j45ViUjRhBZS6Uu58AbDmu+8dOKX37tL+JerbsHar2FMmd4BFJGiMwaszWLMnSce0/Lec2PLl/F8xUpE4mEtUYP48olfOj5Yy1Y8h5+q1wF2EYlVGICfqmfZiueO/fTRYC1bdQ1+2eWauiAiiRDkwC+7nGWrrun51NFgWXuv3g0UkUSJTve7t+ePUbDuWXU9nlkQzWAXEUmIMATPLOCeVddDT7CMvRPPR1MYRCRZbDSp1Ng7AQyfebaK0f5uDKP0zqCIJI4xYGmhOWhIUZtagg1r4x6TiEivrAVLLbWpJR5eMJdUemDrYomIFEMqbfCCuV60UqgOtotIgtkQ8KZ5WDtDwRKRRIumN8zwtAa7iCSeteCZSZ5iJSJOsLaXk59FRBJKwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOCMV9wBiYYHQHv3obdVVzxz/ISKxGz7BCkLIW8iHkPY597RRXDapltnjqjhlRNlxzfIMbG3qZP3BDla83cI7u9sACykPfA98BUwkDqUdrLA7UBhuPGscl8wYx8IZ9cwcV33Sb728+/+Pdf//17taeWndHlZuauTlHS1R1VImuiqtiBSFYdnK0rsKhQWyAWefUs31cyZw8/zJNNRVkR6CuHTkArYdOMJjP3uL7755gNaOLKT9wY9ZRE6q9IKVC8EzPHzVDG6YP5lx1WUFe6hNB47w+Oq3eHD1jiha2lUUKajSCVZooTPP0oWn8VeLZ1E/onChOtGGA0e44zuvsXpHC5SnQN0SKYjSCFY+5JTqMpb/9zksOrM+liEEFh57aSt3Pbe556KPsYxDpJS5Pw8rF3LpxBrWfO7C2GIF0d7g0kun8svPXhC9kxi6/++ASNK4HayugKun17Fq6UKmjhsR92gAuGBKHTuXXUJFVbr7HUoRGSruBisXcPWZY3n2jgVU+Mn6a0waVcmW/3URM8dWK1oiQyhZr/S+yoV8csY4/u3WC+IeyfuaOKqS5z5zAQ21Fdo9FBki7gUrsMypq+SbS+ZRkUr28CePqeL52+ZDNojmhonIoCT7FX8iC1jLv95+AWOqijdtYTDOmlDDM0vmatdQZAi4FaxswLc+MYvpCTnA3lc3njeZz86bEG1piciAuROsIOTchhpuWXhG3CMZkHuvmgXVZb2vDCEifeJGsCzgeXztutlxj2TAJo+u5FtXTIcubWWJDJQbwcqH3H52PRdMqYt7JINyy0enwMhyvWsoMkBuBItoFnkp+PYV06PzeESk35IfrCDk41PHMGNCTdwjGRKLzp5AQ3Vax7JEBiD5wcqF3PiRyZSVyMnEDTUVXHNWfbT6qYj0S/KDFcJVs0+NexRDasmHG7RbKDIAyQ5WYDl/6hhGpJM9zP6aWl/DpLFVOvgu0k/JLkE+5H/OnRD3KIZc/chyrplUo2CJ9FOyg5XymDJ+ZNyjKIgppypYIv2V3GBZqC73GVtTGfdICuKM+pEKlkg/JTdYWCaW+4yvLc1gTT9FwRLpr+QGy8L48hR1laV56cRZ9SP0TqFIPyU3WJT4ElIl/ZcTKYxEB0tE5FgKlog4Q8ESEWckOli2hA/0hNbqCtEi/ZTcYBk42BXQ1JmPeyQFsfFgu64OLdJPyQ0Whm2ZgF0tHXEPpCDe3NemYIn0U3KDZSCXDWhqy8Q9koJ4e/9hBUukn5IbLIB8yNa9bXGPoiDe2qstLJH+Snaw0h7/9NqeuEcx5Pa2Zfj+zjbwFSyR/kh2sDzD+u3NtGRK68D7pr1tNDZ1gFGwRPoj2cEC8A0rf19aW1nLf7MLUsl/6kWSJvmvmrTPd3/9Dl1BaVzq/Z3WDCs3HtTuoMgAJD9YvmHllibW7W6NeyRDYuXru9nXntPuoMgAJD9YAL7h4Re3xj2KQQuBO5/fDCnFSmQgHAmWx1NvHmDttsa4RzIo3/zZNujQ1pXIQLkRLANYuOFf3nD27MJtje3csWozlJfmgoQixeBGsAB8w87GDh75yea4R9JvIfDFZ9dDLtAJzyKD4E6wANI+d6/azO/2uDX7/clfbOfpdQegxK6vKFJsbr2CDOAbrvvmrzh4pCvu0fTJb99p5tbv/U7zrkSGgHuvIs+wta2LTz3xCm1dyZ4Bv2n/YeY9/gpUpLQrKDIE3AsWQMrjp2+3cu3jv6QroVee2bT/MJd/8xXI5HSSs8gQcTNYAGmPl7c3s/jrv6Ajl6xZ8G8daufMr/6Ct1s6wXf3KRZJGrdfTWU+P9nezPyv/JTf70nGTPgXN+7nQ3/zImTyipXIEHP/FZXyWN/cyfyvruX7r+2K7WLK7dmAv171Jn/4xKvRu4HaDRQZcu4HC8D3yOQD/vjJ17h9+avsai3uKqW/3d3KJQ+t5gsvbItmsWsmu0hBGJatTOZR64HKh9AV8MUrpnHrRWfQUFNRsId6fVcrD/10K0+u3QkjyrRVJVJgpResHtmAhppyrjurntsWnMbU8TVUDsFcqObOHBv2tPLgT7fxg7eaIBtojpVIkZRusACsjba4rOHaqaNZOHUsF59Zz/zJo7D0bWqUBXJByItbGln95j5eeKuJX+8+HK1n5XuaXyVSRKUdrGMFFoIwCljKZ3ZDDRc3jGRmXRVjq9LHnVTtGdjenGFjUwfP7Wpj394jUZhSXhQq7fqJxGL4LB3gG/B9KPPBwrr9h1m3tw1CS69LQHhEB889A1XD52kSSbLh+Uo0HI2RiDhDR4tFxBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnDM9zCUWOZbv/Y0/480mZ45cXMr18ToaUgiXDiyVaJy3s/ggslKcYU5VmYkWK+ooUI9IedeWpD0yWATJByN6OPIG17O7MczAb0JLJQ2c+OrH+3Y/u71DIBk3BktIXdi/k6BlIe0yqLOPC00ZzXkMNH508iurKMqoq01SXpxhZkaYi5ZHqY1wOZwNCC22dWTK5gM6uPJnOHBsb21mzs4WNB9tZv+8wh3Ih5MIoln73umrSb24u4NeeI7bL4wxE2ouu/lworjwfnoHqdOEfxwJhCPloK+rDp49iyaxTmDl5NHMmjWb8iLLCj+EEGw62s3VvK5v3tPK9TY28+lbz8YtC6sIlfeJesNpztD5wJdUVaaxN/tBTvsfPN+zjom+8Uphotefo/IerSae8RD8fnjG0tHdRd9/zhYtWz5ZU2ufGqWNYMH0cN54/iTFVxQ/UybRm8vznm/tYs2E/j25shMNd3ZeH07LbH8S9XUJrSac8fM/gyk825Xt9O4Y7EKE7z0c6VaDnoTtUM8dUcu3Z4/nsR0+nYUw16QQv0FhbkeKGeRO5Yd5ElrV08uqOJr6+ZgfPv9Ma7Tqm9QZ+b9wLFtFhAKcUeMDRllVyX5w9hvxpCC10BYyoq+LbV05n0TmnUlvu3q/0xFGVTJzbwCfmNvD6rha+tWYHj659JzpYn/Zd+NEWjXs/XRFrIRNwTsNI/u+i6Vx/bkPcIxoycyeO4pFPzeW+q2by2Itb+NKandHFU3QpOUATR8U1+ZDKlM/Xr5vN6rsuKqlYHWvCyHL++uOzefPzF3HjzHHdl6tzbddi6ClY4gZrIZPnkzPG8cbdC7njY2dQU8h3XhNi5viRLL/1An5w07kQEoVrGCv9n7i4LwgBw/f/dB7XnTsx7tEUnQH+27kN7J9+Cku/+xr/um4/lKeG5bEtbWFJsuVCPjZhJBv+4uJhGatjnVKd5ju3XsDDH5/ZfT3N4beLqC0sSa5swJ/NncA//slcaofB7l9f+AaWXjqNMSPKWfJvv4+ileDpG0NNW1iSPBY4kuWLi6bxxM3nKVa9uOn8yfzktvnRDHkXznIYIgqWJIuNJoE+fsMcvnDlmXGPJtH+YPo41t75kWhC7jCJloIlyWGBwPL4J2Zx+8IpcY/GCR85fQw/XHJu97SHuEdTeAqWJEd7NorVRWfEPRKnXDlrPP909ZmQDeIeSsEpWJIMXQEPXT+b2xcqVgNx9x9M4/9cOBky+biHUlAKlsQvG3DPx07nrkumxj0Sp9139SwuOWN097y10qRgSbxyIdfNGMuXPj477pE4b3RlmkeunxOtolqix7MULIlPaKkZUcY3Pn1eopeCccnsU2v48uXTIV+ax7MULImHBfIhP771fOqqirAK6TDyvxdN54zRlSU51UHBknjkQ7502VTOnzw67pGUnDLP8NC1sxQskSGRD7n4tFruuXJm3CMpWYvOmsBlk2uj41klRMGS4rIWPI9Hrp9DWoetCqbcN9x7xZnQVVrHshQsKa6ugK8s+hBnn1oT90hK3sIPjeWPZtSV1FaWgiVFY62F6jLu+sPpcQ9lWCjzDbctOK2kFv1TsKRo8ha+e9McyjSFoWj+eN7EaLG/Elk7S8GSohldXc4n5w3vRfji8DcXnx5dOqwEKFhSNJ6Bcl39pegWnz2heysr7pEMnn57RErcnImjuGz8iJKYl6VgiQwD1849tSQOvitYIsPA4ln1JbH2u4IlMgzU1VSwYGKN87uFCpbIMFBbnmLx1DHOr5WlYIkME7OnjI0mwzlMwRIZJi6eOtb503QULJFhYlRFigmOH8dSsESGkZumjXF6K0vBEhlGFkwe7fR5hboGuJSU/e05Nuxr4+DhDB1dAYfbOghyAWAAi/E8RtRUUlNdxvT6Gs4ZPyLuIRfVuLpqSPvRaToOTstSsMRZ+9uzbNrdwtpth/h/W5t4ZVtTdPEF34tejMb0/qK0RFsZ3btGZ04Zzec/fCoXzqjnrPEji/lXKLrT66oZW+bRmO2JuFsULHFKZz5k055WHnxpG798u5ktbdlobpHvQYUP+P2+z417D/OZ/9iAqdrKtZNr+YvLpvHRD40d+sEnwKTaChoqUjR2BS72SsESd6xav4+vvbyNFVuawDfRqSa+Ab//kTpO933YfMgPtxzih5sP8fmPTOK+xbNK8oo+48dU80ZLBheLpYPukni/39vGxQ+tZvE3fsWK7c1Q7kPKG/pz4wzR/aY8Hly7k4a/e5GXtjYO7WMkwHmTa52d2qBgSWIFwKMvbuGcB1fzs3daoSod7foVmgHKfLoyeS59bC3/tWF/4R+ziM6pH+ns1AYFSxLrtuW/YemKjdFvaRwL/3kGUh6XP/kbXtx0oPiPXyDTx1Y5u5ifgiWJk8mH/NFjv+DJV3dDmR+92xcXz4C1XPf0a7zd1BHfOIZQZUUaKtxcgVTBkkTJhZZPPfEKL2w9FL2oksAztGTyXPvEK66fOwxARVmKsVVpXCyWgiWJ8lf/sY4fbWqMtqySJOXxuz2HeWL1trhHMmiVZSkmVWoLS2RQfrJxP195eXs8x6v6Iu1xx8pNHHb8asojK1JMqi5TsEQG6mB7lsuWvx5NWUjq9CBjIBvw0I83xT2SQalMeYyrcPNahQqWJMI//Ncm6Mgmf93xtMfXf7OHA4e74h7JoIwsT9gudx8pWBK7LQcO88Aru6KTcpPOM+xu6uClzW5Pc6iprdQWlshA/P0LmyGbT+6u4InSHk//amfcoxgUz/d0DEukv3Y0d/K9Nw8m90B7bzzDz/ceYfPB9rhHMmCT6tycPOrQb4mUopfX7+VIZy7eyaH9ZQwt7Vm27GqOeyQDVuZ72iUU6a/71+x0a+uqh2f49w0H4x7FgKWKcU5mAbg5aikJ25o62LGzJfnvDPbG9/jWG3vjHsWATR9b7eSKDQqWxOaljQeSN6O9rwzQnmVnaybukQyIg60CFCyJiQV++9ahaPE8V/keb+xujXsUA+JorxQsiUdTe5YVO1vd3B3s4Rt27WuLexQDMrG23MlqKVgSi86uHG8f6nA7WJ5hx8EjcY9iQEZVpvUuoUhfbdx/BPJh3MMYHGNY39RJp4N/DwdbBShYEpOf72h2+/gVgIE3mjrpyrm9eoNLFCyJxfYDR9zeHQQwhl1HsgSBe1tYrlKwJBatrZ1uzW7vjQEUrKJSsKTo2nMhjRmHTnb+IMawo7kz7lEMGwqWFF1rJkdTrkS2Sgx0ZHUMq1gULCm6I115mnJuXir9PTzDxgNuTm1wkYIlRdfZlWd/LqQ0igWBq3MEHKRgSdFlsoH7c7B6GOjULmHRKFhSdK6/OXgcY9ilg+5Fo2CJDFJJBTjhFCyJh17kMgAKlhRdPhdA3ipa0m8KlhRdrisHOv9OBkDBkuIzRltXMiAKlsggBa6uN+wgBUtkMDxoPuTu9Qldo2CJDIr2bYtJwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZCpaIOEPBEhFnKFgi4gwFS0ScoWCJiDMULBFxhoIlIs5QsETEGQqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGgiUizlCwRMQZTgbLM3GPoH+MKeyAC33/Q82t0ZYm115DPVJxD6DfjKE9kwcgtDGPpQ9SvkdnNl+4V6lnaM/kSKc8rCvPRy4AxyL7QQJrsdbSmQ3iHkqfeIboNeTgz8CwbKUDv+YnaM/hxKuzR8qDigL+2+Da85H2odyPexRDJ7DQmYt7FP1jDFSn4x5Fv7m3hQVOPtEFpecjXr6BEWVxj2JYcPIYlogMTwqWiDhDwRIRZyhYIuIMBUtEnKFgiYgzFCwRcYaCJSLOULBExBkKlog4Q8ESEWcoWCLiDAVLRJyhYImIMxQsEXGGR5CPewwiIicX5PHIZZxcKlVEhhFjIJfBI5eNeygiIieXy+KR63JrPXARGX6shVwXHl2dELpxtQ8RGabCALo68bAhZNp1HEtEksmYqFE2xMN40NGm3UIRSSZro0YZDw/IkM1qK0tEkqdn6yqbBch4YDfjGWg7pK0sEUkWa6M2eQawmz0w2zAe5HPQ3qKtLBFJBmOiJuVzYDzAbPOAXRgTfbHtEOSyipaIxMuYqEVth3i3T7DLA/sjgnwGDFigeV/3NAdFS0TiYKIGNe+LmoQhapT9UVSlmx/dg2EC1kb7jOWVUDcBRUtEis/Cob3Q1Xl068qyl6c+d2q0WoO1P8Tzo9saE92wab92DUWkuIyJ2tMTKwDPjxrFu8vLeM8Q5DvevYExkDkCjbshDBUuESksY6LWNO6O2nNsi4J8B3jPQE+wnv7zn4NdhfGPuQMvqlzjLsh0dB+lFxEZYsaLGtO4q3vL6pjWGB+wq6JGHbuAX87eR5jnuONWxkRvKTbthbaD0fEtbW2JyFAwpnue1cGoMfncCX0xEOajNnU7ukm17rkm5lx1Cp5//nETSHvuoKszmnEKUFbZ/XnFS0T6wxxtR3sLtBw4epbNiRtD0bGrx3jmrqeP+e4T3PzIOjz/rPddwaFnK2vEKCivgnR5dMfYo18XEYFjItQ9VSHXBV0dcKTlg/fYPB/CYD1PLZ197KdT730A727C4HsYbyw2fP8BHG6OHtRPRdEqK4dUefRnERGAIA/5Lsh2RbEK8kdD9X6xMh6EQSPGu/s9X+r1Gz798P8A7wk8TJ+2mN69jX13Q0tEJCrMMe/4nfT2BkIshLfw9F1P9np3vbr50U9i7Q/wPNPrlpaIyFAyHoShxZjreOpz/97bTfzePgnAG6s2cvaV+4AL8f1KHZsSkYLxfAjDJkL7eZYvXf5+Nzv5NtqSRxfh2W/g+VMIQ7TPJyJDx4DnQRhsJzR3sPxzL5zk1n108yNPA0u6S4jCJSID926oAJbz1NJP9+W7+j59/amln8YL5hMGPwYb4KU0iVRE+scY8FKADQiDH+MF8/saKxjozM8/fXgxofkzDJcAo/BTfrTSQ6h5WCJylDHRwfTonMAAaMHyEp79Nv9818p+392gB7TkqzfhhwuwdhqW0/C8GYqWiHSf0LwJw9sYs4XAW8vyP39mMHf5/wE/pJZJKs/o/AAAAABJRU5ErkJggg==" }</t>
+  </si>
+  <si>
+    <t>status=200||mediaId=(OPQA-5253_mediaId)||entityId=(SYS_USER2)||entityType=profile||mediaType=image/png||context=1p-profile</t>
+  </si>
+  <si>
+    <t>{ "mediaId": "(OPQA-5253_mediaId)", "mediaType" : "image/png", "pathPrefix" : "stable-pics1", "base64Media": "data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAMgAAADLCAYAAAArzNwwAAAAGXRFWHRTb2Z0d2FyZQBBZG9iZSBJbWFnZVJlYWR5ccllPAAADylJREFUeNrsnb1y20gWhRvwuso1ienM2VCRNxsqm0xUttGYfAJR2WYys8kkPYHIJxAZTW0karKNTGWTGcrWkaFM2XKSqZlysNtXurBhivjvBvrnnCoUbYmkgO7++tzb3WgIAUEQBEEQBClWgCJoR98NfurJlwH/t89HWi9Tv090s+OrYj5I0R/RrxuULgCxBYKk4Q/l8X0KhL7mPx3JY8Ovd/wKeABI544w5F7/gF97hp1mAg050RrQAJA2gHjLr31LLyViWG4kLCvULABpAsWAYTjakR+4ohU7zEoCE6PWAUgZKAiIkcUu0cRdloAFgOwKnyaOO0VVrVOwbACIn2Ak4dMEPOQm+hSGzSUoEQDxwy0ofDr1MIRS4ioSlAUAcROMd/I4EeYNx9omyk/OfQi/AoABNQy/5vKYuQpKADAgVaBISM4AiB1wnAGM7kIvl3KUwDEwKPm+QPJtRDJPoKwBiBlgEBCX4nHWGzJH5CRTm/OT0JFw6gPgMFITeXySdTSBg7QPxoBdAzPf9oRdx7YtYXlmsWv8Io/XaHfWiMLgyfPXb/76fP/xNziIvlzjCq5hvVbsJsbnJqFFcEw41wAc9mvEuYnxeeMzS+CgXIPCqhdoW87oBYdcgQy51gixEFJBFoZcgcFwEBTvBWbDfVHEkBi1pD40FI4k3wAc/uihQzQtLwkNhIOWilyivXipHkMyQZKenYz/E+3Ee41MSd4DQ8DosWuM0DaglBYyJzn22kEYDkrGh2gP0HZeIp2kL53k2ktAUnBgGBcyEpJngAMCJIYBAjggWyDpapgXcEB1NOGRTncdhC/wH6hrqIGT9KST/Ns5QBiOCeoYaqgfJSR3EhLty1LCFuF4BzgghbrkTTq0KmgJDrqQK9QppFi0+vdQ5wLHoAU4sCoX0qlYHvu6lsqHmuHosXMADkiX+jqjE905yKXAJm6Qfg15FbhyaRvF4p1HsDIXaks0snX7+f7jf4zPQfiml/eoM6iDpH1f5d5boQY4kqXrENS2lLc9HTkI8o78Hm4mj7E8DpND9njk5K/4/1PxuKdtjOKqnY+cGRliYb4jU9TYKz8WgHd1oXD1QNj9bPYutK9ifiRQCAfZ2yeBId1tx5iqel5G6rntJ4ClUJEs9/2mX6JsFOv56ze0Vy5W6H7VQyglK0nZPrSf7z/e07628pjL8qZl33+Kx/2J0Sk91WsV97UrcRCMWj1xjXGbD49hZ6HHWY/gLE+012RUK1BQOdR7fUDFPGjNcHS2QyBvmXMkcI//lzqR9XHYWYglbexngd1ISLQDx1ha+p9dngQtAZfHkpaDc8jre/jVbzKB2MhBeJQFOyAasD1Njrufisen/fosCrFqLWhsOg9yCjjMhINEDUIeNK9yyLmRty5St5Oo7SBIzM2GIyOR9/mRdRtO2Ct1FE0c5NRzOGgSamrLyfKk2SGft4+iSKfyit9aDgL30H8nm2Yn8fkGtkrDvnUdxHf3mNsIR8pJxh7XXaW2W9lB4B4ilo1sz/aL4BuMfB3dKu0ioW4CHdS5Q9fh68hW6TZcyUHgHm64R6o+zzzu8F6VGdGq6iBHnrvHyrHrmXlcl6XCy9KA8Kz5xHNAli5dDPegK0/r8kR1DnLiORwbW0euCnTtaX32yjwLsQogvruHqxNsa4/r9EQJIEya72uuYhcvioc7fR3NGvDEaWMH8T05J93BHf1zkUJAUhsHQJCLGjV1ENwM5b5uPL72Xt5jFMoAcoL2Azmuo1qAcALTR/lBrodZfPdlZQdBeAX5omEdQN6i3LzQDyiC3W09zAmvKLTCRnBfdeByoorq3R0thVUtBwIgrpYBr1YvDQjCq2/Vd/jaEClkmAIcxHNAipZa+J6HhDmFBtvdnZfBPRx20u3h3hDu4b2LYAQrp+1nAXKAcvKmt0VnmFPHcJBq6gF653WQCwjH2cg/ditGESDEQo+yWwtVj1IzTDNU7ROTGACQ6po6el3nqNon6ucBglGNp1p3+dQonXL1ulTlZXAQCMpJ1MM8e4G+CIMWntZ3mJWcQH64qqOrA7SFWOgpsxuSq5AAkJyOYxuQIYrGOxdBned0HCHKoXrihuvyFxAM8frX08JBKgCCHCSnwFxLaPP2g4J2J+lQvi4cux7seVYQeoaeJKKqNCqzZb4l7nGG8Kq6gyDE8sBF+K65U1QlQiwd6jmQiyBSACBoYDlCaFWyjABIgwQO5w8HgRzrgTn/gIMAEL0hlsV5COAAIGhoOcLj9ABIK7Juko3DK8yeAxCEWRl6h2oDIG3Kmsk2dg8sLQEgrSrz0V0GaiKwUqKKNgCkuXo2hC1YWlJLEQBRlKxbkIu8g3uoCbFiFEktFzG2d2Z44R4ApNv4ftfjuwzRJaoHOYgRDdG0hF2eD4VWQ1RNLd3CQdSKQpkLg+AYCPfugOw8xLpDkTQOtSYGwEFOdoXqaKSdo1jYyLi5LrrcZI7heC+wIZyWHCRCuTTWQwPtcOiXwircMajJQZCDqIPkqu2kXf49GrGaoPibK3ksRLj1QwCiToO2nIRAlMd7wKHWPXY5CMIs9ZB80JmTMIAExxDFrUxxHiBwET05yUQDHHRvxwfkHMp1mwfILcqntjY5kNBEopK8hFyDvks8DuVijVXLIdYa5VMbjkN57OeAQj3+J9rVsA4onGucsWvk3Rm4EBiyVwJIsKsS5Mt/UUbV4fgj+jXiMhxw794v+Aw15GXyuYJQ6m2JJJy+81h+34rP4RLhV/W6lOX3KhMQrpBPAhNNteDY6miuSibPMfda6fD2JTfussk3fX6cHonkc7gUuA+9ilayDMdFgGA8vZzW3GPHOb0/hUS6l5ufy3M4yzmHIZ/DEFVWrSyzVvPeoJxKhTKHRXNHXNh7mnI7+s69PDj4HOh91Cueo+pKlakocpABJ4LQUzDm8pglM60Vk2xVPfmKzoMbftVz6PM5IELY3ZkEhYAgD1ELRkYHdMS5QdkyphxjyTFyrOAcElDoHDBUzO5BUUFZQJCHPCbPS1Vg5MAyYFC+59dNKmEnl4h0/X0+B6rnt0jmxVSW86wsIBPh7+2a1Chp+HXh00Wndl488jSh398ejQwKCsun+ZA4FdvHwnNxCDZhWHwItWNZ73vbPwwKCsn1RXAbhuKaJtcQgudGE667ykK2gePtH/6t4EPXDhYKoKgoDjUXnC+dOJqbXu/6YZGDkLV+cqQAVpxXAAp1ucqJcGMpyzfLS0oDwoVh+3LqFY9OxGjaWmChCMP2Wfqd4RWpzL5Yc4uTbprpHgMOreFXMncwFfauIF5m/aIMIDaGJHTO+3VmmqHaoND8AS31t+2O1DivnYQlLjxZlm2TXY51TqxBmW3lwbUt61SXeb8su/XotS3OkRVLQq1B8rCQ0yInWTQGhEd+TI/jk4qBzIHEhg41VuEgNiTr5wirjIIksiA0Xxa9oQogC2HuKEW8vcgMMkJTw9vMShkg3DubmnzhRiBzQ62FzW0mdKAhxr6turVMJobmpTv7sGKPEBvYIyzRBo12ERPbzLxsvlrnCVOmuQjcw3yZ1IkRGKXz1dDyHmGFZSRWuMhamDNNMK8y2ln3GYWmuMg1mp81MmGAp5J71AbEEBfZIDlHmKXTPZo4iAkuskabsyrMijoOs+Kq7tEIEHaRLiFBeIUwq1KHXmelRdPnpM9EdzOluDPQPnXVqUV1w/FGgDCR044uGOuu7AuzugqLa7fRUMFFLzrIB5B/IMwqq0UTMMOuCa0pbK5tr9qsu8YRjhJAeISizYQdDmKv2ryR6rhpKB6oPJuWdkCh/GMf7cxeyXbyvzZCufSDcLoOsb4QC/eADKhDZXc0KgWkpVALT+FFmKU9tNLlIMkTlSKLCxfSL52d3ELl7pmhppMcC00TiEVPhIW8dpBYKB5RDTU14lhTPoL8wwFp7OSU74cWaiwEsrmZhh4CQqKelXcoBy/UWQLyhKeKC+IO7coZqezsFrpufQhbKIixwsJAiOWOVHV2kc7dNLUDwjGhqqQdCxQRYm270KHOk2zDQZKk7FjR90BuaKPg89o3KQ/bKg1O2ptAAjgckoLObtxGhxm2XCiUSNWdaUd4hUQ90XFb95aEbZcIz7TXGXGAgwCQBI5FWycYdlEqPOpQ9SJ/R3vyHpDjtneyCbsqmRqQwEHc053JcHQKSA1IkIO4p43JcHQOSEVIAIh7ikyGwwhAUpDMCt6DEMs/HXe9e2ZoSknwuq3MeZLvBj9N0F6c01FOtDA2YWvZwLQSYxAu5NHb8WsqsCn2xLJbso6pbq/kMcyA49CUiCEwtABp44f3GZBEQtPSZqiVuiUoLuXRz6jbsUmPtAhNLERu/HsZSdwDPAi5rITjjDu+XXCs2Dlik845MLxAexxuZcGwEgpv0Ie01WOfXWOY8ZZzXmFhnAJLCjgvL9kwJNjM2sy6eydfTnPqbtzhnr1uAJLKSy5F9sZ0K07gYzRLY+rrIsc11tyxGV1fz2wp8M/3H++fv37zL/nPF/L4ccdb/k6hmHzPX/K9v6GJdhcWyzr4Wf7zl4xcIwmpjmU9GR8aB5ZWwojdpJfxlojdZI0m23oofJoDhnUjkIHFldFjSEY5b7PCxh0AY8hgDHPeZmwi7iQgW5VzmdNrkRZcQQBFbdn3Rf7olJWu4RQgKTdJRksEQGkFDCrrSc7bNlzWM5uvNXCw4i4Kwi6AojeUIs1EzYdmAhCzKpJylDnmUEol3yei+NkvzuV8geMVO2JH6Re8lSqUHnS/gKt848YnHEb1SoBx7uKoYeBJZU9E/vBjWuQm9LjilW9LWDiXG5V0C6fB8AqQGqFXkmQSLDcuw5KC4m2J3C3dicx9mGfyCpBUoxikwgdRoVEksMQOXD91Ekei/DMlkw7Dq8ENLwHZ6j2TBLRf4aMxhxcETGT6GH8KiAN+7VX4OF3b3MeQ03tAdoRfRxxm9Cp+fMMN6YZf466g4esg2H9gdxjW+JqY3WLp+41pAGR3I0vH5L0GXxWl4Pk99X9RJ35nx0tCoj4fL/ln/YoumBVCXWPYG4BUheWAYelr/nOx+Lrb4KAhnGUBXsMpAIgqWPpbsXzfskuIUqHgCndiApA2gBnwcdBSr1/FjQiGW3aJCEAAEBOg6aWg6TE4ukKmTSqvuU1CNNwHA0Bsh2i49aM8eBIIvggAQBAEQRAEQRbr/wIMAB2nwEL3kwxHAAAAAElFTkSuQmCC" }</t>
+  </si>
+  <si>
+    <t>/media/(OPQA-5253_mediaId)</t>
+  </si>
+  <si>
+    <t>OPQA-5254</t>
+  </si>
+  <si>
+    <t>OPQA-5255</t>
+  </si>
+  <si>
+    <t>OPQA-5256</t>
+  </si>
+  <si>
+    <t>OPQA-5257</t>
+  </si>
+  <si>
+    <t>OPQA-5258</t>
+  </si>
+  <si>
+    <t>OPQA-5259</t>
+  </si>
+  <si>
+    <t>OPQA-5260</t>
+  </si>
+  <si>
+    <t>OPQA-5261</t>
+  </si>
+  <si>
+    <t>OPQA-5262</t>
+  </si>
+  <si>
+    <t>OPQA-5263</t>
+  </si>
+  <si>
+    <t>OPQA-5264</t>
+  </si>
+  <si>
+    <t>OPQA-5265</t>
+  </si>
+  <si>
+    <t>OPQA-5266</t>
+  </si>
+  <si>
+    <t>OPQA-5267</t>
+  </si>
+  <si>
+    <t>OPQA-5268</t>
+  </si>
+  <si>
+    <t>OPQA-5268_1</t>
+  </si>
+  <si>
+    <t>OPQA-5269</t>
+  </si>
+  <si>
+    <t>OPQA-5270</t>
+  </si>
+  <si>
+    <t>OPQA-5271</t>
+  </si>
+  <si>
+    <t>/internal/media/(OPQA-5271_mediaId)</t>
+  </si>
+  <si>
+    <t>status=200||mediaId=(OPQA-5271_mediaId)||entityId=(SYS_USER1)||entityType=profile||mediaType=image/jpeg||context=1p-profile</t>
+  </si>
+  <si>
+    <t>OPQA-5272</t>
+  </si>
+  <si>
+    <t>{"entityId" : "(SYS_USER1)", "entityType" : "profile", "mediaType" : "image/jpeg", "context" : "1p-profile", "mediaStorageLocation" : "(OPQA-5272_mediaStorageLocation)"}</t>
+  </si>
+  <si>
+    <t>status=201||entityId=(SYS_USER1)||entityType=profile||mediaType=image/jpeg||context=1p-profile||mediaStorageLocation=(OPQA-5272_mediaStorageLocation)</t>
+  </si>
+  <si>
+    <t>OPQA-5273</t>
+  </si>
+  <si>
+    <t>OPQA-5274</t>
+  </si>
+  <si>
+    <t>OPQA-5275</t>
+  </si>
+  <si>
+    <t>OPQA-5276</t>
+  </si>
+  <si>
+    <t>OPQA-5275||OPQA-5276</t>
+  </si>
+  <si>
+    <t>status=200||mediaId=(OPQA-5275_mediaId)||entityId=(SYS_USER1)||entityType=profile||mediaType=image/jpeg||context=1p-profile||mediaStorageLocation=(OPQA-5275_mediaStorageLocation)||mediaUrl=(OPQA-5275_mediaUrl)||entityId=(SYS_USER3)||mediaId=(OPQA-5276_mediaId)||mediaStorageLocation=(OPQA-5276_mediaStorageLocation)||mediaUrl=(OPQA-5276_mediaUrl)</t>
+  </si>
+  <si>
+    <t>OPQA-5277</t>
+  </si>
+  <si>
+    <t>OPQA-5278</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,6 +429,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -416,10 +480,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -448,12 +513,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -500,7 +575,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -532,9 +607,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -566,6 +642,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -741,14 +818,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H17" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L26"/>
+    <sheetView tabSelected="1" topLeftCell="H25" workbookViewId="0">
+      <selection activeCell="L29" sqref="L2:L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="53.140625" style="5" customWidth="1" collapsed="1"/>
@@ -764,7 +841,7 @@
     <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -802,18 +879,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="255">
+    <row r="2" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>15</v>
@@ -823,28 +900,28 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="240">
-      <c r="A3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>26</v>
-      </c>
       <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>15</v>
@@ -854,28 +931,28 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="240">
-      <c r="A4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>32</v>
-      </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
@@ -885,28 +962,28 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>19</v>
-      </c>
       <c r="J4" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:12" ht="240">
+    <row r="5" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>11</v>
@@ -916,26 +993,26 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="7" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:12" ht="240">
+    <row r="6" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>11</v>
@@ -945,26 +1022,26 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="7" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:12" ht="240">
+    <row r="7" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>11</v>
@@ -974,28 +1051,28 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="6" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:12" ht="240">
+    <row r="8" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>11</v>
@@ -1005,28 +1082,28 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="6" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:12" ht="240">
+    <row r="9" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>11</v>
@@ -1036,28 +1113,28 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="6" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:12" ht="31.5">
+    <row r="10" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>0</v>
@@ -1065,25 +1142,25 @@
       <c r="G10" s="1"/>
       <c r="H10" s="4"/>
       <c r="I10" s="8" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>14</v>
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="47.25">
+    <row r="11" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>0</v>
@@ -1092,25 +1169,25 @@
       <c r="G11" s="1"/>
       <c r="H11" s="4"/>
       <c r="I11" s="8" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="31.5">
+    <row r="12" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>51</v>
+        <v>102</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>0</v>
@@ -1118,25 +1195,25 @@
       <c r="G12" s="1"/>
       <c r="H12" s="4"/>
       <c r="I12" s="8" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>14</v>
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:12" s="10" customFormat="1" ht="47.25">
+    <row r="13" spans="1:12" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>0</v>
@@ -1145,109 +1222,109 @@
       <c r="G13"/>
       <c r="H13"/>
       <c r="I13" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>17</v>
+        <v>99</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="K13"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:12" ht="47.25">
+    <row r="14" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="8" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="47.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>60</v>
+        <v>105</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="8" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="47.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="H16"/>
       <c r="I16" s="8" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="31.5">
+    <row r="17" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>18</v>
@@ -1255,24 +1332,24 @@
       <c r="F17" s="10"/>
       <c r="H17" s="11"/>
       <c r="I17" s="8" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="J17" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="31.5">
+    <row r="18" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>18</v>
@@ -1280,24 +1357,24 @@
       <c r="G18" s="5"/>
       <c r="H18"/>
       <c r="I18" s="8" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="47.25">
+    <row r="19" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>18</v>
@@ -1306,25 +1383,25 @@
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="8" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="47.25">
+    <row r="20" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>18</v>
@@ -1332,201 +1409,305 @@
       <c r="G20" s="5"/>
       <c r="H20"/>
       <c r="I20" s="8" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="45">
+    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="6" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="E22" t="s">
         <v>11</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="47.25">
+        <v>114</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="6" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="47.25">
+    <row r="24" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>103</v>
+        <v>65</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="6" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="K24" s="8"/>
     </row>
-    <row r="25" spans="1:11" ht="45">
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>105</v>
+        <v>66</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D25" t="s">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="6" t="s">
-        <v>107</v>
+        <v>68</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="1:11" ht="31.5">
+        <v>114</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="B26" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5"/>
+      <c r="G26" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C26" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" t="s">
-        <v>106</v>
-      </c>
-      <c r="E26" s="10" t="s">
+      <c r="H26" s="6"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="G27" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="12"/>
+      <c r="H28" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G26" s="5"/>
-      <c r="H26"/>
-      <c r="I26" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="J26" s="7" t="s">
+      <c r="G29" s="5"/>
+      <c r="H29"/>
+      <c r="I29" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="J29" s="7" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30"/>
+      <c r="H30"/>
+      <c r="J30"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G27" r:id="rId1" display="http://ec2-52-24-117-253.us-west-2.compute.amazonaws.com:7001/media/1p-profile/profile/bulk?id=c8c90799-784f-48c9-90b8-e1f90574004c&amp;id=8fda8edf-1fda-4e69-b64e-110de0218c24"/>
+    <hyperlink ref="G26" r:id="rId2" display="http://ec2-52-24-117-253.us-west-2.compute.amazonaws.com:7001/media/1p-profile/profile/bulk?id=c8c90799-784f-48c9-90b8-e1f90574004c&amp;id=8fda8edf-1fda-4e69-b64e-110de0218c24"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="51.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1540,7 +1721,7 @@
     <col min="10" max="10" width="64.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Fixed failed tests in 1PMEDIA service.
</commit_message>
<xml_diff>
--- a/src/test/test-data/MediaTestData.xlsx
+++ b/src/test/test-data/MediaTestData.xlsx
@@ -1057,7 +1057,7 @@
         <v>80</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="K7" s="8"/>
     </row>
@@ -1531,8 +1531,8 @@
       <c r="I24" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="J24" s="7" t="s">
-        <v>50</v>
+      <c r="J24" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="K24" s="8"/>
     </row>

</xml_diff>